<commit_message>
Made changes to the code related to exception and emails.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\55651C\Documents\UiPath\P002_090_PayCycleAfternoon_Dispatcher\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AC251E3-8B7C-495C-9672-E91951B19B9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EB467CC-9978-4353-A609-F2DECE5423CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="330">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="405">
   <si>
     <t>Name</t>
   </si>
@@ -99,11 +99,11 @@
   </si>
   <si>
     <t>Orchestrator queue Name. The value must match with the queue name defined on Orchestrator.</t>
-    <phoneticPr fontId="11"/>
+    <phoneticPr fontId="16"/>
   </si>
   <si>
     <t>Logging field which allows grouping of log data of two or more subprocesses under the same business process name</t>
-    <phoneticPr fontId="11"/>
+    <phoneticPr fontId="16"/>
   </si>
   <si>
     <t>Must be 0 if working with Orchestrator queues. If &gt; 0, the robot will retry the same transaction which failed with a system exception. Must be an integer value.</t>
@@ -550,12 +550,6 @@
     <t>Workflow to check Trigger Email is started.</t>
   </si>
   <si>
-    <t>TriggerEmailNotFound</t>
-  </si>
-  <si>
-    <t>There was an error as the Trigger email was not found.</t>
-  </si>
-  <si>
     <t>TriggerEmailWorkflowCompleted</t>
   </si>
   <si>
@@ -679,9 +673,6 @@
     <t>CheckValidateQueryWorkflowBE</t>
   </si>
   <si>
-    <t>NoDataFoundBE</t>
-  </si>
-  <si>
     <t>No data or more than 1 rows found for OBATCNN query for a day</t>
   </si>
   <si>
@@ -761,9 +752,6 @@
   </si>
   <si>
     <t>NoSuccessRecordLog</t>
-  </si>
-  <si>
-    <t>NoSuccessRecordBE</t>
   </si>
   <si>
     <t>CheckPendingRecord</t>
@@ -1029,6 +1017,243 @@
   </si>
   <si>
     <t>11:30PM</t>
+  </si>
+  <si>
+    <t>BE_1: There was an error as the Trigger email was not found.</t>
+  </si>
+  <si>
+    <t>BE_1Subject</t>
+  </si>
+  <si>
+    <t>MailsWithCustomMessages</t>
+  </si>
+  <si>
+    <t>Pay Cycle Afternoon confirmation email not received</t>
+  </si>
+  <si>
+    <t>OKBATCNN -Job ran to No Success</t>
+  </si>
+  <si>
+    <t>PeopleSoft application unavailable</t>
+  </si>
+  <si>
+    <t>PeopleSoft login failed</t>
+  </si>
+  <si>
+    <t>BE_1Body</t>
+  </si>
+  <si>
+    <t>BE_1RecipientEmailAddress</t>
+  </si>
+  <si>
+    <t>BE_1CCEmailAddress</t>
+  </si>
+  <si>
+    <t>BE_2Subject</t>
+  </si>
+  <si>
+    <t>BE_2Body</t>
+  </si>
+  <si>
+    <t>BE_2RecipientEmailAddress</t>
+  </si>
+  <si>
+    <t>BE_2CCEmailAddress</t>
+  </si>
+  <si>
+    <t>TableNotFound</t>
+  </si>
+  <si>
+    <t>TableNotFoundSE</t>
+  </si>
+  <si>
+    <t>No table found on the page for BATCHPROD</t>
+  </si>
+  <si>
+    <t>No Pending or No Success Record found.</t>
+  </si>
+  <si>
+    <t>PendingRetryBlockErrorMessage</t>
+  </si>
+  <si>
+    <t>SE_1Subject</t>
+  </si>
+  <si>
+    <t>SE_1Body</t>
+  </si>
+  <si>
+    <t>SE_1RecipientEmailAddress</t>
+  </si>
+  <si>
+    <t>SE_1CCEmailAddress</t>
+  </si>
+  <si>
+    <t>SE_2Subject</t>
+  </si>
+  <si>
+    <t>SE_2Body</t>
+  </si>
+  <si>
+    <t>SE_2RecipientEmailAddress</t>
+  </si>
+  <si>
+    <t>SE_2CCEmailAddress</t>
+  </si>
+  <si>
+    <t>BE_1,BE_2,SE_1,SE_2,BE_3</t>
+  </si>
+  <si>
+    <t>BE_3Subject</t>
+  </si>
+  <si>
+    <t>BE_3Body</t>
+  </si>
+  <si>
+    <t>BE_3RecipientEmailAddress</t>
+  </si>
+  <si>
+    <t>BE_3CCEmailAddress</t>
+  </si>
+  <si>
+    <t>Unable to view OKBATCNN job</t>
+  </si>
+  <si>
+    <t>GetMailDetailsWorkflowStarted</t>
+  </si>
+  <si>
+    <t>GetMailDetailsWorkflowCompleted</t>
+  </si>
+  <si>
+    <t>GetMailDetailsWorkflowSE</t>
+  </si>
+  <si>
+    <t>Workflow to Get Mail Details started.</t>
+  </si>
+  <si>
+    <t>Workflow to Get Mail Details completed successfully.</t>
+  </si>
+  <si>
+    <t>Workflow to Get Mail Details has a System Exception.</t>
+  </si>
+  <si>
+    <t>RowIndexOKBATCNN</t>
+  </si>
+  <si>
+    <t>BE_1TimeStampAddMinutes</t>
+  </si>
+  <si>
+    <t>Shared_O365TenantID</t>
+  </si>
+  <si>
+    <t>GraphAPIO365TenantID</t>
+  </si>
+  <si>
+    <t>Shared_O365ApplicationID</t>
+  </si>
+  <si>
+    <t>GraphAPIO365ApplicationID</t>
+  </si>
+  <si>
+    <t>Shared_O365ApplicationSecret</t>
+  </si>
+  <si>
+    <t>GraphAPIApplicationSecret</t>
+  </si>
+  <si>
+    <t>PeopleSoftLoginErrorKeyword1</t>
+  </si>
+  <si>
+    <t>PeopleSoftLoginErrorKeyword2</t>
+  </si>
+  <si>
+    <t>PeopleSoftLoginErrorKeyword3</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>user</t>
+  </si>
+  <si>
+    <t>invalid</t>
+  </si>
+  <si>
+    <t>TriggerEmailNotFoundBE_1</t>
+  </si>
+  <si>
+    <t>TriggerEmailNotFound</t>
+  </si>
+  <si>
+    <t>There was an error as the Trigger email was not found.</t>
+  </si>
+  <si>
+    <t>SE_2: Credentials Error.</t>
+  </si>
+  <si>
+    <t>SE_1: Peoplesoft Unavailable.</t>
+  </si>
+  <si>
+    <t>AllValuesPresent</t>
+  </si>
+  <si>
+    <t>All mandatory values are present.</t>
+  </si>
+  <si>
+    <t>PeoplesoftLoginCredentialsSE_2</t>
+  </si>
+  <si>
+    <t>PeoplesoftLoginPageUnavailableSE_1</t>
+  </si>
+  <si>
+    <t>PeopleSoft_HomepageURL</t>
+  </si>
+  <si>
+    <t>https://soklfpub-tst.opc.oracleoutsourcing.com/psc/SOKLFTSTNSS/EMPLOYEE/ERP/c/NUI_FRAMEWORK.PT_LANDINGPAGE.GBL</t>
+  </si>
+  <si>
+    <t>URL for homepage after login.</t>
+  </si>
+  <si>
+    <t>PeopleSoft_ProcessMonitorURL</t>
+  </si>
+  <si>
+    <t>https://soklfpub-tst.opc.oracleoutsourcing.com/psp/SOKLFTSTNSS/EMPLOYEE/ERP/c/PROCESSMONITOR.PROCESSMONITOR.GBL</t>
+  </si>
+  <si>
+    <t>URL for Process Monitor Page.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hi Statewide Accounting Team,&lt;br&gt;&lt;br&gt;OKBATCNN status as 'No Success' is halting the afternoon pay cycle. Please complete it manually today; the bot will resume next business day.&lt;br&gt; &lt;br&gt; Thanks,&lt;br&gt;Automation Team                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hi Statewide Accounting Team,&lt;br&gt;&lt;br&gt;PeopleSoft app is unavailable. Please complete today's pay cycle manually; bot will resume next business day.&lt;br&gt;&lt;br&gt;  Thanks,&lt;br&gt;Automation Team                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hi Statewide Accounting Team,&lt;br&gt;&lt;br&gt;PeopleSoft login failed for user ID &lt;Bot_user_ID&gt;. Please complete today's pay cycle manually; bot will resume next business day.&lt;br&gt;Automation support team: Please confirm that the login credentials are valid / updated prior to the next Bot run&lt;br&gt; &lt;br&gt; Thanks,&lt;br&gt;Automation Team                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hi Statewide Accounting Team,&lt;br&gt;&lt;br&gt;OKBATCNN job is unavailable on process monitor screen due to which bot failed to check the status of the job.&lt;br&gt; &lt;br&gt; Thanks,&lt;br&gt;Automation Team                        </t>
+  </si>
+  <si>
+    <t>NoSuccessRecordBE_2</t>
+  </si>
+  <si>
+    <t>BE_2: A record was found with No Success and hence the data will not be added to dispacher.</t>
+  </si>
+  <si>
+    <t>Hi Statewide Accounting Team,&lt;br&gt;&lt;br&gt;Bot hasn't received the correct confirmation email&lt;br&gt;Please send the email within &lt;15mintime_stamp&gt;&lt;br&gt;Subject Line : P0002PayCycleAfternoonTrigger&lt;br&gt;Bot Email Address :  &lt;bot_email_address&gt;&lt;br&gt; &lt;br&gt; Thanks,&lt;br&gt;Automation Team</t>
+  </si>
+  <si>
+    <t>SenderEmailAddress</t>
+  </si>
+  <si>
+    <t>NoDataFoundBE_3</t>
+  </si>
+  <si>
+    <t>BE_3: No data or more than 1 rows found for OBATCNN query for a day</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Index for OKBATCNN job </t>
   </si>
 </sst>
 </file>
@@ -1038,11 +1263,46 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="19">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1156,12 +1416,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1200,69 +1454,75 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="23">
+  <cellStyleXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="4" fontId="16" fillId="2" borderId="1" applyNumberFormat="0" applyProtection="0">
+    <xf numFmtId="4" fontId="21" fillId="2" borderId="1" applyNumberFormat="0" applyProtection="0">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="20"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="20"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="20" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="20" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="20" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="20" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="20" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="20" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="20" applyFont="1"/>
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="20" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="20" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="20" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="20" applyFont="1"/>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="20" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="22"/>
   </cellXfs>
-  <cellStyles count="23">
+  <cellStyles count="24">
     <cellStyle name="Comma 2" xfId="2" xr:uid="{DA952E48-534A-4104-8A72-2BE892964A18}"/>
     <cellStyle name="Comma 3" xfId="11" xr:uid="{856AAB38-97AE-41B8-BFBC-5E8E757493AE}"/>
     <cellStyle name="Comma 4" xfId="15" xr:uid="{15E63A3B-FADD-4F72-8A15-82B5F65A0D08}"/>
     <cellStyle name="Comma 5" xfId="18" xr:uid="{927AECA0-D30A-42CF-8940-CE1B2E2FC2DF}"/>
-    <cellStyle name="Hyperlink" xfId="22" builtinId="8"/>
     <cellStyle name="Hyperlink 2" xfId="5" xr:uid="{3D82F709-362D-4D82-AFB0-BF8FA139F966}"/>
     <cellStyle name="Hyperlink 3" xfId="21" xr:uid="{021947CE-673E-4762-9284-139DFB8EC828}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 10" xfId="22" xr:uid="{67BF97D7-1302-4E51-A423-B074EC7495CE}"/>
     <cellStyle name="Normal 2" xfId="3" xr:uid="{E450A2C8-8DC8-43AF-8A35-C8D4EBD3CDF0}"/>
     <cellStyle name="Normal 2 2" xfId="4" xr:uid="{7EDF15AA-B908-4ECC-B667-C8372380DAA9}"/>
+    <cellStyle name="Normal 2 2 2" xfId="23" xr:uid="{4FF5A161-890E-4F75-9DA9-991C0B3DE49E}"/>
     <cellStyle name="Normal 3" xfId="7" xr:uid="{09200420-0922-4EBF-A7BE-DA4219BD3BB6}"/>
     <cellStyle name="Normal 3 2" xfId="9" xr:uid="{42A2E569-406F-4F88-9D89-0967D461C4A6}"/>
     <cellStyle name="Normal 3 3" xfId="12" xr:uid="{DF97DA59-1504-4713-9E90-2506C826A8F0}"/>
@@ -1587,10 +1847,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z73"/>
+  <dimension ref="A1:Z104"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="A75" sqref="A75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="14.5"/>
@@ -1637,10 +1897,10 @@
     </row>
     <row r="2" spans="1:26">
       <c r="A2" s="2" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>20</v>
@@ -1651,7 +1911,7 @@
         <v>28</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>29</v>
@@ -1662,7 +1922,7 @@
         <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>21</v>
@@ -1672,7 +1932,7 @@
       <c r="A5" t="s">
         <v>43</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" t="s">
         <v>41</v>
       </c>
       <c r="C5" s="4" t="s">
@@ -1681,683 +1941,934 @@
     </row>
     <row r="6" spans="1:26">
       <c r="A6" t="s">
-        <v>44</v>
+        <v>388</v>
       </c>
       <c r="B6" t="s">
-        <v>178</v>
-      </c>
-      <c r="C6" t="s">
-        <v>45</v>
+        <v>389</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>390</v>
       </c>
     </row>
     <row r="7" spans="1:26">
       <c r="A7" t="s">
-        <v>46</v>
+        <v>391</v>
       </c>
       <c r="B7" t="s">
-        <v>154</v>
-      </c>
-      <c r="C7" t="s">
-        <v>47</v>
+        <v>392</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>393</v>
       </c>
     </row>
     <row r="8" spans="1:26">
       <c r="A8" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B8" t="s">
-        <v>154</v>
+        <v>176</v>
       </c>
       <c r="C8" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:26">
       <c r="A9" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B9" t="s">
         <v>154</v>
       </c>
       <c r="C9" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:26">
       <c r="A10" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B10" t="s">
         <v>154</v>
       </c>
       <c r="C10" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:26">
       <c r="A11" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B11" t="s">
         <v>154</v>
       </c>
       <c r="C11" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:26">
       <c r="A12" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B12" t="s">
         <v>154</v>
       </c>
       <c r="C12" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26" ht="43.5">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26">
       <c r="A13" t="s">
-        <v>58</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>292</v>
+        <v>54</v>
+      </c>
+      <c r="B13" t="s">
+        <v>154</v>
       </c>
       <c r="C13" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:26">
       <c r="A14" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B14" t="s">
-        <v>61</v>
+        <v>154</v>
       </c>
       <c r="C14" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="43.5">
       <c r="A15" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>155</v>
+        <v>288</v>
       </c>
       <c r="C15" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:26">
       <c r="A16" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B16" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="C16" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="43.5">
       <c r="A17" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C17" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B18" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C18" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="43.5">
       <c r="A19" t="s">
-        <v>73</v>
-      </c>
-      <c r="B19" t="s">
-        <v>74</v>
+        <v>68</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>156</v>
       </c>
       <c r="C19" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="B20" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="C20" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B21" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="C21" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="B22" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C22" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>85</v>
+        <v>79</v>
+      </c>
+      <c r="B23" t="s">
+        <v>80</v>
       </c>
       <c r="C23" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B24" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="C24" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>90</v>
-      </c>
-      <c r="B25" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C25" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="B26" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="C26" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="B27" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C27" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>5</v>
+        <v>93</v>
+      </c>
+      <c r="B28" t="s">
+        <v>94</v>
       </c>
       <c r="C28" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>100</v>
-      </c>
-      <c r="B29" s="3"/>
+        <v>96</v>
+      </c>
+      <c r="B29" t="s">
+        <v>97</v>
+      </c>
       <c r="C29" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>102</v>
-      </c>
-      <c r="B30" t="s">
-        <v>103</v>
+        <v>5</v>
       </c>
       <c r="C30" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
-        <v>105</v>
-      </c>
-      <c r="B31" t="s">
-        <v>106</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="B31" s="3"/>
       <c r="C31" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B32" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C32" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B33" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="C33" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="B34" t="s">
-        <v>94</v>
+        <v>109</v>
       </c>
       <c r="C34" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" t="s">
+        <v>111</v>
+      </c>
+      <c r="B35" t="s">
+        <v>112</v>
+      </c>
+      <c r="C35" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" t="s">
+        <v>114</v>
+      </c>
+      <c r="B36" t="s">
+        <v>94</v>
+      </c>
+      <c r="C36" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" t="s">
         <v>116</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B37" t="s">
         <v>97</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C37" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
-      <c r="A36" s="2" t="s">
+    <row r="38" spans="1:3">
+      <c r="A38" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B38" t="s">
         <v>118</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C38" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
-      <c r="A37" s="9" t="s">
+    <row r="39" spans="1:3">
+      <c r="A39" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="B37" s="5" t="s">
+      <c r="B39" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="C37" s="5" t="s">
+      <c r="C39" s="5" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
-      <c r="A38" s="9" t="s">
+    <row r="40" spans="1:3">
+      <c r="A40" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="B38" s="9" t="s">
+      <c r="B40" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="C38" s="5" t="s">
+      <c r="C40" s="5" t="s">
         <v>124</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3">
-      <c r="A39" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="B39" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="C39" s="5" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3">
-      <c r="A40" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="B40" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="C40" s="5" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" s="5" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" s="5" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>134</v>
+        <v>94</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" s="5" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>97</v>
+        <v>131</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="B44" t="s">
-        <v>139</v>
+        <v>133</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>134</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" s="5" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>142</v>
+        <v>97</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="B46">
-        <v>5000</v>
+        <v>138</v>
+      </c>
+      <c r="B46" t="s">
+        <v>139</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="B47">
-        <v>5000</v>
+        <v>141</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>142</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" s="5" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B48">
-        <v>2000</v>
+        <v>5000</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="B49" t="b">
-        <v>1</v>
+        <v>146</v>
+      </c>
+      <c r="B49">
+        <v>5000</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" s="5" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B50">
-        <v>20</v>
+        <v>2000</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
     </row>
     <row r="51" spans="1:3">
       <c r="A51" s="5" t="s">
-        <v>159</v>
-      </c>
-      <c r="B51" t="s">
-        <v>158</v>
+        <v>150</v>
+      </c>
+      <c r="B51" t="b">
+        <v>1</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="B52">
+        <v>20</v>
+      </c>
+      <c r="C52" s="5" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="B53" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54" s="5" t="s">
         <v>160</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B54" t="s">
         <v>161</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3">
-      <c r="A53" s="6" t="s">
-        <v>163</v>
-      </c>
-      <c r="B53" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3">
-      <c r="A54" s="11" t="s">
-        <v>165</v>
-      </c>
-      <c r="B54">
-        <v>5</v>
       </c>
     </row>
     <row r="55" spans="1:3">
       <c r="A55" s="6" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B55" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="56" spans="1:3">
-      <c r="A56" s="8" t="s">
-        <v>187</v>
+      <c r="A56" s="11" t="s">
+        <v>165</v>
       </c>
       <c r="B56">
         <v>5</v>
       </c>
     </row>
     <row r="57" spans="1:3">
-      <c r="A57" s="7" t="s">
-        <v>200</v>
-      </c>
-      <c r="B57">
-        <v>1</v>
+      <c r="A57" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="B57" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="58" spans="1:3">
-      <c r="A58" s="7" t="s">
-        <v>201</v>
-      </c>
-      <c r="B58" t="s">
-        <v>202</v>
+      <c r="A58" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="B58">
+        <v>5</v>
       </c>
     </row>
     <row r="59" spans="1:3">
       <c r="A59" s="7" t="s">
-        <v>203</v>
-      </c>
-      <c r="B59" t="s">
-        <v>204</v>
+        <v>198</v>
+      </c>
+      <c r="B59">
+        <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:3">
       <c r="A60" s="7" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="B60" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
     </row>
     <row r="61" spans="1:3">
       <c r="A61" s="7" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="B61" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
     </row>
     <row r="62" spans="1:3">
       <c r="A62" s="7" t="s">
-        <v>226</v>
+        <v>203</v>
       </c>
       <c r="B62" t="s">
-        <v>225</v>
+        <v>204</v>
       </c>
     </row>
     <row r="63" spans="1:3">
-      <c r="A63" s="8" t="s">
-        <v>227</v>
+      <c r="A63" s="7" t="s">
+        <v>205</v>
       </c>
       <c r="B63" t="s">
-        <v>323</v>
+        <v>206</v>
       </c>
     </row>
     <row r="64" spans="1:3">
-      <c r="A64" s="12" t="s">
-        <v>228</v>
-      </c>
-      <c r="B64" s="13" t="s">
-        <v>326</v>
+      <c r="A64" s="7" t="s">
+        <v>223</v>
+      </c>
+      <c r="B64" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="65" spans="1:2">
       <c r="A65" s="8" t="s">
-        <v>247</v>
+        <v>224</v>
       </c>
       <c r="B65" t="s">
-        <v>246</v>
+        <v>319</v>
       </c>
     </row>
     <row r="66" spans="1:2">
-      <c r="A66" s="8" t="s">
-        <v>259</v>
-      </c>
-      <c r="B66" t="s">
-        <v>257</v>
+      <c r="A66" s="12" t="s">
+        <v>225</v>
+      </c>
+      <c r="B66" s="13" t="s">
+        <v>322</v>
       </c>
     </row>
     <row r="67" spans="1:2">
       <c r="A67" s="8" t="s">
-        <v>258</v>
+        <v>243</v>
       </c>
       <c r="B67" t="s">
-        <v>260</v>
+        <v>242</v>
       </c>
     </row>
     <row r="68" spans="1:2">
-      <c r="A68" s="12" t="s">
-        <v>304</v>
-      </c>
-      <c r="B68">
+      <c r="A68" s="8" t="s">
+        <v>255</v>
+      </c>
+      <c r="B68" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2">
+      <c r="A69" s="8" t="s">
+        <v>254</v>
+      </c>
+      <c r="B69" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
+      <c r="A70" s="12" t="s">
+        <v>300</v>
+      </c>
+      <c r="B70">
         <v>3</v>
       </c>
     </row>
-    <row r="69" spans="1:2">
-      <c r="A69" s="10" t="s">
-        <v>314</v>
-      </c>
-      <c r="B69" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2">
-      <c r="A70" s="11" t="s">
-        <v>315</v>
-      </c>
-      <c r="B70" t="s">
-        <v>316</v>
-      </c>
-    </row>
     <row r="71" spans="1:2">
-      <c r="A71" s="11" t="s">
-        <v>317</v>
+      <c r="A71" s="10" t="s">
+        <v>310</v>
       </c>
       <c r="B71" t="s">
-        <v>329</v>
+        <v>318</v>
       </c>
     </row>
     <row r="72" spans="1:2">
-      <c r="A72" s="12" t="s">
-        <v>324</v>
-      </c>
-      <c r="B72" t="b">
+      <c r="A72" s="11" t="s">
+        <v>311</v>
+      </c>
+      <c r="B72" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2">
+      <c r="A73" s="11" t="s">
+        <v>313</v>
+      </c>
+      <c r="B73" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2">
+      <c r="A74" s="12" t="s">
+        <v>320</v>
+      </c>
+      <c r="B74" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:2">
-      <c r="A73" s="14" t="s">
-        <v>325</v>
-      </c>
-      <c r="B73" t="str">
+    <row r="75" spans="1:2">
+      <c r="A75" s="14" t="s">
+        <v>321</v>
+      </c>
+      <c r="B75" t="str">
         <f ca="1">TEXT(TODAY(), "mm/dd/yyyy")</f>
         <v>12/15/2023</v>
       </c>
     </row>
+    <row r="76" spans="1:2">
+      <c r="A76" s="16" t="s">
+        <v>328</v>
+      </c>
+      <c r="B76" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2">
+      <c r="A77" s="15" t="s">
+        <v>327</v>
+      </c>
+      <c r="B77" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" ht="58">
+      <c r="A78" s="15" t="s">
+        <v>333</v>
+      </c>
+      <c r="B78" s="3" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2">
+      <c r="A79" s="16" t="s">
+        <v>366</v>
+      </c>
+      <c r="B79" s="3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2">
+      <c r="A80" s="19" t="s">
+        <v>401</v>
+      </c>
+      <c r="B80" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2">
+      <c r="A81" s="16" t="s">
+        <v>334</v>
+      </c>
+      <c r="B81" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2">
+      <c r="A82" s="16" t="s">
+        <v>335</v>
+      </c>
+      <c r="B82" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2">
+      <c r="A83" s="19" t="s">
+        <v>336</v>
+      </c>
+      <c r="B83" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" ht="43.5">
+      <c r="A84" s="15" t="s">
+        <v>337</v>
+      </c>
+      <c r="B84" s="3" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2">
+      <c r="A85" s="16" t="s">
+        <v>338</v>
+      </c>
+      <c r="B85" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2">
+      <c r="A86" s="15" t="s">
+        <v>339</v>
+      </c>
+      <c r="B86" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2">
+      <c r="A87" s="15" t="s">
+        <v>345</v>
+      </c>
+      <c r="B87" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" ht="29">
+      <c r="A88" s="15" t="s">
+        <v>346</v>
+      </c>
+      <c r="B88" s="3" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2">
+      <c r="A89" s="15" t="s">
+        <v>347</v>
+      </c>
+      <c r="B89" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2">
+      <c r="A90" s="15" t="s">
+        <v>348</v>
+      </c>
+      <c r="B90" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2">
+      <c r="A91" s="15" t="s">
+        <v>349</v>
+      </c>
+      <c r="B91" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" ht="58">
+      <c r="A92" s="15" t="s">
+        <v>350</v>
+      </c>
+      <c r="B92" s="3" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2">
+      <c r="A93" s="15" t="s">
+        <v>351</v>
+      </c>
+      <c r="B93" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2">
+      <c r="A94" s="15" t="s">
+        <v>352</v>
+      </c>
+      <c r="B94" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2">
+      <c r="A95" s="15" t="s">
+        <v>354</v>
+      </c>
+      <c r="B95" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" ht="29">
+      <c r="A96" s="15" t="s">
+        <v>355</v>
+      </c>
+      <c r="B96" s="3" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2">
+      <c r="A97" s="15" t="s">
+        <v>356</v>
+      </c>
+      <c r="B97" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2">
+      <c r="A98" s="15" t="s">
+        <v>357</v>
+      </c>
+      <c r="B98" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2">
+      <c r="A99" s="18" t="s">
+        <v>373</v>
+      </c>
+      <c r="B99" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2">
+      <c r="A100" s="17" t="s">
+        <v>374</v>
+      </c>
+      <c r="B100" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2">
+      <c r="A101" s="17" t="s">
+        <v>375</v>
+      </c>
+      <c r="B101" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2">
+      <c r="A102" t="s">
+        <v>372</v>
+      </c>
+      <c r="B102" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2">
+      <c r="A103" t="s">
+        <v>368</v>
+      </c>
+      <c r="B103" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2">
+      <c r="A104" t="s">
+        <v>370</v>
+      </c>
+      <c r="B104" t="s">
+        <v>369</v>
+      </c>
+    </row>
   </sheetData>
-  <phoneticPr fontId="11"/>
-  <hyperlinks>
-    <hyperlink ref="B5" r:id="rId1" xr:uid="{BC7B3224-FBD3-48CE-BB69-8DE38A38920B}"/>
-  </hyperlinks>
+  <phoneticPr fontId="16"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2366,7 +2877,7 @@
   <dimension ref="A1:Z988"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -3519,7 +4030,7 @@
     <row r="987" ht="14.25" customHeight="1"/>
     <row r="988" ht="14.25" customHeight="1"/>
   </sheetData>
-  <phoneticPr fontId="11"/>
+  <phoneticPr fontId="16"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3529,7 +4040,7 @@
   <dimension ref="A1:Z2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="14.5"/>
@@ -3545,7 +4056,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>27</v>
@@ -3578,24 +4089,24 @@
     </row>
     <row r="2" spans="1:26">
       <c r="A2" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="B2" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="11"/>
+  <phoneticPr fontId="16"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1D9DC59-3960-42CB-B3EC-EFF452A90D4F}">
-  <dimension ref="A1:Z64"/>
+  <dimension ref="A1:Z75"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="B52" sqref="B52"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -3649,50 +4160,50 @@
     </row>
     <row r="3" spans="1:26">
       <c r="A3" t="s">
-        <v>170</v>
+        <v>380</v>
       </c>
       <c r="B3" t="s">
-        <v>171</v>
+        <v>381</v>
       </c>
     </row>
     <row r="4" spans="1:26">
       <c r="A4" t="s">
-        <v>172</v>
+        <v>379</v>
       </c>
       <c r="B4" t="s">
-        <v>173</v>
+        <v>326</v>
       </c>
     </row>
     <row r="5" spans="1:26">
       <c r="A5" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="B5" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="6" spans="1:26">
       <c r="A6" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="B6" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
     </row>
     <row r="7" spans="1:26">
       <c r="A7" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="B7" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="8" spans="1:26">
       <c r="A8" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="B8" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
     </row>
     <row r="9" spans="1:26">
@@ -3700,447 +4211,535 @@
         <v>181</v>
       </c>
       <c r="B9" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="10" spans="1:26">
       <c r="A10" t="s">
-        <v>182</v>
+        <v>386</v>
       </c>
       <c r="B10" t="s">
-        <v>186</v>
+        <v>382</v>
       </c>
     </row>
     <row r="11" spans="1:26">
       <c r="A11" t="s">
-        <v>188</v>
+        <v>387</v>
       </c>
       <c r="B11" t="s">
-        <v>191</v>
+        <v>383</v>
       </c>
     </row>
     <row r="12" spans="1:26">
       <c r="A12" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
       <c r="B12" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
     </row>
     <row r="13" spans="1:26">
       <c r="A13" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="B13" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
     </row>
     <row r="14" spans="1:26">
       <c r="A14" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="B14" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
     </row>
     <row r="15" spans="1:26">
       <c r="A15" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="B15" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
     </row>
     <row r="16" spans="1:26">
       <c r="A16" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="B16" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>209</v>
+        <v>192</v>
       </c>
       <c r="B17" t="s">
-        <v>216</v>
+        <v>195</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>215</v>
+        <v>193</v>
       </c>
       <c r="B18" t="s">
-        <v>214</v>
+        <v>196</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>213</v>
+        <v>194</v>
       </c>
       <c r="B19" t="s">
-        <v>214</v>
+        <v>197</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="B20" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>211</v>
+        <v>340</v>
       </c>
       <c r="B21" t="s">
-        <v>218</v>
+        <v>342</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>212</v>
+        <v>341</v>
       </c>
       <c r="B22" t="s">
-        <v>219</v>
+        <v>342</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="B23" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>234</v>
+        <v>402</v>
       </c>
       <c r="B24" t="s">
-        <v>232</v>
+        <v>403</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>233</v>
+        <v>365</v>
       </c>
       <c r="B25" t="s">
-        <v>231</v>
+        <v>404</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>229</v>
+        <v>208</v>
       </c>
       <c r="B26" t="s">
-        <v>230</v>
+        <v>214</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>236</v>
+        <v>209</v>
       </c>
       <c r="B27" t="s">
-        <v>235</v>
+        <v>215</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" t="s">
-        <v>238</v>
+        <v>210</v>
       </c>
       <c r="B28" t="s">
-        <v>237</v>
+        <v>216</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" t="s">
-        <v>240</v>
+        <v>218</v>
       </c>
       <c r="B29" t="s">
-        <v>239</v>
+        <v>217</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" t="s">
-        <v>241</v>
+        <v>231</v>
       </c>
       <c r="B30" t="s">
-        <v>239</v>
+        <v>229</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" t="s">
-        <v>242</v>
+        <v>230</v>
       </c>
       <c r="B31" t="s">
-        <v>244</v>
+        <v>228</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" t="s">
-        <v>243</v>
+        <v>226</v>
       </c>
       <c r="B32" t="s">
-        <v>245</v>
+        <v>227</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" t="s">
-        <v>249</v>
+        <v>233</v>
       </c>
       <c r="B33" t="s">
-        <v>248</v>
+        <v>232</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" t="s">
-        <v>252</v>
+        <v>235</v>
       </c>
       <c r="B34" t="s">
-        <v>251</v>
+        <v>234</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" t="s">
-        <v>253</v>
+        <v>237</v>
       </c>
       <c r="B35" t="s">
-        <v>254</v>
+        <v>236</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" t="s">
-        <v>222</v>
+        <v>398</v>
       </c>
       <c r="B36" t="s">
-        <v>250</v>
+        <v>399</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" t="s">
-        <v>223</v>
+        <v>238</v>
       </c>
       <c r="B37" t="s">
-        <v>255</v>
+        <v>240</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" t="s">
-        <v>224</v>
+        <v>239</v>
       </c>
       <c r="B38" t="s">
-        <v>256</v>
+        <v>241</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" t="s">
-        <v>261</v>
+        <v>245</v>
       </c>
       <c r="B39" t="s">
-        <v>265</v>
+        <v>244</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" t="s">
-        <v>267</v>
+        <v>248</v>
       </c>
       <c r="B40" t="s">
-        <v>266</v>
+        <v>247</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41" t="s">
-        <v>268</v>
+        <v>249</v>
       </c>
       <c r="B41" t="s">
-        <v>269</v>
+        <v>250</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" t="s">
-        <v>271</v>
+        <v>344</v>
       </c>
       <c r="B42" t="s">
-        <v>270</v>
+        <v>343</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43" t="s">
-        <v>262</v>
+        <v>219</v>
       </c>
       <c r="B43" t="s">
-        <v>273</v>
+        <v>246</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44" t="s">
-        <v>263</v>
+        <v>220</v>
       </c>
       <c r="B44" t="s">
-        <v>274</v>
+        <v>251</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" t="s">
-        <v>264</v>
+        <v>221</v>
       </c>
       <c r="B45" t="s">
-        <v>275</v>
+        <v>252</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46" t="s">
-        <v>277</v>
+        <v>257</v>
       </c>
       <c r="B46" t="s">
-        <v>276</v>
+        <v>261</v>
       </c>
     </row>
     <row r="47" spans="1:2">
       <c r="A47" t="s">
-        <v>281</v>
+        <v>263</v>
       </c>
       <c r="B47" t="s">
-        <v>282</v>
+        <v>262</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48" t="s">
-        <v>284</v>
+        <v>264</v>
       </c>
       <c r="B48" t="s">
-        <v>283</v>
+        <v>265</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49" t="s">
-        <v>278</v>
+        <v>267</v>
       </c>
       <c r="B49" t="s">
-        <v>280</v>
+        <v>266</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50" t="s">
-        <v>279</v>
+        <v>258</v>
       </c>
       <c r="B50" t="s">
-        <v>285</v>
+        <v>269</v>
       </c>
     </row>
     <row r="51" spans="1:2">
       <c r="A51" t="s">
-        <v>286</v>
+        <v>259</v>
       </c>
       <c r="B51" t="s">
-        <v>287</v>
+        <v>270</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52" t="s">
-        <v>288</v>
+        <v>260</v>
       </c>
       <c r="B52" t="s">
-        <v>290</v>
+        <v>271</v>
       </c>
     </row>
     <row r="53" spans="1:2">
       <c r="A53" t="s">
-        <v>289</v>
+        <v>273</v>
       </c>
       <c r="B53" t="s">
-        <v>291</v>
+        <v>272</v>
       </c>
     </row>
     <row r="54" spans="1:2">
       <c r="A54" t="s">
-        <v>294</v>
+        <v>277</v>
       </c>
       <c r="B54" t="s">
-        <v>293</v>
+        <v>278</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" t="s">
-        <v>298</v>
+        <v>280</v>
       </c>
       <c r="B55" t="s">
-        <v>299</v>
+        <v>279</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56" t="s">
-        <v>300</v>
+        <v>274</v>
       </c>
       <c r="B56" t="s">
-        <v>299</v>
+        <v>276</v>
       </c>
     </row>
     <row r="57" spans="1:2">
       <c r="A57" t="s">
-        <v>301</v>
+        <v>275</v>
       </c>
       <c r="B57" t="s">
-        <v>302</v>
+        <v>281</v>
       </c>
     </row>
     <row r="58" spans="1:2">
       <c r="A58" t="s">
-        <v>303</v>
+        <v>282</v>
       </c>
       <c r="B58" t="s">
-        <v>305</v>
+        <v>283</v>
       </c>
     </row>
     <row r="59" spans="1:2">
       <c r="A59" t="s">
-        <v>306</v>
+        <v>284</v>
       </c>
       <c r="B59" t="s">
-        <v>307</v>
+        <v>286</v>
       </c>
     </row>
     <row r="60" spans="1:2">
       <c r="A60" t="s">
-        <v>310</v>
+        <v>285</v>
       </c>
       <c r="B60" t="s">
-        <v>309</v>
+        <v>287</v>
       </c>
     </row>
     <row r="61" spans="1:2">
       <c r="A61" t="s">
-        <v>311</v>
+        <v>290</v>
       </c>
       <c r="B61" t="s">
-        <v>309</v>
+        <v>289</v>
       </c>
     </row>
     <row r="62" spans="1:2">
       <c r="A62" t="s">
-        <v>295</v>
+        <v>384</v>
       </c>
       <c r="B62" t="s">
-        <v>308</v>
+        <v>385</v>
       </c>
     </row>
     <row r="63" spans="1:2">
       <c r="A63" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B63" t="s">
-        <v>313</v>
+        <v>295</v>
       </c>
     </row>
     <row r="64" spans="1:2">
       <c r="A64" t="s">
+        <v>296</v>
+      </c>
+      <c r="B64" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
+      <c r="A65" t="s">
         <v>297</v>
       </c>
-      <c r="B64" t="s">
-        <v>312</v>
+      <c r="B65" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
+      <c r="A66" t="s">
+        <v>299</v>
+      </c>
+      <c r="B66" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2">
+      <c r="A67" t="s">
+        <v>302</v>
+      </c>
+      <c r="B67" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2">
+      <c r="A68" t="s">
+        <v>306</v>
+      </c>
+      <c r="B68" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2">
+      <c r="A69" t="s">
+        <v>307</v>
+      </c>
+      <c r="B69" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
+      <c r="A70" t="s">
+        <v>291</v>
+      </c>
+      <c r="B70" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2">
+      <c r="A71" t="s">
+        <v>292</v>
+      </c>
+      <c r="B71" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2">
+      <c r="A72" t="s">
+        <v>293</v>
+      </c>
+      <c r="B72" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2">
+      <c r="A73" t="s">
+        <v>359</v>
+      </c>
+      <c r="B73" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2">
+      <c r="A74" t="s">
+        <v>360</v>
+      </c>
+      <c r="B74" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2">
+      <c r="A75" t="s">
+        <v>361</v>
+      </c>
+      <c r="B75" t="s">
+        <v>364</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
made library changes and mail changes
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\55651C\Documents\UiPath\P002_090_PayCycleAfternoon_Dispatcher\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EB467CC-9978-4353-A609-F2DECE5423CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77B64ECB-C46C-4414-8293-81556DFE0A00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="405">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="403">
   <si>
     <t>Name</t>
   </si>
@@ -99,11 +99,11 @@
   </si>
   <si>
     <t>Orchestrator queue Name. The value must match with the queue name defined on Orchestrator.</t>
-    <phoneticPr fontId="16"/>
+    <phoneticPr fontId="18"/>
   </si>
   <si>
     <t>Logging field which allows grouping of log data of two or more subprocesses under the same business process name</t>
-    <phoneticPr fontId="16"/>
+    <phoneticPr fontId="18"/>
   </si>
   <si>
     <t>Must be 0 if working with Orchestrator queues. If &gt; 0, the robot will retry the same transaction which failed with a system exception. Must be an integer value.</t>
@@ -346,54 +346,6 @@
     <t>Shared folder Path for inputf files , templates and output files to be placed.</t>
   </si>
   <si>
-    <t>ExceptionTemplateName</t>
-  </si>
-  <si>
-    <t>Exception_Report.xlsx</t>
-  </si>
-  <si>
-    <t>Exception Template name which is kept in templates folder.</t>
-  </si>
-  <si>
-    <t>SummaryTemplateName</t>
-  </si>
-  <si>
-    <t>Summary_Report.xlsx</t>
-  </si>
-  <si>
-    <t>Summary Template name which is kept in Templates folder.</t>
-  </si>
-  <si>
-    <t>TemplateFolderName</t>
-  </si>
-  <si>
-    <t>Templates</t>
-  </si>
-  <si>
-    <t>Template folder name in shared drive</t>
-  </si>
-  <si>
-    <t>IncompleteData</t>
-  </si>
-  <si>
-    <t>Required Data missing</t>
-  </si>
-  <si>
-    <t>If any required data is missing.</t>
-  </si>
-  <si>
-    <t>ExceptionReportSheetName</t>
-  </si>
-  <si>
-    <t>Exception Report sheet name.</t>
-  </si>
-  <si>
-    <t>SummaryReportSheetName</t>
-  </si>
-  <si>
-    <t>Summary report sheet name.</t>
-  </si>
-  <si>
     <t>SUCCESS</t>
   </si>
   <si>
@@ -422,12 +374,6 @@
   </si>
   <si>
     <t>Outlook exe name to kill instance</t>
-  </si>
-  <si>
-    <t>UpdateReportTypeException</t>
-  </si>
-  <si>
-    <t>If exception report needs to be updated.</t>
   </si>
   <si>
     <t>UpdateReportBusinessExceptionType</t>
@@ -998,9 +944,6 @@
     <t>*</t>
   </si>
   <si>
-    <t>\d+\s-\s\w+\sno sbuccess</t>
-  </si>
-  <si>
     <t>RetryScopeContinueOnError</t>
   </si>
   <si>
@@ -1254,6 +1197,57 @@
   </si>
   <si>
     <t xml:space="preserve">Index for OKBATCNN job </t>
+  </si>
+  <si>
+    <t>MailFilterDate</t>
+  </si>
+  <si>
+    <t>BotEmailAddress</t>
+  </si>
+  <si>
+    <t>\d+\s-\s\w+\sno success</t>
+  </si>
+  <si>
+    <t>PeoplesoftLoginPageNotFoundSE</t>
+  </si>
+  <si>
+    <t>PeoplesoftLoginUnexpectedSE</t>
+  </si>
+  <si>
+    <t>Unexpected error encountered while logging into Peoplesoft. Refer to screenshot for error description</t>
+  </si>
+  <si>
+    <t>User ID field was not found in the log in page</t>
+  </si>
+  <si>
+    <t>C:\Users\55651C\Documents\UiPath\P002_090_PayCycleAfternoon_Dispatcher\Exceptions_Screenshots</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Navigation button was not found in Peoplesoft home page </t>
+  </si>
+  <si>
+    <t>NavigationButtonNotFoundSE</t>
+  </si>
+  <si>
+    <t>RefreshButtonNotFoundSE</t>
+  </si>
+  <si>
+    <t>Refresh Button was not found in the process monitor page or the page was not load in time</t>
+  </si>
+  <si>
+    <t>OrchestratorGraphAPIAssetsFolder</t>
+  </si>
+  <si>
+    <t>DEV</t>
+  </si>
+  <si>
+    <t>MarkEmailAsRead</t>
+  </si>
+  <si>
+    <t>BotPeoplesoftUserID</t>
+  </si>
+  <si>
+    <t>deepali.chaudhry@ey.com</t>
   </si>
 </sst>
 </file>
@@ -1263,11 +1257,25 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="25">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1456,60 +1464,63 @@
   </borders>
   <cellStyleXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="20" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="4" fontId="21" fillId="2" borderId="1" applyNumberFormat="0" applyProtection="0">
+    <xf numFmtId="4" fontId="23" fillId="2" borderId="1" applyNumberFormat="0" applyProtection="0">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="20"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="20"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="20" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="20" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="20" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="20" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="20" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="20" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="20" applyFont="1"/>
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="20" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="20" applyFont="1"/>
-    <xf numFmtId="49" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="20" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="20" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="20" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="20" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="20" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="24">
     <cellStyle name="Comma 2" xfId="2" xr:uid="{DA952E48-534A-4104-8A72-2BE892964A18}"/>
@@ -1847,10 +1858,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z104"/>
+  <dimension ref="A1:Z102"/>
   <sheetViews>
-    <sheetView topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="A75" sqref="A75"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="B92" sqref="B92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="14.5"/>
@@ -1897,10 +1908,10 @@
     </row>
     <row r="2" spans="1:26">
       <c r="A2" s="2" t="s">
-        <v>268</v>
+        <v>250</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>316</v>
+        <v>298</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>20</v>
@@ -1911,7 +1922,7 @@
         <v>28</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>323</v>
+        <v>304</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>29</v>
@@ -1922,7 +1933,7 @@
         <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>324</v>
+        <v>305</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>21</v>
@@ -1941,24 +1952,24 @@
     </row>
     <row r="6" spans="1:26">
       <c r="A6" t="s">
-        <v>388</v>
+        <v>369</v>
       </c>
       <c r="B6" t="s">
-        <v>389</v>
+        <v>370</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>390</v>
+        <v>371</v>
       </c>
     </row>
     <row r="7" spans="1:26">
       <c r="A7" t="s">
-        <v>391</v>
+        <v>372</v>
       </c>
       <c r="B7" t="s">
-        <v>392</v>
+        <v>373</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>393</v>
+        <v>374</v>
       </c>
     </row>
     <row r="8" spans="1:26">
@@ -1966,7 +1977,7 @@
         <v>44</v>
       </c>
       <c r="B8" t="s">
-        <v>176</v>
+        <v>158</v>
       </c>
       <c r="C8" t="s">
         <v>45</v>
@@ -1977,7 +1988,7 @@
         <v>46</v>
       </c>
       <c r="B9" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="C9" t="s">
         <v>47</v>
@@ -1987,8 +1998,8 @@
       <c r="A10" t="s">
         <v>48</v>
       </c>
-      <c r="B10" t="s">
-        <v>154</v>
+      <c r="B10" s="22" t="s">
+        <v>402</v>
       </c>
       <c r="C10" t="s">
         <v>49</v>
@@ -1999,7 +2010,7 @@
         <v>50</v>
       </c>
       <c r="B11" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="C11" t="s">
         <v>51</v>
@@ -2009,8 +2020,8 @@
       <c r="A12" t="s">
         <v>52</v>
       </c>
-      <c r="B12" t="s">
-        <v>154</v>
+      <c r="B12" s="22" t="s">
+        <v>402</v>
       </c>
       <c r="C12" t="s">
         <v>53</v>
@@ -2021,7 +2032,7 @@
         <v>54</v>
       </c>
       <c r="B13" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="C13" t="s">
         <v>55</v>
@@ -2032,7 +2043,7 @@
         <v>56</v>
       </c>
       <c r="B14" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="C14" t="s">
         <v>57</v>
@@ -2043,7 +2054,7 @@
         <v>58</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>288</v>
+        <v>270</v>
       </c>
       <c r="C15" t="s">
         <v>59</v>
@@ -2065,7 +2076,7 @@
         <v>63</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>155</v>
+        <v>137</v>
       </c>
       <c r="C17" t="s">
         <v>64</v>
@@ -2087,7 +2098,7 @@
         <v>68</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>156</v>
+        <v>138</v>
       </c>
       <c r="C19" t="s">
         <v>69</v>
@@ -2204,6 +2215,9 @@
       <c r="A30" t="s">
         <v>5</v>
       </c>
+      <c r="B30" t="s">
+        <v>393</v>
+      </c>
       <c r="C30" t="s">
         <v>99</v>
       </c>
@@ -2218,110 +2232,110 @@
       </c>
     </row>
     <row r="32" spans="1:3">
-      <c r="A32" t="s">
+      <c r="A32" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B32" t="s">
         <v>102</v>
       </c>
-      <c r="B32" t="s">
+      <c r="C32" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="C32" t="s">
+      <c r="B33" s="5" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="33" spans="1:3">
-      <c r="A33" t="s">
+      <c r="C33" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="B33" t="s">
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="C33" t="s">
+      <c r="B34" s="9" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="34" spans="1:3">
-      <c r="A34" t="s">
+      <c r="C34" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="B34" t="s">
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="C34" t="s">
+      <c r="B35" s="5" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="35" spans="1:3">
-      <c r="A35" t="s">
+      <c r="C35" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="B35" t="s">
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="C35" t="s">
+      <c r="B36" s="5" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="36" spans="1:3">
-      <c r="A36" t="s">
+      <c r="C36" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="B36" t="s">
-        <v>94</v>
-      </c>
-      <c r="C36" t="s">
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" s="5" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="37" spans="1:3">
-      <c r="A37" t="s">
+      <c r="B37" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="B37" t="s">
+      <c r="C37" s="5" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="B38" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="C37" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3">
-      <c r="A38" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="B38" t="s">
-        <v>118</v>
-      </c>
-      <c r="C38" t="s">
-        <v>162</v>
+      <c r="C38" s="5" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="39" spans="1:3">
-      <c r="A39" s="9" t="s">
-        <v>119</v>
-      </c>
-      <c r="B39" s="5" t="s">
+      <c r="A39" s="5" t="s">
         <v>120</v>
       </c>
+      <c r="B39" t="s">
+        <v>121</v>
+      </c>
       <c r="C39" s="5" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="40" spans="1:3">
-      <c r="A40" s="9" t="s">
-        <v>122</v>
-      </c>
-      <c r="B40" s="9" t="s">
+      <c r="A40" s="5" t="s">
         <v>123</v>
       </c>
+      <c r="B40" s="5" t="s">
+        <v>124</v>
+      </c>
       <c r="C40" s="5" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="B41" s="5" t="s">
         <v>126</v>
+      </c>
+      <c r="B41">
+        <v>5000</v>
       </c>
       <c r="C41" s="5" t="s">
         <v>127</v>
@@ -2331,8 +2345,8 @@
       <c r="A42" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="B42" s="5" t="s">
-        <v>94</v>
+      <c r="B42">
+        <v>5000</v>
       </c>
       <c r="C42" s="5" t="s">
         <v>129</v>
@@ -2342,531 +2356,492 @@
       <c r="A43" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="B43" s="5" t="s">
+      <c r="B43">
+        <v>2000</v>
+      </c>
+      <c r="C43" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="C43" s="5" t="s">
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" s="21" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="44" spans="1:3">
-      <c r="A44" s="5" t="s">
+      <c r="B44" t="b">
+        <v>1</v>
+      </c>
+      <c r="C44" s="5" t="s">
         <v>133</v>
-      </c>
-      <c r="B44" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="C44" s="5" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="B45" s="5" t="s">
-        <v>97</v>
+        <v>134</v>
+      </c>
+      <c r="B45">
+        <v>20</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" s="5" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="B46" t="s">
-        <v>139</v>
-      </c>
-      <c r="C46" s="5" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="B47" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="C47" s="5" t="s">
+      <c r="B47" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="48" spans="1:3">
-      <c r="A48" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="B48">
-        <v>5000</v>
-      </c>
-      <c r="C48" s="5" t="s">
+      <c r="A48" s="6" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="49" spans="1:3">
-      <c r="A49" s="5" t="s">
+      <c r="B48" t="s">
         <v>146</v>
       </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" s="11" t="s">
+        <v>147</v>
+      </c>
       <c r="B49">
-        <v>5000</v>
-      </c>
-      <c r="C49" s="5" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3">
-      <c r="A50" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="B50">
-        <v>2000</v>
-      </c>
-      <c r="C50" s="5" t="s">
+      <c r="B50" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="51" spans="1:3">
-      <c r="A51" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="B51" t="b">
+    <row r="51" spans="1:2">
+      <c r="A51" s="21" t="s">
+        <v>167</v>
+      </c>
+      <c r="B51">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="B52">
         <v>1</v>
       </c>
-      <c r="C51" s="5" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3">
-      <c r="A52" s="5" t="s">
-        <v>152</v>
-      </c>
-      <c r="B52">
-        <v>20</v>
-      </c>
-      <c r="C52" s="5" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3">
-      <c r="A53" s="5" t="s">
-        <v>159</v>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" s="7" t="s">
+        <v>181</v>
       </c>
       <c r="B53" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3">
-      <c r="A54" s="5" t="s">
-        <v>160</v>
+        <v>182</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54" s="7" t="s">
+        <v>183</v>
       </c>
       <c r="B54" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3">
-      <c r="A55" s="6" t="s">
-        <v>163</v>
+        <v>184</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" s="7" t="s">
+        <v>185</v>
       </c>
       <c r="B55" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3">
-      <c r="A56" s="11" t="s">
-        <v>165</v>
-      </c>
-      <c r="B56">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3">
-      <c r="A57" s="6" t="s">
-        <v>166</v>
+        <v>186</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="B56" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57" s="7" t="s">
+        <v>205</v>
       </c>
       <c r="B57" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
       <c r="A58" s="8" t="s">
-        <v>185</v>
-      </c>
-      <c r="B58">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3">
-      <c r="A59" s="7" t="s">
-        <v>198</v>
-      </c>
-      <c r="B59">
+        <v>206</v>
+      </c>
+      <c r="B58" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59" s="12" t="s">
+        <v>207</v>
+      </c>
+      <c r="B59" s="13" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60" s="8" t="s">
+        <v>225</v>
+      </c>
+      <c r="B60" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
+      <c r="A61" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="B61" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
+      <c r="A62" s="8" t="s">
+        <v>236</v>
+      </c>
+      <c r="B62" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
+      <c r="A63" s="12" t="s">
+        <v>282</v>
+      </c>
+      <c r="B63">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2">
+      <c r="A64" s="10" t="s">
+        <v>292</v>
+      </c>
+      <c r="B64" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
+      <c r="A65" s="20" t="s">
+        <v>386</v>
+      </c>
+      <c r="B65" t="str">
+        <f ca="1">TEXT(TODAY(), "yyyy-MM-dd")</f>
+        <v>2024-01-03</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
+      <c r="A66" s="11" t="s">
+        <v>293</v>
+      </c>
+      <c r="B66" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2">
+      <c r="A67" s="11" t="s">
+        <v>295</v>
+      </c>
+      <c r="B67" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2">
+      <c r="A68" s="12" t="s">
+        <v>301</v>
+      </c>
+      <c r="B68" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:3">
-      <c r="A60" s="7" t="s">
-        <v>199</v>
-      </c>
-      <c r="B60" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3">
-      <c r="A61" s="7" t="s">
-        <v>201</v>
-      </c>
-      <c r="B61" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3">
-      <c r="A62" s="7" t="s">
-        <v>203</v>
-      </c>
-      <c r="B62" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3">
-      <c r="A63" s="7" t="s">
-        <v>205</v>
-      </c>
-      <c r="B63" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3">
-      <c r="A64" s="7" t="s">
-        <v>223</v>
-      </c>
-      <c r="B64" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2">
-      <c r="A65" s="8" t="s">
-        <v>224</v>
-      </c>
-      <c r="B65" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2">
-      <c r="A66" s="12" t="s">
-        <v>225</v>
-      </c>
-      <c r="B66" s="13" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2">
-      <c r="A67" s="8" t="s">
-        <v>243</v>
-      </c>
-      <c r="B67" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2">
-      <c r="A68" s="8" t="s">
-        <v>255</v>
-      </c>
-      <c r="B68" t="s">
-        <v>253</v>
-      </c>
-    </row>
     <row r="69" spans="1:2">
-      <c r="A69" s="8" t="s">
-        <v>254</v>
-      </c>
-      <c r="B69" t="s">
-        <v>256</v>
+      <c r="A69" s="14" t="s">
+        <v>302</v>
+      </c>
+      <c r="B69" t="str">
+        <f ca="1">TEXT(TODAY(), "mm/dd/yyyy")</f>
+        <v>01/03/2024</v>
       </c>
     </row>
     <row r="70" spans="1:2">
-      <c r="A70" s="12" t="s">
-        <v>300</v>
-      </c>
-      <c r="B70">
-        <v>3</v>
+      <c r="A70" s="16" t="s">
+        <v>309</v>
+      </c>
+      <c r="B70" t="s">
+        <v>334</v>
       </c>
     </row>
     <row r="71" spans="1:2">
-      <c r="A71" s="10" t="s">
+      <c r="A71" s="15" t="s">
+        <v>308</v>
+      </c>
+      <c r="B71" t="s">
         <v>310</v>
       </c>
-      <c r="B71" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2">
-      <c r="A72" s="11" t="s">
-        <v>311</v>
-      </c>
-      <c r="B72" t="s">
-        <v>312</v>
+    </row>
+    <row r="72" spans="1:2" ht="58">
+      <c r="A72" s="15" t="s">
+        <v>314</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>381</v>
       </c>
     </row>
     <row r="73" spans="1:2">
-      <c r="A73" s="11" t="s">
-        <v>313</v>
-      </c>
-      <c r="B73" t="s">
-        <v>325</v>
+      <c r="A73" s="16" t="s">
+        <v>347</v>
+      </c>
+      <c r="B73" s="3">
+        <v>15</v>
       </c>
     </row>
     <row r="74" spans="1:2">
-      <c r="A74" s="12" t="s">
-        <v>320</v>
-      </c>
-      <c r="B74" t="b">
-        <v>1</v>
+      <c r="A74" s="19" t="s">
+        <v>382</v>
+      </c>
+      <c r="B74" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="75" spans="1:2">
-      <c r="A75" s="14" t="s">
-        <v>321</v>
-      </c>
-      <c r="B75" t="str">
-        <f ca="1">TEXT(TODAY(), "mm/dd/yyyy")</f>
-        <v>12/15/2023</v>
+      <c r="A75" s="16" t="s">
+        <v>315</v>
+      </c>
+      <c r="B75" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="76" spans="1:2">
       <c r="A76" s="16" t="s">
-        <v>328</v>
-      </c>
-      <c r="B76" t="s">
-        <v>353</v>
+        <v>316</v>
+      </c>
+      <c r="B76" s="22" t="s">
+        <v>402</v>
       </c>
     </row>
     <row r="77" spans="1:2">
-      <c r="A77" s="15" t="s">
-        <v>327</v>
+      <c r="A77" s="19" t="s">
+        <v>317</v>
       </c>
       <c r="B77" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" ht="58">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" ht="43.5">
       <c r="A78" s="15" t="s">
-        <v>333</v>
+        <v>318</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>400</v>
+        <v>375</v>
       </c>
     </row>
     <row r="79" spans="1:2">
       <c r="A79" s="16" t="s">
-        <v>366</v>
-      </c>
-      <c r="B79" s="3">
-        <v>15</v>
+        <v>319</v>
+      </c>
+      <c r="B79" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="80" spans="1:2">
-      <c r="A80" s="19" t="s">
-        <v>401</v>
-      </c>
-      <c r="B80" t="s">
-        <v>154</v>
+      <c r="A80" s="15" t="s">
+        <v>320</v>
+      </c>
+      <c r="B80" s="22" t="s">
+        <v>402</v>
       </c>
     </row>
     <row r="81" spans="1:2">
-      <c r="A81" s="16" t="s">
-        <v>334</v>
+      <c r="A81" s="15" t="s">
+        <v>326</v>
       </c>
       <c r="B81" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2">
-      <c r="A82" s="16" t="s">
-        <v>335</v>
-      </c>
-      <c r="B82" t="s">
-        <v>154</v>
+        <v>312</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" ht="29">
+      <c r="A82" s="15" t="s">
+        <v>327</v>
+      </c>
+      <c r="B82" s="3" t="s">
+        <v>376</v>
       </c>
     </row>
     <row r="83" spans="1:2">
-      <c r="A83" s="19" t="s">
-        <v>336</v>
+      <c r="A83" s="15" t="s">
+        <v>328</v>
       </c>
       <c r="B83" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2">
+      <c r="A84" s="15" t="s">
+        <v>329</v>
+      </c>
+      <c r="B84" s="22" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2">
+      <c r="A85" s="15" t="s">
         <v>330</v>
       </c>
-    </row>
-    <row r="84" spans="1:2" ht="43.5">
-      <c r="A84" s="15" t="s">
-        <v>337</v>
-      </c>
-      <c r="B84" s="3" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2">
-      <c r="A85" s="16" t="s">
-        <v>338</v>
-      </c>
       <c r="B85" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" ht="58">
       <c r="A86" s="15" t="s">
-        <v>339</v>
-      </c>
-      <c r="B86" t="s">
-        <v>154</v>
+        <v>331</v>
+      </c>
+      <c r="B86" s="3" t="s">
+        <v>377</v>
       </c>
     </row>
     <row r="87" spans="1:2">
       <c r="A87" s="15" t="s">
-        <v>345</v>
+        <v>332</v>
       </c>
       <c r="B87" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" ht="29">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2">
       <c r="A88" s="15" t="s">
-        <v>346</v>
-      </c>
-      <c r="B88" s="3" t="s">
-        <v>395</v>
+        <v>333</v>
+      </c>
+      <c r="B88" s="22" t="s">
+        <v>402</v>
       </c>
     </row>
     <row r="89" spans="1:2">
       <c r="A89" s="15" t="s">
-        <v>347</v>
+        <v>335</v>
       </c>
       <c r="B89" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" ht="29">
       <c r="A90" s="15" t="s">
-        <v>348</v>
-      </c>
-      <c r="B90" t="s">
-        <v>154</v>
+        <v>336</v>
+      </c>
+      <c r="B90" s="3" t="s">
+        <v>378</v>
       </c>
     </row>
     <row r="91" spans="1:2">
       <c r="A91" s="15" t="s">
+        <v>337</v>
+      </c>
+      <c r="B91" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2">
+      <c r="A92" s="15" t="s">
+        <v>338</v>
+      </c>
+      <c r="B92" s="22" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2">
+      <c r="A93" s="18" t="s">
+        <v>354</v>
+      </c>
+      <c r="B93" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2">
+      <c r="A94" s="17" t="s">
+        <v>355</v>
+      </c>
+      <c r="B94" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2">
+      <c r="A95" s="17" t="s">
+        <v>356</v>
+      </c>
+      <c r="B95" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2">
+      <c r="A96" t="s">
+        <v>353</v>
+      </c>
+      <c r="B96" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2">
+      <c r="A97" t="s">
         <v>349</v>
       </c>
-      <c r="B91" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" ht="58">
-      <c r="A92" s="15" t="s">
+      <c r="B97" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2">
+      <c r="A98" t="s">
+        <v>351</v>
+      </c>
+      <c r="B98" t="s">
         <v>350</v>
       </c>
-      <c r="B92" s="3" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2">
-      <c r="A93" s="15" t="s">
-        <v>351</v>
-      </c>
-      <c r="B93" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2">
-      <c r="A94" s="15" t="s">
-        <v>352</v>
-      </c>
-      <c r="B94" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2">
-      <c r="A95" s="15" t="s">
-        <v>354</v>
-      </c>
-      <c r="B95" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" ht="29">
-      <c r="A96" s="15" t="s">
-        <v>355</v>
-      </c>
-      <c r="B96" s="3" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2">
-      <c r="A97" s="15" t="s">
-        <v>356</v>
-      </c>
-      <c r="B97" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2">
-      <c r="A98" s="15" t="s">
-        <v>357</v>
-      </c>
-      <c r="B98" t="s">
-        <v>154</v>
-      </c>
     </row>
     <row r="99" spans="1:2">
-      <c r="A99" s="18" t="s">
-        <v>373</v>
+      <c r="A99" t="s">
+        <v>387</v>
       </c>
       <c r="B99" t="s">
-        <v>376</v>
+        <v>136</v>
       </c>
     </row>
     <row r="100" spans="1:2">
-      <c r="A100" s="17" t="s">
-        <v>374</v>
+      <c r="A100" t="s">
+        <v>398</v>
       </c>
       <c r="B100" t="s">
-        <v>377</v>
+        <v>399</v>
       </c>
     </row>
     <row r="101" spans="1:2">
-      <c r="A101" s="17" t="s">
-        <v>375</v>
-      </c>
-      <c r="B101" t="s">
-        <v>378</v>
+      <c r="A101" t="s">
+        <v>400</v>
+      </c>
+      <c r="B101" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="102" spans="1:2">
       <c r="A102" t="s">
-        <v>372</v>
-      </c>
-      <c r="B102" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2">
-      <c r="A103" t="s">
-        <v>368</v>
-      </c>
-      <c r="B103" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2">
-      <c r="A104" t="s">
-        <v>370</v>
-      </c>
-      <c r="B104" t="s">
-        <v>369</v>
+        <v>401</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="16"/>
+  <phoneticPr fontId="18"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -4030,7 +4005,7 @@
     <row r="987" ht="14.25" customHeight="1"/>
     <row r="988" ht="14.25" customHeight="1"/>
   </sheetData>
-  <phoneticPr fontId="16"/>
+  <phoneticPr fontId="18"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -4056,7 +4031,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>317</v>
+        <v>299</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>27</v>
@@ -4089,24 +4064,24 @@
     </row>
     <row r="2" spans="1:26">
       <c r="A2" t="s">
-        <v>315</v>
+        <v>297</v>
       </c>
       <c r="B2" t="s">
-        <v>314</v>
+        <v>296</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="16"/>
+  <phoneticPr fontId="18"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1D9DC59-3960-42CB-B3EC-EFF452A90D4F}">
-  <dimension ref="A1:Z75"/>
+  <dimension ref="A1:Z79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -4152,594 +4127,626 @@
     </row>
     <row r="2" spans="1:26">
       <c r="A2" t="s">
-        <v>168</v>
+        <v>150</v>
       </c>
       <c r="B2" t="s">
-        <v>169</v>
+        <v>151</v>
       </c>
     </row>
     <row r="3" spans="1:26">
       <c r="A3" t="s">
-        <v>380</v>
+        <v>361</v>
       </c>
       <c r="B3" t="s">
-        <v>381</v>
+        <v>362</v>
       </c>
     </row>
     <row r="4" spans="1:26">
       <c r="A4" t="s">
-        <v>379</v>
+        <v>360</v>
       </c>
       <c r="B4" t="s">
-        <v>326</v>
+        <v>307</v>
       </c>
     </row>
     <row r="5" spans="1:26">
       <c r="A5" t="s">
-        <v>170</v>
+        <v>152</v>
       </c>
       <c r="B5" t="s">
-        <v>171</v>
+        <v>153</v>
       </c>
     </row>
     <row r="6" spans="1:26">
       <c r="A6" t="s">
-        <v>172</v>
+        <v>154</v>
       </c>
       <c r="B6" t="s">
-        <v>173</v>
+        <v>155</v>
       </c>
     </row>
     <row r="7" spans="1:26">
       <c r="A7" t="s">
-        <v>174</v>
+        <v>156</v>
       </c>
       <c r="B7" t="s">
-        <v>175</v>
+        <v>157</v>
       </c>
     </row>
     <row r="8" spans="1:26">
       <c r="A8" t="s">
-        <v>178</v>
+        <v>160</v>
       </c>
       <c r="B8" t="s">
-        <v>177</v>
+        <v>159</v>
       </c>
     </row>
     <row r="9" spans="1:26">
       <c r="A9" t="s">
-        <v>181</v>
+        <v>163</v>
       </c>
       <c r="B9" t="s">
-        <v>182</v>
+        <v>164</v>
       </c>
     </row>
     <row r="10" spans="1:26">
       <c r="A10" t="s">
-        <v>386</v>
+        <v>367</v>
       </c>
       <c r="B10" t="s">
-        <v>382</v>
+        <v>363</v>
       </c>
     </row>
     <row r="11" spans="1:26">
       <c r="A11" t="s">
-        <v>387</v>
+        <v>368</v>
       </c>
       <c r="B11" t="s">
-        <v>383</v>
+        <v>364</v>
       </c>
     </row>
     <row r="12" spans="1:26">
       <c r="A12" t="s">
-        <v>179</v>
+        <v>389</v>
       </c>
       <c r="B12" t="s">
-        <v>183</v>
+        <v>392</v>
       </c>
     </row>
     <row r="13" spans="1:26">
       <c r="A13" t="s">
-        <v>180</v>
+        <v>390</v>
       </c>
       <c r="B13" t="s">
-        <v>184</v>
+        <v>391</v>
       </c>
     </row>
     <row r="14" spans="1:26">
       <c r="A14" t="s">
-        <v>186</v>
+        <v>161</v>
       </c>
       <c r="B14" t="s">
-        <v>189</v>
+        <v>165</v>
       </c>
     </row>
     <row r="15" spans="1:26">
       <c r="A15" t="s">
-        <v>187</v>
+        <v>162</v>
       </c>
       <c r="B15" t="s">
-        <v>190</v>
+        <v>166</v>
       </c>
     </row>
     <row r="16" spans="1:26">
       <c r="A16" t="s">
-        <v>188</v>
+        <v>168</v>
       </c>
       <c r="B16" t="s">
-        <v>191</v>
+        <v>171</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>192</v>
+        <v>395</v>
       </c>
       <c r="B17" t="s">
-        <v>195</v>
+        <v>394</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>193</v>
+        <v>169</v>
       </c>
       <c r="B18" t="s">
-        <v>196</v>
+        <v>172</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>194</v>
+        <v>170</v>
       </c>
       <c r="B19" t="s">
-        <v>197</v>
+        <v>173</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>207</v>
+        <v>174</v>
       </c>
       <c r="B20" t="s">
-        <v>213</v>
+        <v>177</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>340</v>
+        <v>396</v>
       </c>
       <c r="B21" t="s">
-        <v>342</v>
+        <v>397</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>341</v>
+        <v>175</v>
       </c>
       <c r="B22" t="s">
-        <v>342</v>
+        <v>178</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>212</v>
+        <v>176</v>
       </c>
       <c r="B23" t="s">
-        <v>211</v>
+        <v>179</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>402</v>
+        <v>189</v>
       </c>
       <c r="B24" t="s">
-        <v>403</v>
+        <v>195</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>365</v>
+        <v>321</v>
       </c>
       <c r="B25" t="s">
-        <v>404</v>
+        <v>323</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>208</v>
+        <v>322</v>
       </c>
       <c r="B26" t="s">
-        <v>214</v>
+        <v>323</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>209</v>
+        <v>194</v>
       </c>
       <c r="B27" t="s">
-        <v>215</v>
+        <v>193</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" t="s">
-        <v>210</v>
+        <v>383</v>
       </c>
       <c r="B28" t="s">
-        <v>216</v>
+        <v>384</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" t="s">
-        <v>218</v>
+        <v>346</v>
       </c>
       <c r="B29" t="s">
-        <v>217</v>
+        <v>385</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" t="s">
-        <v>231</v>
+        <v>190</v>
       </c>
       <c r="B30" t="s">
-        <v>229</v>
+        <v>196</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" t="s">
-        <v>230</v>
+        <v>191</v>
       </c>
       <c r="B31" t="s">
-        <v>228</v>
+        <v>197</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" t="s">
-        <v>226</v>
+        <v>192</v>
       </c>
       <c r="B32" t="s">
-        <v>227</v>
+        <v>198</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" t="s">
-        <v>233</v>
+        <v>200</v>
       </c>
       <c r="B33" t="s">
-        <v>232</v>
+        <v>199</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" t="s">
-        <v>235</v>
+        <v>213</v>
       </c>
       <c r="B34" t="s">
-        <v>234</v>
+        <v>211</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" t="s">
-        <v>237</v>
+        <v>212</v>
       </c>
       <c r="B35" t="s">
-        <v>236</v>
+        <v>210</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" t="s">
-        <v>398</v>
+        <v>208</v>
       </c>
       <c r="B36" t="s">
-        <v>399</v>
+        <v>209</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" t="s">
-        <v>238</v>
+        <v>215</v>
       </c>
       <c r="B37" t="s">
-        <v>240</v>
+        <v>214</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" t="s">
-        <v>239</v>
+        <v>217</v>
       </c>
       <c r="B38" t="s">
-        <v>241</v>
+        <v>216</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" t="s">
-        <v>245</v>
+        <v>219</v>
       </c>
       <c r="B39" t="s">
-        <v>244</v>
+        <v>218</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" t="s">
-        <v>248</v>
+        <v>379</v>
       </c>
       <c r="B40" t="s">
-        <v>247</v>
+        <v>380</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41" t="s">
-        <v>249</v>
+        <v>220</v>
       </c>
       <c r="B41" t="s">
-        <v>250</v>
+        <v>222</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" t="s">
-        <v>344</v>
+        <v>221</v>
       </c>
       <c r="B42" t="s">
-        <v>343</v>
+        <v>223</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43" t="s">
-        <v>219</v>
+        <v>227</v>
       </c>
       <c r="B43" t="s">
-        <v>246</v>
+        <v>226</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44" t="s">
-        <v>220</v>
+        <v>230</v>
       </c>
       <c r="B44" t="s">
-        <v>251</v>
+        <v>229</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" t="s">
-        <v>221</v>
+        <v>231</v>
       </c>
       <c r="B45" t="s">
-        <v>252</v>
+        <v>232</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46" t="s">
-        <v>257</v>
+        <v>325</v>
       </c>
       <c r="B46" t="s">
-        <v>261</v>
+        <v>324</v>
       </c>
     </row>
     <row r="47" spans="1:2">
       <c r="A47" t="s">
-        <v>263</v>
+        <v>201</v>
       </c>
       <c r="B47" t="s">
-        <v>262</v>
+        <v>228</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48" t="s">
-        <v>264</v>
+        <v>202</v>
       </c>
       <c r="B48" t="s">
-        <v>265</v>
+        <v>233</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49" t="s">
-        <v>267</v>
+        <v>203</v>
       </c>
       <c r="B49" t="s">
-        <v>266</v>
+        <v>234</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50" t="s">
-        <v>258</v>
+        <v>239</v>
       </c>
       <c r="B50" t="s">
-        <v>269</v>
+        <v>243</v>
       </c>
     </row>
     <row r="51" spans="1:2">
       <c r="A51" t="s">
-        <v>259</v>
+        <v>245</v>
       </c>
       <c r="B51" t="s">
-        <v>270</v>
+        <v>244</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52" t="s">
-        <v>260</v>
+        <v>246</v>
       </c>
       <c r="B52" t="s">
-        <v>271</v>
+        <v>247</v>
       </c>
     </row>
     <row r="53" spans="1:2">
       <c r="A53" t="s">
-        <v>273</v>
+        <v>249</v>
       </c>
       <c r="B53" t="s">
-        <v>272</v>
+        <v>248</v>
       </c>
     </row>
     <row r="54" spans="1:2">
       <c r="A54" t="s">
-        <v>277</v>
+        <v>240</v>
       </c>
       <c r="B54" t="s">
-        <v>278</v>
+        <v>251</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" t="s">
-        <v>280</v>
+        <v>241</v>
       </c>
       <c r="B55" t="s">
-        <v>279</v>
+        <v>252</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56" t="s">
-        <v>274</v>
+        <v>242</v>
       </c>
       <c r="B56" t="s">
-        <v>276</v>
+        <v>253</v>
       </c>
     </row>
     <row r="57" spans="1:2">
       <c r="A57" t="s">
-        <v>275</v>
+        <v>255</v>
       </c>
       <c r="B57" t="s">
-        <v>281</v>
+        <v>254</v>
       </c>
     </row>
     <row r="58" spans="1:2">
       <c r="A58" t="s">
-        <v>282</v>
+        <v>259</v>
       </c>
       <c r="B58" t="s">
-        <v>283</v>
+        <v>260</v>
       </c>
     </row>
     <row r="59" spans="1:2">
       <c r="A59" t="s">
-        <v>284</v>
+        <v>262</v>
       </c>
       <c r="B59" t="s">
-        <v>286</v>
+        <v>261</v>
       </c>
     </row>
     <row r="60" spans="1:2">
       <c r="A60" t="s">
-        <v>285</v>
+        <v>256</v>
       </c>
       <c r="B60" t="s">
-        <v>287</v>
+        <v>258</v>
       </c>
     </row>
     <row r="61" spans="1:2">
       <c r="A61" t="s">
-        <v>290</v>
+        <v>257</v>
       </c>
       <c r="B61" t="s">
-        <v>289</v>
+        <v>263</v>
       </c>
     </row>
     <row r="62" spans="1:2">
       <c r="A62" t="s">
-        <v>384</v>
+        <v>264</v>
       </c>
       <c r="B62" t="s">
-        <v>385</v>
+        <v>265</v>
       </c>
     </row>
     <row r="63" spans="1:2">
       <c r="A63" t="s">
-        <v>294</v>
+        <v>266</v>
       </c>
       <c r="B63" t="s">
-        <v>295</v>
+        <v>268</v>
       </c>
     </row>
     <row r="64" spans="1:2">
       <c r="A64" t="s">
-        <v>296</v>
+        <v>267</v>
       </c>
       <c r="B64" t="s">
-        <v>295</v>
+        <v>269</v>
       </c>
     </row>
     <row r="65" spans="1:2">
       <c r="A65" t="s">
-        <v>297</v>
+        <v>272</v>
       </c>
       <c r="B65" t="s">
-        <v>298</v>
+        <v>271</v>
       </c>
     </row>
     <row r="66" spans="1:2">
       <c r="A66" t="s">
-        <v>299</v>
+        <v>365</v>
       </c>
       <c r="B66" t="s">
-        <v>301</v>
+        <v>366</v>
       </c>
     </row>
     <row r="67" spans="1:2">
       <c r="A67" t="s">
-        <v>302</v>
+        <v>276</v>
       </c>
       <c r="B67" t="s">
-        <v>303</v>
+        <v>277</v>
       </c>
     </row>
     <row r="68" spans="1:2">
       <c r="A68" t="s">
-        <v>306</v>
+        <v>278</v>
       </c>
       <c r="B68" t="s">
-        <v>305</v>
+        <v>277</v>
       </c>
     </row>
     <row r="69" spans="1:2">
       <c r="A69" t="s">
-        <v>307</v>
+        <v>279</v>
       </c>
       <c r="B69" t="s">
-        <v>305</v>
+        <v>280</v>
       </c>
     </row>
     <row r="70" spans="1:2">
       <c r="A70" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="B70" t="s">
-        <v>304</v>
+        <v>283</v>
       </c>
     </row>
     <row r="71" spans="1:2">
       <c r="A71" t="s">
-        <v>292</v>
+        <v>284</v>
       </c>
       <c r="B71" t="s">
-        <v>309</v>
+        <v>285</v>
       </c>
     </row>
     <row r="72" spans="1:2">
       <c r="A72" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="B72" t="s">
-        <v>308</v>
+        <v>287</v>
       </c>
     </row>
     <row r="73" spans="1:2">
       <c r="A73" t="s">
-        <v>359</v>
+        <v>289</v>
       </c>
       <c r="B73" t="s">
-        <v>362</v>
+        <v>287</v>
       </c>
     </row>
     <row r="74" spans="1:2">
       <c r="A74" t="s">
-        <v>360</v>
+        <v>273</v>
       </c>
       <c r="B74" t="s">
-        <v>363</v>
+        <v>286</v>
       </c>
     </row>
     <row r="75" spans="1:2">
       <c r="A75" t="s">
-        <v>361</v>
+        <v>274</v>
       </c>
       <c r="B75" t="s">
-        <v>364</v>
+        <v>291</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2">
+      <c r="A76" t="s">
+        <v>275</v>
+      </c>
+      <c r="B76" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2">
+      <c r="A77" t="s">
+        <v>340</v>
+      </c>
+      <c r="B77" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2">
+      <c r="A78" t="s">
+        <v>341</v>
+      </c>
+      <c r="B78" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2">
+      <c r="A79" t="s">
+        <v>342</v>
+      </c>
+      <c r="B79" t="s">
+        <v>345</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changes in error screenshots and login.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\55651C\Documents\UiPath\P002_090_PayCycleAfternoon_Dispatcher\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77B64ECB-C46C-4414-8293-81556DFE0A00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5407F702-C161-42FE-B2CA-08FFE1CB057F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="403">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="407">
   <si>
     <t>Name</t>
   </si>
@@ -99,11 +99,11 @@
   </si>
   <si>
     <t>Orchestrator queue Name. The value must match with the queue name defined on Orchestrator.</t>
-    <phoneticPr fontId="18"/>
+    <phoneticPr fontId="19"/>
   </si>
   <si>
     <t>Logging field which allows grouping of log data of two or more subprocesses under the same business process name</t>
-    <phoneticPr fontId="18"/>
+    <phoneticPr fontId="19"/>
   </si>
   <si>
     <t>Must be 0 if working with Orchestrator queues. If &gt; 0, the robot will retry the same transaction which failed with a system exception. Must be an integer value.</t>
@@ -161,9 +161,6 @@
   </si>
   <si>
     <t xml:space="preserve">The maximum number of consecutive system exceptions was reached. </t>
-  </si>
-  <si>
-    <t>https://soklfpub-tst.opc.oracleoutsourcing.com/psp/SOKLFTSTNSS/?cmd=login&amp;languageCd=ENG&amp;</t>
   </si>
   <si>
     <t>PeopleSoft URL for lauching the web application.</t>
@@ -950,9 +947,6 @@
     <t>QueueReference</t>
   </si>
   <si>
-    <t>00:00:20</t>
-  </si>
-  <si>
     <t>udbhavagarwal's workspace</t>
   </si>
   <si>
@@ -1205,49 +1199,67 @@
     <t>BotEmailAddress</t>
   </si>
   <si>
+    <t>PeoplesoftLoginPageNotFoundSE</t>
+  </si>
+  <si>
+    <t>PeoplesoftLoginUnexpectedSE</t>
+  </si>
+  <si>
+    <t>Unexpected error encountered while logging into Peoplesoft. Refer to screenshot for error description</t>
+  </si>
+  <si>
+    <t>User ID field was not found in the log in page</t>
+  </si>
+  <si>
+    <t>C:\Users\55651C\Documents\UiPath\P002_090_PayCycleAfternoon_Dispatcher\Exceptions_Screenshots</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Navigation button was not found in Peoplesoft home page </t>
+  </si>
+  <si>
+    <t>NavigationButtonNotFoundSE</t>
+  </si>
+  <si>
+    <t>RefreshButtonNotFoundSE</t>
+  </si>
+  <si>
+    <t>Refresh Button was not found in the process monitor page or the page was not load in time</t>
+  </si>
+  <si>
+    <t>OrchestratorGraphAPIAssetsFolder</t>
+  </si>
+  <si>
+    <t>DEV</t>
+  </si>
+  <si>
+    <t>MarkEmailAsRead</t>
+  </si>
+  <si>
+    <t>BotPeoplesoftUserID</t>
+  </si>
+  <si>
+    <t>deepali.chaudhry@ey.com</t>
+  </si>
+  <si>
+    <t>00:00:30</t>
+  </si>
+  <si>
+    <t>LoginRetries</t>
+  </si>
+  <si>
+    <t>Error in retry scope for login</t>
+  </si>
+  <si>
+    <t>LoginRetryScopeError</t>
+  </si>
+  <si>
+    <t>ErrorScreenShotPath</t>
+  </si>
+  <si>
+    <t>https://soklfpub-tst.opc.oracleoutsourcing.com/psp/SOKLFTSTNSS/?cmd=login&amp;languageCd=ENG&amp;</t>
+  </si>
+  <si>
     <t>\d+\s-\s\w+\sno success</t>
-  </si>
-  <si>
-    <t>PeoplesoftLoginPageNotFoundSE</t>
-  </si>
-  <si>
-    <t>PeoplesoftLoginUnexpectedSE</t>
-  </si>
-  <si>
-    <t>Unexpected error encountered while logging into Peoplesoft. Refer to screenshot for error description</t>
-  </si>
-  <si>
-    <t>User ID field was not found in the log in page</t>
-  </si>
-  <si>
-    <t>C:\Users\55651C\Documents\UiPath\P002_090_PayCycleAfternoon_Dispatcher\Exceptions_Screenshots</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Navigation button was not found in Peoplesoft home page </t>
-  </si>
-  <si>
-    <t>NavigationButtonNotFoundSE</t>
-  </si>
-  <si>
-    <t>RefreshButtonNotFoundSE</t>
-  </si>
-  <si>
-    <t>Refresh Button was not found in the process monitor page or the page was not load in time</t>
-  </si>
-  <si>
-    <t>OrchestratorGraphAPIAssetsFolder</t>
-  </si>
-  <si>
-    <t>DEV</t>
-  </si>
-  <si>
-    <t>MarkEmailAsRead</t>
-  </si>
-  <si>
-    <t>BotPeoplesoftUserID</t>
-  </si>
-  <si>
-    <t>deepali.chaudhry@ey.com</t>
   </si>
 </sst>
 </file>
@@ -1257,11 +1269,18 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="25">
+  <fonts count="26">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1464,54 +1483,55 @@
   </borders>
   <cellStyleXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="20" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="4" fontId="23" fillId="2" borderId="1" applyNumberFormat="0" applyProtection="0">
+    <xf numFmtId="4" fontId="24" fillId="2" borderId="1" applyNumberFormat="0" applyProtection="0">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="20"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="20"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="20" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="20" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="20" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="20" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="20" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="20" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="20" applyFont="1"/>
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="20" applyFont="1"/>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="20" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="20" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="20" applyFont="1"/>
@@ -1520,7 +1540,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="20" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="20" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="20" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="24">
     <cellStyle name="Comma 2" xfId="2" xr:uid="{DA952E48-534A-4104-8A72-2BE892964A18}"/>
@@ -1858,10 +1877,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z102"/>
+  <dimension ref="A1:Z104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="B92" sqref="B92"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="B93" sqref="B93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="14.5"/>
@@ -1908,10 +1927,10 @@
     </row>
     <row r="2" spans="1:26">
       <c r="A2" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>20</v>
@@ -1922,7 +1941,7 @@
         <v>28</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>29</v>
@@ -1933,7 +1952,7 @@
         <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>21</v>
@@ -1941,274 +1960,274 @@
     </row>
     <row r="5" spans="1:26">
       <c r="A5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B5" t="s">
+        <v>405</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>41</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:26">
       <c r="A6" t="s">
+        <v>367</v>
+      </c>
+      <c r="B6" t="s">
+        <v>368</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>369</v>
-      </c>
-      <c r="B6" t="s">
-        <v>370</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>371</v>
       </c>
     </row>
     <row r="7" spans="1:26">
       <c r="A7" t="s">
+        <v>370</v>
+      </c>
+      <c r="B7" t="s">
+        <v>371</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>372</v>
-      </c>
-      <c r="B7" t="s">
-        <v>373</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>374</v>
       </c>
     </row>
     <row r="8" spans="1:26">
       <c r="A8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" t="s">
+        <v>157</v>
+      </c>
+      <c r="C8" t="s">
         <v>44</v>
-      </c>
-      <c r="B8" t="s">
-        <v>158</v>
-      </c>
-      <c r="C8" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:26">
       <c r="A9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" t="s">
+        <v>135</v>
+      </c>
+      <c r="C9" t="s">
         <v>46</v>
-      </c>
-      <c r="B9" t="s">
-        <v>136</v>
-      </c>
-      <c r="C9" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:26">
       <c r="A10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" t="s">
+        <v>399</v>
+      </c>
+      <c r="C10" t="s">
         <v>48</v>
-      </c>
-      <c r="B10" s="22" t="s">
-        <v>402</v>
-      </c>
-      <c r="C10" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:26">
       <c r="A11" t="s">
+        <v>49</v>
+      </c>
+      <c r="B11" t="s">
+        <v>135</v>
+      </c>
+      <c r="C11" t="s">
         <v>50</v>
-      </c>
-      <c r="B11" t="s">
-        <v>136</v>
-      </c>
-      <c r="C11" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:26">
       <c r="A12" t="s">
+        <v>51</v>
+      </c>
+      <c r="B12" t="s">
+        <v>399</v>
+      </c>
+      <c r="C12" t="s">
         <v>52</v>
-      </c>
-      <c r="B12" s="22" t="s">
-        <v>402</v>
-      </c>
-      <c r="C12" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:26">
       <c r="A13" t="s">
+        <v>53</v>
+      </c>
+      <c r="B13" t="s">
+        <v>135</v>
+      </c>
+      <c r="C13" t="s">
         <v>54</v>
-      </c>
-      <c r="B13" t="s">
-        <v>136</v>
-      </c>
-      <c r="C13" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:26">
       <c r="A14" t="s">
+        <v>55</v>
+      </c>
+      <c r="B14" t="s">
+        <v>135</v>
+      </c>
+      <c r="C14" t="s">
         <v>56</v>
-      </c>
-      <c r="B14" t="s">
-        <v>136</v>
-      </c>
-      <c r="C14" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="43.5">
       <c r="A15" t="s">
+        <v>57</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>269</v>
+      </c>
+      <c r="C15" t="s">
         <v>58</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>270</v>
-      </c>
-      <c r="C15" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:26">
       <c r="A16" t="s">
+        <v>59</v>
+      </c>
+      <c r="B16" t="s">
         <v>60</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>61</v>
-      </c>
-      <c r="C16" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="43.5">
       <c r="A17" t="s">
+        <v>62</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="C17" t="s">
         <v>63</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="C17" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
+        <v>64</v>
+      </c>
+      <c r="B18" t="s">
         <v>65</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>66</v>
-      </c>
-      <c r="C18" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="43.5">
       <c r="A19" t="s">
+        <v>67</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="C19" t="s">
         <v>68</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="C19" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
+        <v>69</v>
+      </c>
+      <c r="B20" t="s">
         <v>70</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>71</v>
-      </c>
-      <c r="C20" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
+        <v>72</v>
+      </c>
+      <c r="B21" t="s">
         <v>73</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>74</v>
-      </c>
-      <c r="C21" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
+        <v>75</v>
+      </c>
+      <c r="B22" t="s">
         <v>76</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>77</v>
-      </c>
-      <c r="C22" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
+        <v>78</v>
+      </c>
+      <c r="B23" t="s">
         <v>79</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
         <v>80</v>
-      </c>
-      <c r="C23" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
+        <v>81</v>
+      </c>
+      <c r="B24" t="s">
         <v>82</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
         <v>83</v>
-      </c>
-      <c r="C24" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
+        <v>84</v>
+      </c>
+      <c r="C25" t="s">
         <v>85</v>
-      </c>
-      <c r="C25" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
+        <v>86</v>
+      </c>
+      <c r="B26" t="s">
         <v>87</v>
       </c>
-      <c r="B26" t="s">
+      <c r="C26" t="s">
         <v>88</v>
-      </c>
-      <c r="C26" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
+        <v>89</v>
+      </c>
+      <c r="B27" t="s">
         <v>90</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" t="s">
         <v>91</v>
-      </c>
-      <c r="C27" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
+        <v>92</v>
+      </c>
+      <c r="B28" t="s">
         <v>93</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C28" t="s">
         <v>94</v>
-      </c>
-      <c r="C28" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
+        <v>95</v>
+      </c>
+      <c r="B29" t="s">
         <v>96</v>
       </c>
-      <c r="B29" t="s">
+      <c r="C29" t="s">
         <v>97</v>
-      </c>
-      <c r="C29" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -2216,202 +2235,202 @@
         <v>5</v>
       </c>
       <c r="B30" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="C30" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B31" s="3"/>
       <c r="C31" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B32" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C32" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="B33" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="B33" s="5" t="s">
+      <c r="C33" s="5" t="s">
         <v>104</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="B34" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="B34" s="9" t="s">
+      <c r="C34" s="5" t="s">
         <v>107</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="B35" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="B35" s="5" t="s">
+      <c r="C35" s="5" t="s">
         <v>110</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="B36" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="B36" s="5" t="s">
+      <c r="C36" s="5" t="s">
         <v>113</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="B37" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="B37" s="5" t="s">
+      <c r="C37" s="5" t="s">
         <v>116</v>
-      </c>
-      <c r="C37" s="5" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C38" s="5" t="s">
         <v>118</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="C38" s="5" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="B39" t="s">
         <v>120</v>
       </c>
-      <c r="B39" t="s">
+      <c r="C39" s="5" t="s">
         <v>121</v>
-      </c>
-      <c r="C39" s="5" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B40" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="B40" s="5" t="s">
+      <c r="C40" s="5" t="s">
         <v>124</v>
-      </c>
-      <c r="C40" s="5" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B41">
         <v>5000</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B42">
         <v>5000</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B43">
         <v>2000</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B44" t="b">
         <v>1</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B45">
         <v>20</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B46" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="B47" t="s">
         <v>142</v>
-      </c>
-      <c r="B47" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="B48" t="s">
         <v>145</v>
-      </c>
-      <c r="B48" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49" s="11" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B49">
         <v>5</v>
@@ -2419,15 +2438,15 @@
     </row>
     <row r="50" spans="1:2">
       <c r="A50" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="B50" t="s">
         <v>148</v>
-      </c>
-      <c r="B50" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="51" spans="1:2">
       <c r="A51" s="21" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B51">
         <v>5</v>
@@ -2435,7 +2454,7 @@
     </row>
     <row r="52" spans="1:2">
       <c r="A52" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B52">
         <v>1</v>
@@ -2443,87 +2462,87 @@
     </row>
     <row r="53" spans="1:2">
       <c r="A53" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="B53" t="s">
         <v>181</v>
-      </c>
-      <c r="B53" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="54" spans="1:2">
       <c r="A54" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="B54" t="s">
         <v>183</v>
-      </c>
-      <c r="B54" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="B55" t="s">
         <v>185</v>
-      </c>
-      <c r="B55" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="B56" t="s">
         <v>187</v>
-      </c>
-      <c r="B56" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="57" spans="1:2">
       <c r="A57" s="7" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B57" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="58" spans="1:2">
       <c r="A58" s="8" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B58" t="s">
-        <v>388</v>
+        <v>406</v>
       </c>
     </row>
     <row r="59" spans="1:2">
       <c r="A59" s="12" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B59" s="13" t="s">
-        <v>303</v>
+        <v>400</v>
       </c>
     </row>
     <row r="60" spans="1:2">
       <c r="A60" s="8" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B60" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="61" spans="1:2">
       <c r="A61" s="8" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B61" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="62" spans="1:2">
       <c r="A62" s="8" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B62" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="63" spans="1:2">
       <c r="A63" s="12" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B63">
         <v>3</v>
@@ -2531,40 +2550,40 @@
     </row>
     <row r="64" spans="1:2">
       <c r="A64" s="10" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B64" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="65" spans="1:2">
       <c r="A65" s="20" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="B65" t="str">
         <f ca="1">TEXT(TODAY(), "yyyy-MM-dd")</f>
-        <v>2024-01-03</v>
+        <v>2024-01-04</v>
       </c>
     </row>
     <row r="66" spans="1:2">
       <c r="A66" s="11" t="s">
+        <v>292</v>
+      </c>
+      <c r="B66" t="s">
         <v>293</v>
-      </c>
-      <c r="B66" t="s">
-        <v>294</v>
       </c>
     </row>
     <row r="67" spans="1:2">
       <c r="A67" s="11" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B67" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="68" spans="1:2">
-      <c r="A68" s="12" t="s">
-        <v>301</v>
+      <c r="A68" s="22" t="s">
+        <v>300</v>
       </c>
       <c r="B68" t="b">
         <v>1</v>
@@ -2572,40 +2591,40 @@
     </row>
     <row r="69" spans="1:2">
       <c r="A69" s="14" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B69" t="str">
         <f ca="1">TEXT(TODAY(), "mm/dd/yyyy")</f>
-        <v>01/03/2024</v>
+        <v>01/04/2024</v>
       </c>
     </row>
     <row r="70" spans="1:2">
       <c r="A70" s="16" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="B70" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
     <row r="71" spans="1:2">
       <c r="A71" s="15" t="s">
+        <v>306</v>
+      </c>
+      <c r="B71" t="s">
         <v>308</v>
-      </c>
-      <c r="B71" t="s">
-        <v>310</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="58">
       <c r="A72" s="15" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
     <row r="73" spans="1:2">
       <c r="A73" s="16" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="B73" s="3">
         <v>15</v>
@@ -2613,223 +2632,223 @@
     </row>
     <row r="74" spans="1:2">
       <c r="A74" s="19" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="B74" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="75" spans="1:2">
       <c r="A75" s="16" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="B75" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="76" spans="1:2">
       <c r="A76" s="16" t="s">
-        <v>316</v>
-      </c>
-      <c r="B76" s="22" t="s">
-        <v>402</v>
+        <v>314</v>
+      </c>
+      <c r="B76" t="s">
+        <v>399</v>
       </c>
     </row>
     <row r="77" spans="1:2">
       <c r="A77" s="19" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B77" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="43.5">
       <c r="A78" s="15" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
     </row>
     <row r="79" spans="1:2">
       <c r="A79" s="16" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="B79" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="80" spans="1:2">
       <c r="A80" s="15" t="s">
-        <v>320</v>
-      </c>
-      <c r="B80" s="22" t="s">
-        <v>402</v>
+        <v>318</v>
+      </c>
+      <c r="B80" t="s">
+        <v>399</v>
       </c>
     </row>
     <row r="81" spans="1:2">
       <c r="A81" s="15" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B81" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="29">
       <c r="A82" s="15" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="83" spans="1:2">
       <c r="A83" s="15" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="B83" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="84" spans="1:2">
       <c r="A84" s="15" t="s">
-        <v>329</v>
-      </c>
-      <c r="B84" s="22" t="s">
-        <v>402</v>
+        <v>327</v>
+      </c>
+      <c r="B84" t="s">
+        <v>399</v>
       </c>
     </row>
     <row r="85" spans="1:2">
       <c r="A85" s="15" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B85" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="86" spans="1:2" ht="58">
       <c r="A86" s="15" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
     </row>
     <row r="87" spans="1:2">
       <c r="A87" s="15" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B87" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="88" spans="1:2">
       <c r="A88" s="15" t="s">
-        <v>333</v>
-      </c>
-      <c r="B88" s="22" t="s">
-        <v>402</v>
+        <v>331</v>
+      </c>
+      <c r="B88" t="s">
+        <v>399</v>
       </c>
     </row>
     <row r="89" spans="1:2">
       <c r="A89" s="15" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="B89" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="29">
       <c r="A90" s="15" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
     </row>
     <row r="91" spans="1:2">
       <c r="A91" s="15" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="B91" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="92" spans="1:2">
       <c r="A92" s="15" t="s">
-        <v>338</v>
-      </c>
-      <c r="B92" s="22" t="s">
-        <v>402</v>
+        <v>336</v>
+      </c>
+      <c r="B92" t="s">
+        <v>399</v>
       </c>
     </row>
     <row r="93" spans="1:2">
       <c r="A93" s="18" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="B93" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="94" spans="1:2">
       <c r="A94" s="17" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="B94" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row r="95" spans="1:2">
       <c r="A95" s="17" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="B95" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="96" spans="1:2">
       <c r="A96" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="B96" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="97" spans="1:2">
       <c r="A97" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B97" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
     </row>
     <row r="98" spans="1:2">
       <c r="A98" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="B98" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
     <row r="99" spans="1:2">
       <c r="A99" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="B99" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="100" spans="1:2">
       <c r="A100" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="B100" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
     </row>
     <row r="101" spans="1:2">
       <c r="A101" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="B101" t="b">
         <v>0</v>
@@ -2837,11 +2856,24 @@
     </row>
     <row r="102" spans="1:2">
       <c r="A102" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2">
+      <c r="A103" t="s">
         <v>401</v>
       </c>
+      <c r="B103">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2">
+      <c r="A104" t="s">
+        <v>404</v>
+      </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="18"/>
+  <phoneticPr fontId="19"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -4005,7 +4037,7 @@
     <row r="987" ht="14.25" customHeight="1"/>
     <row r="988" ht="14.25" customHeight="1"/>
   </sheetData>
-  <phoneticPr fontId="18"/>
+  <phoneticPr fontId="19"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -4031,7 +4063,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>27</v>
@@ -4064,24 +4096,24 @@
     </row>
     <row r="2" spans="1:26">
       <c r="A2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="18"/>
+  <phoneticPr fontId="19"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1D9DC59-3960-42CB-B3EC-EFF452A90D4F}">
-  <dimension ref="A1:Z79"/>
+  <dimension ref="A1:Z80"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -4127,266 +4159,266 @@
     </row>
     <row r="2" spans="1:26">
       <c r="A2" t="s">
+        <v>149</v>
+      </c>
+      <c r="B2" t="s">
         <v>150</v>
-      </c>
-      <c r="B2" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="3" spans="1:26">
       <c r="A3" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="B3" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="4" spans="1:26">
       <c r="A4" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="B4" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="5" spans="1:26">
       <c r="A5" t="s">
+        <v>151</v>
+      </c>
+      <c r="B5" t="s">
         <v>152</v>
-      </c>
-      <c r="B5" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="6" spans="1:26">
       <c r="A6" t="s">
+        <v>153</v>
+      </c>
+      <c r="B6" t="s">
         <v>154</v>
-      </c>
-      <c r="B6" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="7" spans="1:26">
       <c r="A7" t="s">
+        <v>155</v>
+      </c>
+      <c r="B7" t="s">
         <v>156</v>
-      </c>
-      <c r="B7" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="8" spans="1:26">
       <c r="A8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B8" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="9" spans="1:26">
       <c r="A9" t="s">
+        <v>162</v>
+      </c>
+      <c r="B9" t="s">
         <v>163</v>
-      </c>
-      <c r="B9" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="10" spans="1:26">
       <c r="A10" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="B10" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="11" spans="1:26">
       <c r="A11" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="B11" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
     </row>
     <row r="12" spans="1:26">
       <c r="A12" t="s">
+        <v>386</v>
+      </c>
+      <c r="B12" t="s">
         <v>389</v>
-      </c>
-      <c r="B12" t="s">
-        <v>392</v>
       </c>
     </row>
     <row r="13" spans="1:26">
       <c r="A13" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="B13" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="14" spans="1:26">
       <c r="A14" t="s">
-        <v>161</v>
+        <v>403</v>
       </c>
       <c r="B14" t="s">
-        <v>165</v>
+        <v>402</v>
       </c>
     </row>
     <row r="15" spans="1:26">
       <c r="A15" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B15" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="16" spans="1:26">
       <c r="A16" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="B16" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>395</v>
+        <v>167</v>
       </c>
       <c r="B17" t="s">
-        <v>394</v>
+        <v>170</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>169</v>
+        <v>392</v>
       </c>
       <c r="B18" t="s">
-        <v>172</v>
+        <v>391</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B19" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="B20" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>396</v>
+        <v>173</v>
       </c>
       <c r="B21" t="s">
-        <v>397</v>
+        <v>176</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>175</v>
+        <v>393</v>
       </c>
       <c r="B22" t="s">
-        <v>178</v>
+        <v>394</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B23" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>189</v>
+        <v>175</v>
       </c>
       <c r="B24" t="s">
-        <v>195</v>
+        <v>178</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>321</v>
+        <v>188</v>
       </c>
       <c r="B25" t="s">
-        <v>323</v>
+        <v>194</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="B26" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>194</v>
+        <v>320</v>
       </c>
       <c r="B27" t="s">
-        <v>193</v>
+        <v>321</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" t="s">
-        <v>383</v>
+        <v>193</v>
       </c>
       <c r="B28" t="s">
-        <v>384</v>
+        <v>192</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" t="s">
-        <v>346</v>
+        <v>381</v>
       </c>
       <c r="B29" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" t="s">
-        <v>190</v>
+        <v>344</v>
       </c>
       <c r="B30" t="s">
-        <v>196</v>
+        <v>383</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B31" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B32" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="B33" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" t="s">
-        <v>213</v>
+        <v>199</v>
       </c>
       <c r="B34" t="s">
-        <v>211</v>
+        <v>198</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -4399,7 +4431,7 @@
     </row>
     <row r="36" spans="1:2">
       <c r="A36" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="B36" t="s">
         <v>209</v>
@@ -4407,303 +4439,303 @@
     </row>
     <row r="37" spans="1:2">
       <c r="A37" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="B37" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="B38" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B39" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" t="s">
-        <v>379</v>
+        <v>218</v>
       </c>
       <c r="B40" t="s">
-        <v>380</v>
+        <v>217</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41" t="s">
-        <v>220</v>
+        <v>377</v>
       </c>
       <c r="B41" t="s">
-        <v>222</v>
+        <v>378</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" t="s">
+        <v>219</v>
+      </c>
+      <c r="B42" t="s">
         <v>221</v>
-      </c>
-      <c r="B42" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="B43" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="B44" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B45" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46" t="s">
-        <v>325</v>
+        <v>230</v>
       </c>
       <c r="B46" t="s">
-        <v>324</v>
+        <v>231</v>
       </c>
     </row>
     <row r="47" spans="1:2">
       <c r="A47" t="s">
-        <v>201</v>
+        <v>323</v>
       </c>
       <c r="B47" t="s">
-        <v>228</v>
+        <v>322</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B48" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B49" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50" t="s">
-        <v>239</v>
+        <v>202</v>
       </c>
       <c r="B50" t="s">
-        <v>243</v>
+        <v>233</v>
       </c>
     </row>
     <row r="51" spans="1:2">
       <c r="A51" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="B51" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B52" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
     </row>
     <row r="53" spans="1:2">
       <c r="A53" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="B53" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="54" spans="1:2">
       <c r="A54" t="s">
-        <v>240</v>
+        <v>248</v>
       </c>
       <c r="B54" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B55" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B56" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="57" spans="1:2">
       <c r="A57" t="s">
-        <v>255</v>
+        <v>241</v>
       </c>
       <c r="B57" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="58" spans="1:2">
       <c r="A58" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="B58" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
     </row>
     <row r="59" spans="1:2">
       <c r="A59" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="B59" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="60" spans="1:2">
       <c r="A60" t="s">
-        <v>256</v>
+        <v>261</v>
       </c>
       <c r="B60" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
     </row>
     <row r="61" spans="1:2">
       <c r="A61" t="s">
+        <v>255</v>
+      </c>
+      <c r="B61" t="s">
         <v>257</v>
-      </c>
-      <c r="B61" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="62" spans="1:2">
       <c r="A62" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="B62" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
     </row>
     <row r="63" spans="1:2">
       <c r="A63" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="B63" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
     </row>
     <row r="64" spans="1:2">
       <c r="A64" t="s">
+        <v>265</v>
+      </c>
+      <c r="B64" t="s">
         <v>267</v>
-      </c>
-      <c r="B64" t="s">
-        <v>269</v>
       </c>
     </row>
     <row r="65" spans="1:2">
       <c r="A65" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="B65" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="66" spans="1:2">
       <c r="A66" t="s">
-        <v>365</v>
+        <v>271</v>
       </c>
       <c r="B66" t="s">
-        <v>366</v>
+        <v>270</v>
       </c>
     </row>
     <row r="67" spans="1:2">
       <c r="A67" t="s">
-        <v>276</v>
+        <v>363</v>
       </c>
       <c r="B67" t="s">
-        <v>277</v>
+        <v>364</v>
       </c>
     </row>
     <row r="68" spans="1:2">
       <c r="A68" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="B68" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="69" spans="1:2">
       <c r="A69" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B69" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
     </row>
     <row r="70" spans="1:2">
       <c r="A70" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="B70" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
     </row>
     <row r="71" spans="1:2">
       <c r="A71" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="B71" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
     <row r="72" spans="1:2">
       <c r="A72" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="B72" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
     </row>
     <row r="73" spans="1:2">
       <c r="A73" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B73" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="74" spans="1:2">
       <c r="A74" t="s">
-        <v>273</v>
+        <v>288</v>
       </c>
       <c r="B74" t="s">
         <v>286</v>
@@ -4711,15 +4743,15 @@
     </row>
     <row r="75" spans="1:2">
       <c r="A75" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B75" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
     </row>
     <row r="76" spans="1:2">
       <c r="A76" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B76" t="s">
         <v>290</v>
@@ -4727,26 +4759,34 @@
     </row>
     <row r="77" spans="1:2">
       <c r="A77" t="s">
-        <v>340</v>
+        <v>274</v>
       </c>
       <c r="B77" t="s">
-        <v>343</v>
+        <v>289</v>
       </c>
     </row>
     <row r="78" spans="1:2">
       <c r="A78" t="s">
+        <v>338</v>
+      </c>
+      <c r="B78" t="s">
         <v>341</v>
-      </c>
-      <c r="B78" t="s">
-        <v>344</v>
       </c>
     </row>
     <row r="79" spans="1:2">
       <c r="A79" t="s">
+        <v>339</v>
+      </c>
+      <c r="B79" t="s">
         <v>342</v>
       </c>
-      <c r="B79" t="s">
-        <v>345</v>
+    </row>
+    <row r="80" spans="1:2">
+      <c r="A80" t="s">
+        <v>340</v>
+      </c>
+      <c r="B80" t="s">
+        <v>343</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change in screenshot for a business exception.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\55651C\Documents\UiPath\P002_090_PayCycleAfternoon_Dispatcher\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5407F702-C161-42FE-B2CA-08FFE1CB057F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E89C2A1-B5CC-4714-9ADB-26C3DDC90701}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1256,10 +1256,10 @@
     <t>ErrorScreenShotPath</t>
   </si>
   <si>
+    <t>\d+\s-\s\w+\sno success</t>
+  </si>
+  <si>
     <t>https://soklfpub-tst.opc.oracleoutsourcing.com/psp/SOKLFTSTNSS/?cmd=login&amp;languageCd=ENG&amp;</t>
-  </si>
-  <si>
-    <t>\d+\s-\s\w+\sno success</t>
   </si>
 </sst>
 </file>
@@ -1512,7 +1512,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1540,6 +1540,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="20" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="20" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="20" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="24">
     <cellStyle name="Comma 2" xfId="2" xr:uid="{DA952E48-534A-4104-8A72-2BE892964A18}"/>
@@ -1879,8 +1880,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="B93" sqref="B93"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="14.5"/>
@@ -1962,8 +1963,8 @@
       <c r="A5" t="s">
         <v>42</v>
       </c>
-      <c r="B5" t="s">
-        <v>405</v>
+      <c r="B5" s="23" t="s">
+        <v>406</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>41</v>
@@ -2505,7 +2506,7 @@
         <v>205</v>
       </c>
       <c r="B58" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="59" spans="1:2">

</xml_diff>

<commit_message>
changes to config file and assets, also made changes to root folder
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\55651C\Documents\GitHub\P002_090_PayCyleAfternoon_Dispatcher\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B328045-0E69-419A-AA12-EF3774A01A6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9AA92C2-ECEE-44CD-8890-01016A893151}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="398">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="387">
   <si>
     <t>Name</t>
   </si>
@@ -99,11 +99,11 @@
   </si>
   <si>
     <t>Orchestrator queue Name. The value must match with the queue name defined on Orchestrator.</t>
-    <phoneticPr fontId="20"/>
+    <phoneticPr fontId="17"/>
   </si>
   <si>
     <t>Logging field which allows grouping of log data of two or more subprocesses under the same business process name</t>
-    <phoneticPr fontId="20"/>
+    <phoneticPr fontId="17"/>
   </si>
   <si>
     <t>Must be 0 if working with Orchestrator queues. If &gt; 0, the robot will retry the same transaction which failed with a system exception. Must be an integer value.</t>
@@ -163,9 +163,6 @@
     <t xml:space="preserve">The maximum number of consecutive system exceptions was reached. </t>
   </si>
   <si>
-    <t>PeopleSoft URL for lauching the web application.</t>
-  </si>
-  <si>
     <t>PeopleSoft_LoginURL</t>
   </si>
   <si>
@@ -178,39 +175,15 @@
     <t>RecipientEmailAddress</t>
   </si>
   <si>
-    <t>Email ID for recipients for Success Email</t>
-  </si>
-  <si>
     <t>CcRecipientEmailAddress</t>
   </si>
   <si>
-    <t>Email ID for CC recipients for Success Email</t>
-  </si>
-  <si>
-    <t>RecipientEmailAddressBE</t>
-  </si>
-  <si>
-    <t>Email ID for recipients for Business Exception Email</t>
-  </si>
-  <si>
-    <t>CcRecipientEmailAddressBE</t>
-  </si>
-  <si>
-    <t>Email ID for CC recipients for Business Exception Email</t>
-  </si>
-  <si>
     <t>RecipientEmailAddressSE</t>
   </si>
   <si>
-    <t>Email ID for recipients for System Exception Email</t>
-  </si>
-  <si>
     <t>CcRecipientEmailAddressSE</t>
   </si>
   <si>
-    <t>Email ID for CC recipients for System Exception Email</t>
-  </si>
-  <si>
     <t>EmailBody</t>
   </si>
   <si>
@@ -226,21 +199,6 @@
     <t>Success Email Subject</t>
   </si>
   <si>
-    <t>EmailBodyBE</t>
-  </si>
-  <si>
-    <t>Business Exception Email Body</t>
-  </si>
-  <si>
-    <t>EmailSubjectBE</t>
-  </si>
-  <si>
-    <t>Process Business Exception</t>
-  </si>
-  <si>
-    <t>Business Exception Email Subject</t>
-  </si>
-  <si>
     <t>EmailBodySE</t>
   </si>
   <si>
@@ -274,24 +232,6 @@
     <t>mail type is failure</t>
   </si>
   <si>
-    <t>ErrorTypeBE</t>
-  </si>
-  <si>
-    <t>Business</t>
-  </si>
-  <si>
-    <t>Error type is business exception</t>
-  </si>
-  <si>
-    <t>ErrorTypeSE</t>
-  </si>
-  <si>
-    <t>System</t>
-  </si>
-  <si>
-    <t>Error type is system exception</t>
-  </si>
-  <si>
     <t>Summary</t>
   </si>
   <si>
@@ -328,24 +268,6 @@
     <t>Outlook exe name to kill instance</t>
   </si>
   <si>
-    <t>UpdateReportBusinessExceptionType</t>
-  </si>
-  <si>
-    <t>Business Exception</t>
-  </si>
-  <si>
-    <t>Exception type to be updated in exception report , if business.</t>
-  </si>
-  <si>
-    <t>UpdateReportSystemExceptionType</t>
-  </si>
-  <si>
-    <t>System Exception</t>
-  </si>
-  <si>
-    <t>Exception type to be updated in exception report , if system.</t>
-  </si>
-  <si>
     <t>UpdateReportTypeSummary</t>
   </si>
   <si>
@@ -400,12 +322,6 @@
     <t>Number of queue items to be checked before adding, please add is input items are more than 20.</t>
   </si>
   <si>
-    <t>Udbhav.Agarwal.CTR@omes.ok.gov</t>
-  </si>
-  <si>
-    <t>Hello RPA Support Team,&lt;br&gt;&lt;br&gt;This email notification was raised for process P002_090_PayCycleAfternoon. The process execution met a business exception for Pay cycle &lt;PC&gt;  , details for which can be found below:&lt;br&gt;&lt;br&gt;Exception Message: Excp_Message&lt;br&gt;&lt;br&gt;</t>
-  </si>
-  <si>
     <t>Hello RPA Support Team,&lt;br&gt;&lt;br&gt;This email notification was raised for process P002_090_PayCycleAfternoon. The process execution met a System exception, details for which can be found below:&lt;br&gt;&lt;br&gt;Exception Message: Excp_Message&lt;br&gt;&lt;br&gt;</t>
   </si>
   <si>
@@ -538,9 +454,6 @@
     <t>RefreshMonitorUserID</t>
   </si>
   <si>
-    <t>BATCHPROD</t>
-  </si>
-  <si>
     <t>RefreshMonitorDurationType</t>
   </si>
   <si>
@@ -688,18 +601,6 @@
     <t>Workflow To Check Record Status has a Business Exception.</t>
   </si>
   <si>
-    <t>C:\Users\55651C\Documents\UiPath\P002_090_PayCycleAfternoon_Dispatcher\Data.xlsx</t>
-  </si>
-  <si>
-    <t>ExcelFileQueueDataSheetName</t>
-  </si>
-  <si>
-    <t>ExcelFileQueueDataFilePath</t>
-  </si>
-  <si>
-    <t>Queue Data</t>
-  </si>
-  <si>
     <t>AddDataToQueueWorkflowStarted</t>
   </si>
   <si>
@@ -859,15 +760,6 @@
     <t>ReturnButtonCounterSelector</t>
   </si>
   <si>
-    <t>MailFilterStartTime</t>
-  </si>
-  <si>
-    <t>00:00AM</t>
-  </si>
-  <si>
-    <t>MailFilterEndTime</t>
-  </si>
-  <si>
     <t>P002_090_PayCycleAfternoon_PayCycleValues</t>
   </si>
   <si>
@@ -886,18 +778,12 @@
     <t>RetryScopeContinueOnError</t>
   </si>
   <si>
-    <t>QueueReference</t>
-  </si>
-  <si>
     <t>udbhavagarwal's workspace</t>
   </si>
   <si>
     <t>P002_090_PayCycleAfternoon_Dispatcher</t>
   </si>
   <si>
-    <t>11:30PM</t>
-  </si>
-  <si>
     <t>BE_1: There was an error as the Trigger email was not found.</t>
   </si>
   <si>
@@ -955,18 +841,6 @@
     <t>PendingRetryBlockErrorMessage</t>
   </si>
   <si>
-    <t>SE_1Subject</t>
-  </si>
-  <si>
-    <t>SE_1Body</t>
-  </si>
-  <si>
-    <t>SE_1RecipientEmailAddress</t>
-  </si>
-  <si>
-    <t>SE_1CCEmailAddress</t>
-  </si>
-  <si>
     <t>SE_2Subject</t>
   </si>
   <si>
@@ -1063,42 +937,12 @@
     <t>There was an error as the Trigger email was not found.</t>
   </si>
   <si>
-    <t>SE_2: Credentials Error.</t>
-  </si>
-  <si>
-    <t>SE_1: Peoplesoft Unavailable.</t>
-  </si>
-  <si>
     <t>AllValuesPresent</t>
   </si>
   <si>
     <t>All mandatory values are present.</t>
   </si>
   <si>
-    <t>PeoplesoftLoginCredentialsSE_2</t>
-  </si>
-  <si>
-    <t>PeoplesoftLoginPageUnavailableSE_1</t>
-  </si>
-  <si>
-    <t>PeopleSoft_HomepageURL</t>
-  </si>
-  <si>
-    <t>https://soklfpub-tst.opc.oracleoutsourcing.com/psc/SOKLFTSTNSS/EMPLOYEE/ERP/c/NUI_FRAMEWORK.PT_LANDINGPAGE.GBL</t>
-  </si>
-  <si>
-    <t>URL for homepage after login.</t>
-  </si>
-  <si>
-    <t>PeopleSoft_ProcessMonitorURL</t>
-  </si>
-  <si>
-    <t>https://soklfpub-tst.opc.oracleoutsourcing.com/psp/SOKLFTSTNSS/EMPLOYEE/ERP/c/PROCESSMONITOR.PROCESSMONITOR.GBL</t>
-  </si>
-  <si>
-    <t>URL for Process Monitor Page.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Hi Statewide Accounting Team,&lt;br&gt;&lt;br&gt;OKBATCNN status as 'No Success' is halting the afternoon pay cycle. Please complete it manually today; the bot will resume next business day.&lt;br&gt; &lt;br&gt; Thanks,&lt;br&gt;Automation Team                        </t>
   </si>
   <si>
@@ -1120,9 +964,6 @@
     <t>Hi Statewide Accounting Team,&lt;br&gt;&lt;br&gt;Bot hasn't received the correct confirmation email&lt;br&gt;Please send the email within &lt;15mintime_stamp&gt;&lt;br&gt;Subject Line : P0002PayCycleAfternoonTrigger&lt;br&gt;Bot Email Address :  &lt;bot_email_address&gt;&lt;br&gt; &lt;br&gt; Thanks,&lt;br&gt;Automation Team</t>
   </si>
   <si>
-    <t>SenderEmailAddress</t>
-  </si>
-  <si>
     <t>NoDataFoundBE_3</t>
   </si>
   <si>
@@ -1132,9 +973,6 @@
     <t xml:space="preserve">Index for OKBATCNN job </t>
   </si>
   <si>
-    <t>MailFilterDate</t>
-  </si>
-  <si>
     <t>BotEmailAddress</t>
   </si>
   <si>
@@ -1150,9 +988,6 @@
     <t>User ID field was not found in the log in page</t>
   </si>
   <si>
-    <t>C:\Users\55651C\Documents\UiPath\P002_090_PayCycleAfternoon_Dispatcher\Exceptions_Screenshots</t>
-  </si>
-  <si>
     <t xml:space="preserve">The Navigation button was not found in Peoplesoft home page </t>
   </si>
   <si>
@@ -1177,9 +1012,6 @@
     <t>BotPeoplesoftUserID</t>
   </si>
   <si>
-    <t>deepali.chaudhry@ey.com</t>
-  </si>
-  <si>
     <t>LoginRetries</t>
   </si>
   <si>
@@ -1192,9 +1024,6 @@
     <t>ErrorScreenShotPath</t>
   </si>
   <si>
-    <t>https://soklfpub-tst.opc.oracleoutsourcing.com/psp/SOKLFTSTNSS/?cmd=login&amp;languageCd=ENG&amp;</t>
-  </si>
-  <si>
     <t>OKBATCNN -Job ran to Pending Record</t>
   </si>
   <si>
@@ -1214,25 +1043,163 @@
   </si>
   <si>
     <t>SE_3CCEmailAddress</t>
-  </si>
-  <si>
-    <t>PendingRecordRetriesSE_3</t>
-  </si>
-  <si>
-    <t>SE_3: A record was found with Pending status even after max retries.</t>
-  </si>
-  <si>
-    <t>BE_1,BE_2,SE_1,SE_2,BE_3,SE_3</t>
   </si>
   <si>
     <t xml:space="preserve">Hello Team,&lt;br&gt;&lt;br&gt;This email notification was raised for P002_090_PayCycleAfternoon process
  &lt;br&gt;The process executed successfully and Paycycle data was added to the queue. In case of any issues with the automation, please reach out to the RPA Support Team.&lt;br&gt;&lt;br&gt;  Thanks,&lt;br&gt;Automation Team  </t>
   </si>
   <si>
-    <t>\d+\s-\s\w+\sno sufccess</t>
-  </si>
-  <si>
-    <t>00:00:10</t>
+    <t>\d+\s-\s\w+\sno success</t>
+  </si>
+  <si>
+    <t>00:04:00</t>
+  </si>
+  <si>
+    <t>PeopleSoftLoginCredentailsFolderName</t>
+  </si>
+  <si>
+    <t>PeopleSoft_NavigationURL</t>
+  </si>
+  <si>
+    <t>DEV/P002_PayCycleAfternoon</t>
+  </si>
+  <si>
+    <t>P002_090_PayCycleAfternoon_PeopleSoftLoginURL</t>
+  </si>
+  <si>
+    <t>P002_090_PayCycleAfternoon_PeopleSoftNavigationURL</t>
+  </si>
+  <si>
+    <t>P002_090_PayCycleAfternoon_RecipientEmailAddress</t>
+  </si>
+  <si>
+    <t>P002_090_PayCycleAfternoon_CcRecipientEmailAddress</t>
+  </si>
+  <si>
+    <t>P002_090_PayCycleAfternoon_RecipientEmailAddressSE</t>
+  </si>
+  <si>
+    <t>P002_090_PayCycleAfternoon_CcRecipientEmailAddressSE</t>
+  </si>
+  <si>
+    <t>P002_090_PayCycleAfternoon_RefreshMonitorUserID</t>
+  </si>
+  <si>
+    <t>P002_090_PayCycleAfternoon_SenderEmailAddress</t>
+  </si>
+  <si>
+    <t>P002_090_PayCycleAfternoon_BE_1RecipientEmailAddress</t>
+  </si>
+  <si>
+    <t>P002_090_PayCycleAfternoon_BE_1CCEmailAddress</t>
+  </si>
+  <si>
+    <t>P002_090_PayCycleAfternoon_BE_2RecipientEmailAddress</t>
+  </si>
+  <si>
+    <t>P002_090_PayCycleAfternoon_BE_2CCEmailAddress</t>
+  </si>
+  <si>
+    <t>P002_090_PayCycleAfternoon_BE_3RecipientEmailAddress</t>
+  </si>
+  <si>
+    <t>P002_090_PayCycleAfternoon_BE_3CCEmailAddress</t>
+  </si>
+  <si>
+    <t>P002_090_PayCycleAfternoon_SE_2RecipientEmailAddress</t>
+  </si>
+  <si>
+    <t>P002_090_PayCycleAfternoon_SE_2CCEmailAddress</t>
+  </si>
+  <si>
+    <t>P002_090_PayCycleAfternoon_SE_3RecipientEmailAddress</t>
+  </si>
+  <si>
+    <t>P002_090_PayCycleAfternoon_SE_3CCEmailAddress</t>
+  </si>
+  <si>
+    <t>SE_4Subject</t>
+  </si>
+  <si>
+    <t>SE_4Body</t>
+  </si>
+  <si>
+    <t>SE_4RecipientEmailAddress</t>
+  </si>
+  <si>
+    <t>SE_4CCEmailAddress</t>
+  </si>
+  <si>
+    <t>P002_090_PayCycleAfternoon_SE_4RecipientEmailAddress</t>
+  </si>
+  <si>
+    <t>P002_090_PayCycleAfternoon_SE_4CCEmailAddress</t>
+  </si>
+  <si>
+    <t>SE_3: Credentials Error.</t>
+  </si>
+  <si>
+    <t>PeoplesoftLoginCredentialsSE_3</t>
+  </si>
+  <si>
+    <t>SE_2: Peoplesoft Unavailable.</t>
+  </si>
+  <si>
+    <t>PeoplesoftLoginPageUnavailableSE_2</t>
+  </si>
+  <si>
+    <t>PendingRecordRetriesSE_4</t>
+  </si>
+  <si>
+    <t>SE_4: A record was found with Pending status even after max retries.</t>
+  </si>
+  <si>
+    <t>LocalRootFolderPath</t>
+  </si>
+  <si>
+    <t>P002_090_PayCycleAfternoon_LocalRootFolderPath</t>
+  </si>
+  <si>
+    <t>CreateLocalFolderWorkflowStarted</t>
+  </si>
+  <si>
+    <t>Workflow to create local folder has started.</t>
+  </si>
+  <si>
+    <t>CreateLocalFolderWorkflowCompleted</t>
+  </si>
+  <si>
+    <t>CreateLocalFolderWorkflowSE</t>
+  </si>
+  <si>
+    <t>Workflow to create local folder completed successfully.</t>
+  </si>
+  <si>
+    <t>Workflow to create local folder has a System Exception.</t>
+  </si>
+  <si>
+    <t>LocalFolderPresent</t>
+  </si>
+  <si>
+    <t>Local Root Folder Present, Create Exception Screenshot Folder</t>
+  </si>
+  <si>
+    <t>LocalFolderNotPresent</t>
+  </si>
+  <si>
+    <t>Local Root Folder Not Present</t>
+  </si>
+  <si>
+    <t>LocalFolderNotPresentSE</t>
+  </si>
+  <si>
+    <t>BE_1,BE_2,SE_4,SE_2,BE_3,SE_3</t>
+  </si>
+  <si>
+    <t>ProcessFolderName</t>
+  </si>
+  <si>
+    <t>PaycycleAfternoon_Dispatcher</t>
   </si>
 </sst>
 </file>
@@ -1242,32 +1209,11 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="27">
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1463,56 +1409,53 @@
   </borders>
   <cellStyleXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="4" fontId="25" fillId="2" borderId="1" applyNumberFormat="0" applyProtection="0">
+    <xf numFmtId="4" fontId="22" fillId="2" borderId="1" applyNumberFormat="0" applyProtection="0">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="20"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="20" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="20" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="20" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="20"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="20" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="20" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="20" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="20" applyFont="1"/>
-    <xf numFmtId="49" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="20" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="20" applyFont="1"/>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="20" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="20" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="20" applyFont="1"/>
@@ -1859,10 +1802,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z102"/>
+  <dimension ref="A1:Z68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B66" sqref="B66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="14.5"/>
@@ -1909,10 +1852,10 @@
     </row>
     <row r="2" spans="1:26">
       <c r="A2" s="2" t="s">
-        <v>231</v>
+        <v>198</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>278</v>
+        <v>242</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>20</v>
@@ -1923,7 +1866,7 @@
         <v>28</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>283</v>
+        <v>246</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>29</v>
@@ -1934,7 +1877,7 @@
         <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>284</v>
+        <v>247</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>21</v>
@@ -1945,888 +1888,569 @@
         <v>42</v>
       </c>
       <c r="B5" t="s">
-        <v>384</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>41</v>
+        <v>114</v>
+      </c>
+      <c r="C5" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:26">
       <c r="A6" t="s">
-        <v>347</v>
-      </c>
-      <c r="B6" s="24" t="s">
-        <v>348</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="7" spans="1:26">
+        <v>338</v>
+      </c>
+      <c r="B6" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" ht="58">
       <c r="A7" t="s">
-        <v>350</v>
-      </c>
-      <c r="B7" t="s">
-        <v>351</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>352</v>
+        <v>48</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>335</v>
+      </c>
+      <c r="C7" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:26">
       <c r="A8" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="B8" t="s">
-        <v>142</v>
+        <v>51</v>
       </c>
       <c r="C8" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="43.5">
       <c r="A9" t="s">
-        <v>45</v>
-      </c>
-      <c r="B9" t="s">
-        <v>120</v>
+        <v>53</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>94</v>
       </c>
       <c r="C9" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:26">
       <c r="A10" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="B10" t="s">
-        <v>120</v>
+        <v>56</v>
       </c>
       <c r="C10" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:26">
       <c r="A11" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="B11" t="s">
-        <v>120</v>
+        <v>59</v>
       </c>
       <c r="C11" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:26">
       <c r="A12" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="B12" t="s">
-        <v>120</v>
+        <v>62</v>
       </c>
       <c r="C12" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
     </row>
     <row r="13" spans="1:26">
       <c r="A13" t="s">
-        <v>53</v>
+        <v>5</v>
       </c>
       <c r="B13" t="s">
-        <v>120</v>
+        <v>6</v>
       </c>
       <c r="C13" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:26">
-      <c r="A14" t="s">
-        <v>55</v>
+      <c r="A14" s="2" t="s">
+        <v>95</v>
       </c>
       <c r="B14" t="s">
-        <v>120</v>
+        <v>66</v>
       </c>
       <c r="C14" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="15" spans="1:26" ht="58">
-      <c r="A15" t="s">
-        <v>57</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>395</v>
-      </c>
-      <c r="C15" t="s">
-        <v>58</v>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26">
+      <c r="A15" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:26">
-      <c r="A16" t="s">
-        <v>59</v>
-      </c>
-      <c r="B16" t="s">
-        <v>60</v>
-      </c>
-      <c r="C16" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="43.5">
-      <c r="A17" t="s">
-        <v>62</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="C17" t="s">
-        <v>63</v>
+      <c r="A16" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" t="s">
+      <c r="A18" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B18" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="B18" t="s">
-        <v>65</v>
-      </c>
-      <c r="C18" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="43.5">
-      <c r="A19" t="s">
-        <v>67</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="C19" t="s">
-        <v>68</v>
+      <c r="C18" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B19" t="s">
+        <v>79</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" t="s">
-        <v>69</v>
-      </c>
-      <c r="B20" t="s">
-        <v>70</v>
-      </c>
-      <c r="C20" t="s">
-        <v>71</v>
+      <c r="A20" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21" t="s">
-        <v>72</v>
-      </c>
-      <c r="B21" t="s">
-        <v>73</v>
-      </c>
-      <c r="C21" t="s">
-        <v>74</v>
+      <c r="A21" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B21">
+        <v>5000</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" t="s">
-        <v>75</v>
-      </c>
-      <c r="B22" t="s">
-        <v>76</v>
-      </c>
-      <c r="C22" t="s">
-        <v>77</v>
+      <c r="A22" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B22">
+        <v>5</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" t="s">
-        <v>78</v>
-      </c>
-      <c r="B23" t="s">
-        <v>79</v>
-      </c>
-      <c r="C23" t="s">
-        <v>80</v>
+      <c r="A23" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B23">
+        <v>2</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="24" spans="1:3">
-      <c r="A24" t="s">
-        <v>81</v>
-      </c>
-      <c r="B24" t="s">
-        <v>82</v>
-      </c>
-      <c r="C24" t="s">
-        <v>83</v>
+      <c r="A24" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="B24" t="b">
+        <v>1</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="25" spans="1:3">
-      <c r="A25" t="s">
+      <c r="A25" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B25">
+        <v>20</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B26" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="B27" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="B28" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="B29">
         <v>5</v>
       </c>
-      <c r="B25" t="s">
-        <v>370</v>
-      </c>
-      <c r="C25" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26" s="2" t="s">
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="B30" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="18" t="s">
         <v>123</v>
       </c>
-      <c r="B26" t="s">
-        <v>86</v>
-      </c>
-      <c r="C26" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="A27" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
-      <c r="A28" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="B28" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
-      <c r="A29" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3">
-      <c r="A30" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3">
-      <c r="A31" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>101</v>
+      <c r="B31">
+        <v>5</v>
       </c>
     </row>
     <row r="32" spans="1:3">
-      <c r="A32" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="B32" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3">
-      <c r="A33" s="5" t="s">
-        <v>104</v>
+      <c r="A32" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="B32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" s="7" t="s">
+        <v>138</v>
       </c>
       <c r="B33" t="s">
-        <v>105</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3">
-      <c r="A34" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="B34" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3">
-      <c r="A35" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="B35">
-        <v>5000</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3">
-      <c r="A36" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="B36">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="B34" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="B35" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="B36" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="B37" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="B38" s="12" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="B39" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="B40">
         <v>5</v>
       </c>
-      <c r="C36" s="5" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3">
-      <c r="A37" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="B37">
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" s="20" t="s">
+        <v>239</v>
+      </c>
+      <c r="B41" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" s="19" t="s">
+        <v>245</v>
+      </c>
+      <c r="B42" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" s="14" t="s">
+        <v>250</v>
+      </c>
+      <c r="B43" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" s="13" t="s">
+        <v>249</v>
+      </c>
+      <c r="B44" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="58">
+      <c r="A45" s="13" t="s">
+        <v>255</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" s="14" t="s">
+        <v>283</v>
+      </c>
+      <c r="B46" s="3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" s="17" t="s">
+        <v>258</v>
+      </c>
+      <c r="B47" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="43.5">
+      <c r="A48" s="13" t="s">
+        <v>259</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" s="20" t="s">
+        <v>267</v>
+      </c>
+      <c r="B49" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="29">
+      <c r="A50" s="20" t="s">
+        <v>268</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" s="20" t="s">
+        <v>331</v>
+      </c>
+      <c r="B51" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="58">
+      <c r="A52" s="20" t="s">
+        <v>332</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" s="13" t="s">
+        <v>271</v>
+      </c>
+      <c r="B53" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" ht="29">
+      <c r="A54" s="13" t="s">
+        <v>272</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" s="20" t="s">
+        <v>359</v>
+      </c>
+      <c r="B55" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" ht="43.5">
+      <c r="A56" s="20" t="s">
+        <v>360</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57" s="16" t="s">
+        <v>290</v>
+      </c>
+      <c r="B57" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58" s="15" t="s">
+        <v>291</v>
+      </c>
+      <c r="B58" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59" s="15" t="s">
+        <v>292</v>
+      </c>
+      <c r="B59" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60" t="s">
+        <v>289</v>
+      </c>
+      <c r="B60" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
+      <c r="A61" t="s">
+        <v>285</v>
+      </c>
+      <c r="B61" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
+      <c r="A62" t="s">
+        <v>287</v>
+      </c>
+      <c r="B62" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
+      <c r="A63" t="s">
+        <v>320</v>
+      </c>
+      <c r="B63" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2">
+      <c r="A64" s="21" t="s">
+        <v>322</v>
+      </c>
+      <c r="B64" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
+      <c r="A65" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
+      <c r="A66" t="s">
+        <v>324</v>
+      </c>
+      <c r="B66">
         <v>2</v>
       </c>
-      <c r="C37" s="5" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3">
-      <c r="A38" s="21" t="s">
-        <v>116</v>
-      </c>
-      <c r="B38" t="b">
-        <v>1</v>
-      </c>
-      <c r="C38" s="5" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3">
-      <c r="A39" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="B39">
-        <v>20</v>
-      </c>
-      <c r="C39" s="5" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3">
-      <c r="A40" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="B40" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3">
-      <c r="A41" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="B41" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3">
-      <c r="A42" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="B42" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3">
-      <c r="A43" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="B43">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3">
-      <c r="A44" s="6" t="s">
-        <v>132</v>
-      </c>
-      <c r="B44" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3">
-      <c r="A45" s="21" t="s">
-        <v>151</v>
-      </c>
-      <c r="B45">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3">
-      <c r="A46" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="B46">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3">
-      <c r="A47" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="B47" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3">
-      <c r="A48" s="7" t="s">
-        <v>167</v>
-      </c>
-      <c r="B48" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2">
-      <c r="A49" s="7" t="s">
-        <v>169</v>
-      </c>
-      <c r="B49" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2">
-      <c r="A50" s="7" t="s">
-        <v>171</v>
-      </c>
-      <c r="B50" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2">
-      <c r="A51" s="7" t="s">
-        <v>189</v>
-      </c>
-      <c r="B51" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2">
-      <c r="A52" s="8" t="s">
-        <v>190</v>
-      </c>
-      <c r="B52" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2">
-      <c r="A53" s="12" t="s">
-        <v>191</v>
-      </c>
-      <c r="B53" s="13" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2">
-      <c r="A54" s="8" t="s">
-        <v>209</v>
-      </c>
-      <c r="B54" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2">
-      <c r="A55" s="8" t="s">
-        <v>218</v>
-      </c>
-      <c r="B55" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2">
-      <c r="A56" s="8" t="s">
-        <v>217</v>
-      </c>
-      <c r="B56" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2">
-      <c r="A57" s="12" t="s">
-        <v>262</v>
-      </c>
-      <c r="B57">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2">
-      <c r="A58" s="10" t="s">
-        <v>272</v>
-      </c>
-      <c r="B58" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2">
-      <c r="A59" s="20" t="s">
-        <v>364</v>
-      </c>
-      <c r="B59" t="str">
-        <f ca="1">TEXT(TODAY(), "yyyy-MM-dd")</f>
-        <v>2024-01-17</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2">
-      <c r="A60" s="11" t="s">
-        <v>273</v>
-      </c>
-      <c r="B60" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2">
-      <c r="A61" s="11" t="s">
-        <v>275</v>
-      </c>
-      <c r="B61" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2">
-      <c r="A62" s="22" t="s">
-        <v>281</v>
-      </c>
-      <c r="B62" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2">
-      <c r="A63" s="14" t="s">
-        <v>282</v>
-      </c>
-      <c r="B63" t="str">
-        <f ca="1">TEXT(TODAY(), "mm/dd/yyyy")</f>
-        <v>01/17/2024</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2">
-      <c r="A64" s="16" t="s">
-        <v>288</v>
-      </c>
-      <c r="B64" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2">
-      <c r="A65" s="15" t="s">
-        <v>287</v>
-      </c>
-      <c r="B65" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" ht="58">
-      <c r="A66" s="15" t="s">
-        <v>293</v>
-      </c>
-      <c r="B66" s="3" t="s">
-        <v>359</v>
-      </c>
     </row>
     <row r="67" spans="1:2">
-      <c r="A67" s="16" t="s">
-        <v>325</v>
-      </c>
-      <c r="B67" s="3">
-        <v>15</v>
+      <c r="A67" t="s">
+        <v>327</v>
       </c>
     </row>
     <row r="68" spans="1:2">
-      <c r="A68" s="19" t="s">
-        <v>360</v>
+      <c r="A68" t="s">
+        <v>385</v>
       </c>
       <c r="B68" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2">
-      <c r="A69" s="16" t="s">
-        <v>294</v>
-      </c>
-      <c r="B69" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2">
-      <c r="A70" s="16" t="s">
-        <v>295</v>
-      </c>
-      <c r="B70" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2">
-      <c r="A71" s="19" t="s">
-        <v>296</v>
-      </c>
-      <c r="B71" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" ht="43.5">
-      <c r="A72" s="15" t="s">
-        <v>297</v>
-      </c>
-      <c r="B72" s="3" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2">
-      <c r="A73" s="16" t="s">
-        <v>298</v>
-      </c>
-      <c r="B73" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2">
-      <c r="A74" s="15" t="s">
-        <v>299</v>
-      </c>
-      <c r="B74" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2">
-      <c r="A75" s="15" t="s">
-        <v>305</v>
-      </c>
-      <c r="B75" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" ht="29">
-      <c r="A76" s="15" t="s">
-        <v>306</v>
-      </c>
-      <c r="B76" s="3" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2">
-      <c r="A77" s="15" t="s">
-        <v>307</v>
-      </c>
-      <c r="B77" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2">
-      <c r="A78" s="15" t="s">
-        <v>308</v>
-      </c>
-      <c r="B78" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2">
-      <c r="A79" s="15" t="s">
-        <v>309</v>
-      </c>
-      <c r="B79" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" ht="58">
-      <c r="A80" s="15" t="s">
-        <v>310</v>
-      </c>
-      <c r="B80" s="3" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2">
-      <c r="A81" s="15" t="s">
-        <v>311</v>
-      </c>
-      <c r="B81" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2">
-      <c r="A82" s="15" t="s">
-        <v>312</v>
-      </c>
-      <c r="B82" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2">
-      <c r="A83" s="15" t="s">
-        <v>313</v>
-      </c>
-      <c r="B83" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" ht="29">
-      <c r="A84" s="15" t="s">
-        <v>314</v>
-      </c>
-      <c r="B84" s="3" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2">
-      <c r="A85" s="15" t="s">
-        <v>315</v>
-      </c>
-      <c r="B85" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2">
-      <c r="A86" s="15" t="s">
-        <v>316</v>
-      </c>
-      <c r="B86" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2">
-      <c r="A87" s="23" t="s">
-        <v>388</v>
-      </c>
-      <c r="B87" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" ht="43.5">
-      <c r="A88" s="23" t="s">
-        <v>389</v>
-      </c>
-      <c r="B88" s="3" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="89" spans="1:2">
-      <c r="A89" s="23" t="s">
-        <v>390</v>
-      </c>
-      <c r="B89" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2">
-      <c r="A90" s="23" t="s">
-        <v>391</v>
-      </c>
-      <c r="B90" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2">
-      <c r="A91" s="18" t="s">
-        <v>332</v>
-      </c>
-      <c r="B91" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2">
-      <c r="A92" s="17" t="s">
-        <v>333</v>
-      </c>
-      <c r="B92" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2">
-      <c r="A93" s="17" t="s">
-        <v>334</v>
-      </c>
-      <c r="B93" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2">
-      <c r="A94" t="s">
-        <v>331</v>
-      </c>
-      <c r="B94" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2">
-      <c r="A95" t="s">
-        <v>327</v>
-      </c>
-      <c r="B95" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2">
-      <c r="A96" t="s">
-        <v>329</v>
-      </c>
-      <c r="B96" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2">
-      <c r="A97" t="s">
-        <v>365</v>
-      </c>
-      <c r="B97" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2">
-      <c r="A98" t="s">
-        <v>375</v>
-      </c>
-      <c r="B98" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2">
-      <c r="A99" t="s">
-        <v>377</v>
-      </c>
-      <c r="B99" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2">
-      <c r="A100" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2">
-      <c r="A101" t="s">
-        <v>380</v>
-      </c>
-      <c r="B101">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2">
-      <c r="A102" t="s">
-        <v>383</v>
-      </c>
-    </row>
   </sheetData>
-  <phoneticPr fontId="20"/>
+  <phoneticPr fontId="17"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -3990,23 +3614,23 @@
     <row r="987" ht="14.25" customHeight="1"/>
     <row r="988" ht="14.25" customHeight="1"/>
   </sheetData>
-  <phoneticPr fontId="20"/>
+  <phoneticPr fontId="17"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:Z2"/>
+  <dimension ref="A1:Z23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="31.90625" customWidth="1"/>
-    <col min="2" max="2" width="39.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50.1796875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="60.36328125" customWidth="1"/>
     <col min="4" max="26" width="65.453125" customWidth="1"/>
   </cols>
@@ -4016,7 +3640,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>279</v>
+        <v>243</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>27</v>
@@ -4049,24 +3673,258 @@
     </row>
     <row r="2" spans="1:26">
       <c r="A2" t="s">
-        <v>277</v>
+        <v>241</v>
       </c>
       <c r="B2" t="s">
-        <v>276</v>
+        <v>240</v>
+      </c>
+      <c r="C2" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26">
+      <c r="A3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" t="s">
+        <v>341</v>
+      </c>
+      <c r="C3" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26">
+      <c r="A4" t="s">
+        <v>339</v>
+      </c>
+      <c r="B4" t="s">
+        <v>342</v>
+      </c>
+      <c r="C4" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26">
+      <c r="A5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" t="s">
+        <v>343</v>
+      </c>
+      <c r="C5" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26">
+      <c r="A6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" t="s">
+        <v>344</v>
+      </c>
+      <c r="C6" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26">
+      <c r="A7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" t="s">
+        <v>345</v>
+      </c>
+      <c r="C7" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26">
+      <c r="A8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" t="s">
+        <v>346</v>
+      </c>
+      <c r="C8" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26">
+      <c r="A9" t="s">
+        <v>137</v>
+      </c>
+      <c r="B9" t="s">
+        <v>347</v>
+      </c>
+      <c r="C9" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26">
+      <c r="A10" t="s">
+        <v>311</v>
+      </c>
+      <c r="B10" t="s">
+        <v>348</v>
+      </c>
+      <c r="C10" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26">
+      <c r="A11" s="20" t="s">
+        <v>256</v>
+      </c>
+      <c r="B11" t="s">
+        <v>349</v>
+      </c>
+      <c r="C11" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26">
+      <c r="A12" s="20" t="s">
+        <v>257</v>
+      </c>
+      <c r="B12" t="s">
+        <v>350</v>
+      </c>
+      <c r="C12" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26">
+      <c r="A13" s="20" t="s">
+        <v>260</v>
+      </c>
+      <c r="B13" t="s">
+        <v>351</v>
+      </c>
+      <c r="C13" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26">
+      <c r="A14" s="20" t="s">
+        <v>261</v>
+      </c>
+      <c r="B14" t="s">
+        <v>352</v>
+      </c>
+      <c r="C14" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26">
+      <c r="A15" s="20" t="s">
+        <v>273</v>
+      </c>
+      <c r="B15" t="s">
+        <v>353</v>
+      </c>
+      <c r="C15" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26">
+      <c r="A16" s="20" t="s">
+        <v>274</v>
+      </c>
+      <c r="B16" t="s">
+        <v>354</v>
+      </c>
+      <c r="C16" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="20" t="s">
+        <v>269</v>
+      </c>
+      <c r="B17" t="s">
+        <v>355</v>
+      </c>
+      <c r="C17" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="20" t="s">
+        <v>270</v>
+      </c>
+      <c r="B18" t="s">
+        <v>356</v>
+      </c>
+      <c r="C18" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="20" t="s">
+        <v>333</v>
+      </c>
+      <c r="B19" t="s">
+        <v>357</v>
+      </c>
+      <c r="C19" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="20" t="s">
+        <v>334</v>
+      </c>
+      <c r="B20" t="s">
+        <v>358</v>
+      </c>
+      <c r="C20" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="20" t="s">
+        <v>361</v>
+      </c>
+      <c r="B21" t="s">
+        <v>363</v>
+      </c>
+      <c r="C21" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="20" t="s">
+        <v>362</v>
+      </c>
+      <c r="B22" t="s">
+        <v>364</v>
+      </c>
+      <c r="C22" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="20" t="s">
+        <v>371</v>
+      </c>
+      <c r="B23" t="s">
+        <v>372</v>
+      </c>
+      <c r="C23" t="s">
+        <v>340</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="20"/>
+  <phoneticPr fontId="17"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1D9DC59-3960-42CB-B3EC-EFF452A90D4F}">
-  <dimension ref="A1:Z80"/>
+  <dimension ref="A1:Z86"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B69" sqref="B69"/>
+    <sheetView topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="B85" sqref="B85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -4112,634 +3970,682 @@
     </row>
     <row r="2" spans="1:26">
       <c r="A2" t="s">
-        <v>134</v>
+        <v>106</v>
       </c>
       <c r="B2" t="s">
-        <v>135</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:26">
       <c r="A3" t="s">
-        <v>339</v>
+        <v>297</v>
       </c>
       <c r="B3" t="s">
-        <v>340</v>
+        <v>298</v>
       </c>
     </row>
     <row r="4" spans="1:26">
       <c r="A4" t="s">
-        <v>338</v>
+        <v>296</v>
       </c>
       <c r="B4" t="s">
-        <v>286</v>
+        <v>248</v>
       </c>
     </row>
     <row r="5" spans="1:26">
       <c r="A5" t="s">
-        <v>136</v>
+        <v>108</v>
       </c>
       <c r="B5" t="s">
-        <v>137</v>
+        <v>109</v>
       </c>
     </row>
     <row r="6" spans="1:26">
       <c r="A6" t="s">
-        <v>138</v>
+        <v>110</v>
       </c>
       <c r="B6" t="s">
-        <v>139</v>
+        <v>111</v>
       </c>
     </row>
     <row r="7" spans="1:26">
       <c r="A7" t="s">
-        <v>140</v>
+        <v>112</v>
       </c>
       <c r="B7" t="s">
-        <v>141</v>
+        <v>113</v>
       </c>
     </row>
     <row r="8" spans="1:26">
       <c r="A8" t="s">
-        <v>144</v>
+        <v>116</v>
       </c>
       <c r="B8" t="s">
-        <v>143</v>
+        <v>115</v>
       </c>
     </row>
     <row r="9" spans="1:26">
       <c r="A9" t="s">
-        <v>147</v>
+        <v>119</v>
       </c>
       <c r="B9" t="s">
-        <v>148</v>
+        <v>120</v>
       </c>
     </row>
     <row r="10" spans="1:26">
       <c r="A10" t="s">
-        <v>345</v>
+        <v>366</v>
       </c>
       <c r="B10" t="s">
-        <v>341</v>
+        <v>365</v>
       </c>
     </row>
     <row r="11" spans="1:26">
       <c r="A11" t="s">
-        <v>346</v>
+        <v>368</v>
       </c>
       <c r="B11" t="s">
-        <v>342</v>
+        <v>367</v>
       </c>
     </row>
     <row r="12" spans="1:26">
       <c r="A12" t="s">
-        <v>366</v>
+        <v>312</v>
       </c>
       <c r="B12" t="s">
-        <v>369</v>
+        <v>315</v>
       </c>
     </row>
     <row r="13" spans="1:26">
       <c r="A13" t="s">
-        <v>367</v>
+        <v>313</v>
       </c>
       <c r="B13" t="s">
-        <v>368</v>
+        <v>314</v>
       </c>
     </row>
     <row r="14" spans="1:26">
       <c r="A14" t="s">
-        <v>382</v>
+        <v>326</v>
       </c>
       <c r="B14" t="s">
-        <v>381</v>
+        <v>325</v>
       </c>
     </row>
     <row r="15" spans="1:26">
       <c r="A15" t="s">
-        <v>145</v>
+        <v>117</v>
       </c>
       <c r="B15" t="s">
-        <v>149</v>
+        <v>121</v>
       </c>
     </row>
     <row r="16" spans="1:26">
       <c r="A16" t="s">
-        <v>146</v>
+        <v>118</v>
       </c>
       <c r="B16" t="s">
-        <v>150</v>
+        <v>122</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>152</v>
+        <v>124</v>
       </c>
       <c r="B17" t="s">
-        <v>155</v>
+        <v>127</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>372</v>
+        <v>317</v>
       </c>
       <c r="B18" t="s">
-        <v>371</v>
+        <v>316</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>153</v>
+        <v>125</v>
       </c>
       <c r="B19" t="s">
-        <v>156</v>
+        <v>128</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>154</v>
+        <v>126</v>
       </c>
       <c r="B20" t="s">
-        <v>157</v>
+        <v>129</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>158</v>
+        <v>130</v>
       </c>
       <c r="B21" t="s">
-        <v>161</v>
+        <v>133</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>373</v>
+        <v>318</v>
       </c>
       <c r="B22" t="s">
-        <v>374</v>
+        <v>319</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>159</v>
+        <v>131</v>
       </c>
       <c r="B23" t="s">
-        <v>162</v>
+        <v>134</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>160</v>
+        <v>132</v>
       </c>
       <c r="B24" t="s">
-        <v>163</v>
+        <v>135</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>173</v>
+        <v>144</v>
       </c>
       <c r="B25" t="s">
-        <v>179</v>
+        <v>150</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>300</v>
+        <v>262</v>
       </c>
       <c r="B26" t="s">
-        <v>302</v>
+        <v>264</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>301</v>
+        <v>263</v>
       </c>
       <c r="B27" t="s">
-        <v>302</v>
+        <v>264</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" t="s">
-        <v>178</v>
+        <v>149</v>
       </c>
       <c r="B28" t="s">
-        <v>177</v>
+        <v>148</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" t="s">
-        <v>361</v>
+        <v>308</v>
       </c>
       <c r="B29" t="s">
-        <v>362</v>
+        <v>309</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" t="s">
-        <v>324</v>
+        <v>282</v>
       </c>
       <c r="B30" t="s">
-        <v>363</v>
+        <v>310</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" t="s">
-        <v>174</v>
+        <v>145</v>
       </c>
       <c r="B31" t="s">
-        <v>180</v>
+        <v>151</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" t="s">
-        <v>175</v>
+        <v>146</v>
       </c>
       <c r="B32" t="s">
-        <v>181</v>
+        <v>152</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" t="s">
-        <v>176</v>
+        <v>147</v>
       </c>
       <c r="B33" t="s">
-        <v>182</v>
+        <v>153</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" t="s">
-        <v>184</v>
+        <v>155</v>
       </c>
       <c r="B34" t="s">
-        <v>183</v>
+        <v>154</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" t="s">
-        <v>197</v>
+        <v>168</v>
       </c>
       <c r="B35" t="s">
-        <v>195</v>
+        <v>166</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" t="s">
-        <v>196</v>
+        <v>167</v>
       </c>
       <c r="B36" t="s">
-        <v>194</v>
+        <v>165</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" t="s">
-        <v>192</v>
+        <v>163</v>
       </c>
       <c r="B37" t="s">
-        <v>193</v>
+        <v>164</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" t="s">
-        <v>199</v>
+        <v>170</v>
       </c>
       <c r="B38" t="s">
-        <v>198</v>
+        <v>169</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" t="s">
-        <v>201</v>
+        <v>172</v>
       </c>
       <c r="B39" t="s">
-        <v>200</v>
+        <v>171</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" t="s">
-        <v>203</v>
+        <v>174</v>
       </c>
       <c r="B40" t="s">
-        <v>202</v>
+        <v>173</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41" t="s">
-        <v>357</v>
+        <v>305</v>
       </c>
       <c r="B41" t="s">
-        <v>358</v>
+        <v>306</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" t="s">
-        <v>204</v>
+        <v>175</v>
       </c>
       <c r="B42" t="s">
-        <v>206</v>
+        <v>177</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43" t="s">
-        <v>205</v>
+        <v>176</v>
       </c>
       <c r="B43" t="s">
-        <v>207</v>
+        <v>178</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44" t="s">
-        <v>211</v>
+        <v>182</v>
       </c>
       <c r="B44" t="s">
-        <v>210</v>
+        <v>181</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" t="s">
-        <v>213</v>
+        <v>184</v>
       </c>
       <c r="B45" t="s">
-        <v>387</v>
+        <v>330</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46" t="s">
-        <v>392</v>
+        <v>369</v>
       </c>
       <c r="B46" t="s">
-        <v>393</v>
+        <v>370</v>
       </c>
     </row>
     <row r="47" spans="1:2">
       <c r="A47" t="s">
-        <v>304</v>
+        <v>266</v>
       </c>
       <c r="B47" t="s">
-        <v>303</v>
+        <v>265</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48" t="s">
-        <v>185</v>
+        <v>156</v>
       </c>
       <c r="B48" t="s">
-        <v>212</v>
+        <v>183</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49" t="s">
-        <v>186</v>
+        <v>157</v>
       </c>
       <c r="B49" t="s">
-        <v>214</v>
+        <v>185</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50" t="s">
-        <v>187</v>
+        <v>158</v>
       </c>
       <c r="B50" t="s">
-        <v>215</v>
+        <v>186</v>
       </c>
     </row>
     <row r="51" spans="1:2">
       <c r="A51" t="s">
-        <v>220</v>
+        <v>187</v>
       </c>
       <c r="B51" t="s">
-        <v>224</v>
+        <v>191</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52" t="s">
-        <v>226</v>
+        <v>193</v>
       </c>
       <c r="B52" t="s">
-        <v>225</v>
+        <v>192</v>
       </c>
     </row>
     <row r="53" spans="1:2">
       <c r="A53" t="s">
-        <v>227</v>
+        <v>194</v>
       </c>
       <c r="B53" t="s">
-        <v>228</v>
+        <v>195</v>
       </c>
     </row>
     <row r="54" spans="1:2">
       <c r="A54" t="s">
-        <v>230</v>
+        <v>197</v>
       </c>
       <c r="B54" t="s">
-        <v>229</v>
+        <v>196</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" t="s">
-        <v>221</v>
+        <v>188</v>
       </c>
       <c r="B55" t="s">
-        <v>232</v>
+        <v>199</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56" t="s">
-        <v>222</v>
+        <v>189</v>
       </c>
       <c r="B56" t="s">
-        <v>233</v>
+        <v>200</v>
       </c>
     </row>
     <row r="57" spans="1:2">
       <c r="A57" t="s">
-        <v>223</v>
+        <v>190</v>
       </c>
       <c r="B57" t="s">
-        <v>234</v>
+        <v>201</v>
       </c>
     </row>
     <row r="58" spans="1:2">
       <c r="A58" t="s">
-        <v>236</v>
+        <v>203</v>
       </c>
       <c r="B58" t="s">
-        <v>235</v>
+        <v>202</v>
       </c>
     </row>
     <row r="59" spans="1:2">
       <c r="A59" t="s">
-        <v>240</v>
+        <v>207</v>
       </c>
       <c r="B59" t="s">
-        <v>241</v>
+        <v>208</v>
       </c>
     </row>
     <row r="60" spans="1:2">
       <c r="A60" t="s">
-        <v>243</v>
+        <v>210</v>
       </c>
       <c r="B60" t="s">
-        <v>242</v>
+        <v>209</v>
       </c>
     </row>
     <row r="61" spans="1:2">
       <c r="A61" t="s">
-        <v>237</v>
+        <v>204</v>
       </c>
       <c r="B61" t="s">
-        <v>239</v>
+        <v>206</v>
       </c>
     </row>
     <row r="62" spans="1:2">
       <c r="A62" t="s">
-        <v>238</v>
+        <v>205</v>
       </c>
       <c r="B62" t="s">
-        <v>244</v>
+        <v>211</v>
       </c>
     </row>
     <row r="63" spans="1:2">
       <c r="A63" t="s">
-        <v>245</v>
+        <v>212</v>
       </c>
       <c r="B63" t="s">
-        <v>246</v>
+        <v>213</v>
       </c>
     </row>
     <row r="64" spans="1:2">
       <c r="A64" t="s">
-        <v>247</v>
+        <v>214</v>
       </c>
       <c r="B64" t="s">
-        <v>249</v>
+        <v>216</v>
       </c>
     </row>
     <row r="65" spans="1:2">
       <c r="A65" t="s">
-        <v>248</v>
+        <v>215</v>
       </c>
       <c r="B65" t="s">
-        <v>250</v>
+        <v>217</v>
       </c>
     </row>
     <row r="66" spans="1:2">
       <c r="A66" t="s">
-        <v>252</v>
+        <v>219</v>
       </c>
       <c r="B66" t="s">
-        <v>251</v>
+        <v>218</v>
       </c>
     </row>
     <row r="67" spans="1:2">
       <c r="A67" t="s">
-        <v>343</v>
+        <v>299</v>
       </c>
       <c r="B67" t="s">
-        <v>344</v>
+        <v>300</v>
       </c>
     </row>
     <row r="68" spans="1:2">
       <c r="A68" t="s">
-        <v>256</v>
+        <v>223</v>
       </c>
       <c r="B68" t="s">
-        <v>257</v>
+        <v>224</v>
       </c>
     </row>
     <row r="69" spans="1:2">
       <c r="A69" t="s">
-        <v>258</v>
+        <v>225</v>
       </c>
       <c r="B69" t="s">
-        <v>257</v>
+        <v>224</v>
       </c>
     </row>
     <row r="70" spans="1:2">
       <c r="A70" t="s">
-        <v>259</v>
+        <v>226</v>
       </c>
       <c r="B70" t="s">
-        <v>260</v>
+        <v>227</v>
       </c>
     </row>
     <row r="71" spans="1:2">
       <c r="A71" t="s">
-        <v>261</v>
+        <v>228</v>
       </c>
       <c r="B71" t="s">
-        <v>263</v>
+        <v>230</v>
       </c>
     </row>
     <row r="72" spans="1:2">
       <c r="A72" t="s">
-        <v>264</v>
+        <v>231</v>
       </c>
       <c r="B72" t="s">
-        <v>265</v>
+        <v>232</v>
       </c>
     </row>
     <row r="73" spans="1:2">
       <c r="A73" t="s">
-        <v>268</v>
+        <v>235</v>
       </c>
       <c r="B73" t="s">
-        <v>267</v>
+        <v>234</v>
       </c>
     </row>
     <row r="74" spans="1:2">
       <c r="A74" t="s">
-        <v>269</v>
+        <v>236</v>
       </c>
       <c r="B74" t="s">
-        <v>267</v>
+        <v>234</v>
       </c>
     </row>
     <row r="75" spans="1:2">
       <c r="A75" t="s">
-        <v>253</v>
+        <v>220</v>
       </c>
       <c r="B75" t="s">
-        <v>266</v>
+        <v>233</v>
       </c>
     </row>
     <row r="76" spans="1:2">
       <c r="A76" t="s">
-        <v>254</v>
+        <v>221</v>
       </c>
       <c r="B76" t="s">
-        <v>271</v>
+        <v>238</v>
       </c>
     </row>
     <row r="77" spans="1:2">
       <c r="A77" t="s">
-        <v>255</v>
+        <v>222</v>
       </c>
       <c r="B77" t="s">
-        <v>270</v>
+        <v>237</v>
       </c>
     </row>
     <row r="78" spans="1:2">
       <c r="A78" t="s">
-        <v>318</v>
+        <v>276</v>
       </c>
       <c r="B78" t="s">
-        <v>321</v>
+        <v>279</v>
       </c>
     </row>
     <row r="79" spans="1:2">
       <c r="A79" t="s">
-        <v>319</v>
+        <v>277</v>
       </c>
       <c r="B79" t="s">
-        <v>322</v>
+        <v>280</v>
       </c>
     </row>
     <row r="80" spans="1:2">
       <c r="A80" t="s">
-        <v>320</v>
+        <v>278</v>
       </c>
       <c r="B80" t="s">
-        <v>323</v>
+        <v>281</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2">
+      <c r="A81" t="s">
+        <v>373</v>
+      </c>
+      <c r="B81" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2">
+      <c r="A82" t="s">
+        <v>379</v>
+      </c>
+      <c r="B82" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2">
+      <c r="A83" t="s">
+        <v>381</v>
+      </c>
+      <c r="B83" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2">
+      <c r="A84" t="s">
+        <v>383</v>
+      </c>
+      <c r="B84" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2">
+      <c r="A85" t="s">
+        <v>375</v>
+      </c>
+      <c r="B85" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2">
+      <c r="A86" t="s">
+        <v>376</v>
+      </c>
+      <c r="B86" t="s">
+        <v>378</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Made changes to kill process workflow and also added combined Graph API library
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\55651C\Documents\GitHub\P002_090_PayCyleAfternoon_Dispatcher\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9AA92C2-ECEE-44CD-8890-01016A893151}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D31D28D7-D62D-4D87-A1CD-2D3144259812}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="387">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="377">
   <si>
     <t>Name</t>
   </si>
@@ -99,11 +99,11 @@
   </si>
   <si>
     <t>Orchestrator queue Name. The value must match with the queue name defined on Orchestrator.</t>
-    <phoneticPr fontId="17"/>
+    <phoneticPr fontId="19"/>
   </si>
   <si>
     <t>Logging field which allows grouping of log data of two or more subprocesses under the same business process name</t>
-    <phoneticPr fontId="17"/>
+    <phoneticPr fontId="19"/>
   </si>
   <si>
     <t>Must be 0 if working with Orchestrator queues. If &gt; 0, the robot will retry the same transaction which failed with a system exception. Must be an integer value.</t>
@@ -232,66 +232,27 @@
     <t>mail type is failure</t>
   </si>
   <si>
-    <t>Summary</t>
-  </si>
-  <si>
-    <t>Folder for placing exception screenshots.</t>
-  </si>
-  <si>
     <t>SUCCESS</t>
   </si>
   <si>
     <t>Kill_excel</t>
   </si>
   <si>
-    <t>Excel.exe</t>
-  </si>
-  <si>
     <t>Excel exe name to kill excel instance</t>
   </si>
   <si>
     <t>Kill_msedge</t>
   </si>
   <si>
-    <t>msedge.exe</t>
-  </si>
-  <si>
     <t>Edge exe name to kill instance</t>
   </si>
   <si>
     <t>Kill_Outlook</t>
   </si>
   <si>
-    <t>outlook.exe</t>
-  </si>
-  <si>
     <t>Outlook exe name to kill instance</t>
   </si>
   <si>
-    <t>UpdateReportTypeSummary</t>
-  </si>
-  <si>
-    <t>If summary report needs to be updated.</t>
-  </si>
-  <si>
-    <t>UpdateReportExceptionStatus</t>
-  </si>
-  <si>
-    <t>Failed</t>
-  </si>
-  <si>
-    <t>If a transaction is failed.</t>
-  </si>
-  <si>
-    <t>UpdateReportSuccessStatus</t>
-  </si>
-  <si>
-    <t>Completed</t>
-  </si>
-  <si>
-    <t>If a transaction completes successfully.</t>
-  </si>
-  <si>
     <t>CloseApplicationTimeout</t>
   </si>
   <si>
@@ -778,9 +739,6 @@
     <t>RetryScopeContinueOnError</t>
   </si>
   <si>
-    <t>udbhavagarwal's workspace</t>
-  </si>
-  <si>
     <t>P002_090_PayCycleAfternoon_Dispatcher</t>
   </si>
   <si>
@@ -1001,9 +959,6 @@
   </si>
   <si>
     <t>OrchestratorGraphAPIAssetsFolder</t>
-  </si>
-  <si>
-    <t>DEV</t>
   </si>
   <si>
     <t>MarkEmailAsRead</t>
@@ -1061,145 +1016,160 @@
     <t>PeopleSoft_NavigationURL</t>
   </si>
   <si>
+    <t>P002_090_PayCycleAfternoon_PeopleSoftLoginURL</t>
+  </si>
+  <si>
+    <t>P002_090_PayCycleAfternoon_PeopleSoftNavigationURL</t>
+  </si>
+  <si>
+    <t>P002_090_PayCycleAfternoon_RecipientEmailAddress</t>
+  </si>
+  <si>
+    <t>P002_090_PayCycleAfternoon_CcRecipientEmailAddress</t>
+  </si>
+  <si>
+    <t>P002_090_PayCycleAfternoon_RecipientEmailAddressSE</t>
+  </si>
+  <si>
+    <t>P002_090_PayCycleAfternoon_CcRecipientEmailAddressSE</t>
+  </si>
+  <si>
+    <t>P002_090_PayCycleAfternoon_RefreshMonitorUserID</t>
+  </si>
+  <si>
+    <t>P002_090_PayCycleAfternoon_SenderEmailAddress</t>
+  </si>
+  <si>
+    <t>P002_090_PayCycleAfternoon_BE_1RecipientEmailAddress</t>
+  </si>
+  <si>
+    <t>P002_090_PayCycleAfternoon_BE_1CCEmailAddress</t>
+  </si>
+  <si>
+    <t>P002_090_PayCycleAfternoon_BE_2RecipientEmailAddress</t>
+  </si>
+  <si>
+    <t>P002_090_PayCycleAfternoon_BE_2CCEmailAddress</t>
+  </si>
+  <si>
+    <t>P002_090_PayCycleAfternoon_BE_3RecipientEmailAddress</t>
+  </si>
+  <si>
+    <t>P002_090_PayCycleAfternoon_BE_3CCEmailAddress</t>
+  </si>
+  <si>
+    <t>P002_090_PayCycleAfternoon_SE_2RecipientEmailAddress</t>
+  </si>
+  <si>
+    <t>P002_090_PayCycleAfternoon_SE_2CCEmailAddress</t>
+  </si>
+  <si>
+    <t>P002_090_PayCycleAfternoon_SE_3RecipientEmailAddress</t>
+  </si>
+  <si>
+    <t>P002_090_PayCycleAfternoon_SE_3CCEmailAddress</t>
+  </si>
+  <si>
+    <t>SE_4Subject</t>
+  </si>
+  <si>
+    <t>SE_4Body</t>
+  </si>
+  <si>
+    <t>SE_4RecipientEmailAddress</t>
+  </si>
+  <si>
+    <t>SE_4CCEmailAddress</t>
+  </si>
+  <si>
+    <t>P002_090_PayCycleAfternoon_SE_4RecipientEmailAddress</t>
+  </si>
+  <si>
+    <t>P002_090_PayCycleAfternoon_SE_4CCEmailAddress</t>
+  </si>
+  <si>
+    <t>SE_3: Credentials Error.</t>
+  </si>
+  <si>
+    <t>PeoplesoftLoginCredentialsSE_3</t>
+  </si>
+  <si>
+    <t>SE_2: Peoplesoft Unavailable.</t>
+  </si>
+  <si>
+    <t>PeoplesoftLoginPageUnavailableSE_2</t>
+  </si>
+  <si>
+    <t>PendingRecordRetriesSE_4</t>
+  </si>
+  <si>
+    <t>SE_4: A record was found with Pending status even after max retries.</t>
+  </si>
+  <si>
+    <t>LocalRootFolderPath</t>
+  </si>
+  <si>
+    <t>P002_090_PayCycleAfternoon_LocalRootFolderPath</t>
+  </si>
+  <si>
+    <t>CreateLocalFolderWorkflowStarted</t>
+  </si>
+  <si>
+    <t>Workflow to create local folder has started.</t>
+  </si>
+  <si>
+    <t>CreateLocalFolderWorkflowCompleted</t>
+  </si>
+  <si>
+    <t>CreateLocalFolderWorkflowSE</t>
+  </si>
+  <si>
+    <t>Workflow to create local folder completed successfully.</t>
+  </si>
+  <si>
+    <t>Workflow to create local folder has a System Exception.</t>
+  </si>
+  <si>
+    <t>LocalFolderPresent</t>
+  </si>
+  <si>
+    <t>Local Root Folder Present, Create Exception Screenshot Folder</t>
+  </si>
+  <si>
+    <t>LocalFolderNotPresent</t>
+  </si>
+  <si>
+    <t>Local Root Folder Not Present</t>
+  </si>
+  <si>
+    <t>LocalFolderNotPresentSE</t>
+  </si>
+  <si>
+    <t>BE_1,BE_2,SE_4,SE_2,BE_3,SE_3</t>
+  </si>
+  <si>
+    <t>ProcessFolderName</t>
+  </si>
+  <si>
+    <t>PaycycleAfternoon_Dispatcher</t>
+  </si>
+  <si>
+    <t>PROD/P002_090_PayCycleAfternoon</t>
+  </si>
+  <si>
+    <t>DEV</t>
+  </si>
+  <si>
     <t>DEV/P002_PayCycleAfternoon</t>
   </si>
   <si>
-    <t>P002_090_PayCycleAfternoon_PeopleSoftLoginURL</t>
-  </si>
-  <si>
-    <t>P002_090_PayCycleAfternoon_PeopleSoftNavigationURL</t>
-  </si>
-  <si>
-    <t>P002_090_PayCycleAfternoon_RecipientEmailAddress</t>
-  </si>
-  <si>
-    <t>P002_090_PayCycleAfternoon_CcRecipientEmailAddress</t>
-  </si>
-  <si>
-    <t>P002_090_PayCycleAfternoon_RecipientEmailAddressSE</t>
-  </si>
-  <si>
-    <t>P002_090_PayCycleAfternoon_CcRecipientEmailAddressSE</t>
-  </si>
-  <si>
-    <t>P002_090_PayCycleAfternoon_RefreshMonitorUserID</t>
-  </si>
-  <si>
-    <t>P002_090_PayCycleAfternoon_SenderEmailAddress</t>
-  </si>
-  <si>
-    <t>P002_090_PayCycleAfternoon_BE_1RecipientEmailAddress</t>
-  </si>
-  <si>
-    <t>P002_090_PayCycleAfternoon_BE_1CCEmailAddress</t>
-  </si>
-  <si>
-    <t>P002_090_PayCycleAfternoon_BE_2RecipientEmailAddress</t>
-  </si>
-  <si>
-    <t>P002_090_PayCycleAfternoon_BE_2CCEmailAddress</t>
-  </si>
-  <si>
-    <t>P002_090_PayCycleAfternoon_BE_3RecipientEmailAddress</t>
-  </si>
-  <si>
-    <t>P002_090_PayCycleAfternoon_BE_3CCEmailAddress</t>
-  </si>
-  <si>
-    <t>P002_090_PayCycleAfternoon_SE_2RecipientEmailAddress</t>
-  </si>
-  <si>
-    <t>P002_090_PayCycleAfternoon_SE_2CCEmailAddress</t>
-  </si>
-  <si>
-    <t>P002_090_PayCycleAfternoon_SE_3RecipientEmailAddress</t>
-  </si>
-  <si>
-    <t>P002_090_PayCycleAfternoon_SE_3CCEmailAddress</t>
-  </si>
-  <si>
-    <t>SE_4Subject</t>
-  </si>
-  <si>
-    <t>SE_4Body</t>
-  </si>
-  <si>
-    <t>SE_4RecipientEmailAddress</t>
-  </si>
-  <si>
-    <t>SE_4CCEmailAddress</t>
-  </si>
-  <si>
-    <t>P002_090_PayCycleAfternoon_SE_4RecipientEmailAddress</t>
-  </si>
-  <si>
-    <t>P002_090_PayCycleAfternoon_SE_4CCEmailAddress</t>
-  </si>
-  <si>
-    <t>SE_3: Credentials Error.</t>
-  </si>
-  <si>
-    <t>PeoplesoftLoginCredentialsSE_3</t>
-  </si>
-  <si>
-    <t>SE_2: Peoplesoft Unavailable.</t>
-  </si>
-  <si>
-    <t>PeoplesoftLoginPageUnavailableSE_2</t>
-  </si>
-  <si>
-    <t>PendingRecordRetriesSE_4</t>
-  </si>
-  <si>
-    <t>SE_4: A record was found with Pending status even after max retries.</t>
-  </si>
-  <si>
-    <t>LocalRootFolderPath</t>
-  </si>
-  <si>
-    <t>P002_090_PayCycleAfternoon_LocalRootFolderPath</t>
-  </si>
-  <si>
-    <t>CreateLocalFolderWorkflowStarted</t>
-  </si>
-  <si>
-    <t>Workflow to create local folder has started.</t>
-  </si>
-  <si>
-    <t>CreateLocalFolderWorkflowCompleted</t>
-  </si>
-  <si>
-    <t>CreateLocalFolderWorkflowSE</t>
-  </si>
-  <si>
-    <t>Workflow to create local folder completed successfully.</t>
-  </si>
-  <si>
-    <t>Workflow to create local folder has a System Exception.</t>
-  </si>
-  <si>
-    <t>LocalFolderPresent</t>
-  </si>
-  <si>
-    <t>Local Root Folder Present, Create Exception Screenshot Folder</t>
-  </si>
-  <si>
-    <t>LocalFolderNotPresent</t>
-  </si>
-  <si>
-    <t>Local Root Folder Not Present</t>
-  </si>
-  <si>
-    <t>LocalFolderNotPresentSE</t>
-  </si>
-  <si>
-    <t>BE_1,BE_2,SE_4,SE_2,BE_3,SE_3</t>
-  </si>
-  <si>
-    <t>ProcessFolderName</t>
-  </si>
-  <si>
-    <t>PaycycleAfternoon_Dispatcher</t>
+    <t>excel</t>
+  </si>
+  <si>
+    <t>msedge</t>
+  </si>
+  <si>
+    <t>outlook</t>
   </si>
 </sst>
 </file>
@@ -1209,11 +1179,25 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="26">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1409,53 +1393,55 @@
   </borders>
   <cellStyleXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="4" fontId="22" fillId="2" borderId="1" applyNumberFormat="0" applyProtection="0">
+    <xf numFmtId="4" fontId="24" fillId="2" borderId="1" applyNumberFormat="0" applyProtection="0">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="20"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="20"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="20" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="20" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="20" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="20" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="20" applyFont="1"/>
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="20" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="20" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="20" applyFont="1"/>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="20" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="20" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="20" applyFont="1"/>
@@ -1464,7 +1450,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="20" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="20" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="20" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="24">
     <cellStyle name="Comma 2" xfId="2" xr:uid="{DA952E48-534A-4104-8A72-2BE892964A18}"/>
@@ -1802,10 +1787,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z68"/>
+  <dimension ref="A1:Z64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B66" sqref="B66"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="14.5"/>
@@ -1852,10 +1837,10 @@
     </row>
     <row r="2" spans="1:26">
       <c r="A2" s="2" t="s">
-        <v>198</v>
+        <v>185</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>242</v>
+        <v>229</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>20</v>
@@ -1866,7 +1851,7 @@
         <v>28</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>246</v>
+        <v>373</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>29</v>
@@ -1877,7 +1862,7 @@
         <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>247</v>
+        <v>233</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>21</v>
@@ -1888,7 +1873,7 @@
         <v>42</v>
       </c>
       <c r="B5" t="s">
-        <v>114</v>
+        <v>101</v>
       </c>
       <c r="C5" t="s">
         <v>43</v>
@@ -1896,10 +1881,10 @@
     </row>
     <row r="6" spans="1:26">
       <c r="A6" t="s">
-        <v>338</v>
+        <v>323</v>
       </c>
       <c r="B6" t="s">
-        <v>340</v>
+        <v>373</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="58">
@@ -1907,7 +1892,7 @@
         <v>48</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>335</v>
+        <v>320</v>
       </c>
       <c r="C7" t="s">
         <v>49</v>
@@ -1929,7 +1914,7 @@
         <v>53</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
       <c r="C9" t="s">
         <v>54</v>
@@ -1969,488 +1954,447 @@
       </c>
     </row>
     <row r="13" spans="1:26">
-      <c r="A13" t="s">
-        <v>5</v>
+      <c r="A13" s="2" t="s">
+        <v>82</v>
       </c>
       <c r="B13" t="s">
-        <v>6</v>
+        <v>64</v>
       </c>
       <c r="C13" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26">
+      <c r="A14" s="9" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="14" spans="1:26">
-      <c r="A14" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="B14" t="s">
+      <c r="B14" s="21" t="s">
+        <v>374</v>
+      </c>
+      <c r="C14" s="5" t="s">
         <v>66</v>
-      </c>
-      <c r="C14" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="15" spans="1:26">
       <c r="A15" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="21" t="s">
+        <v>375</v>
+      </c>
+      <c r="C15" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="C15" s="5" t="s">
+    </row>
+    <row r="16" spans="1:26">
+      <c r="A16" s="5" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="16" spans="1:26">
-      <c r="A16" s="9" t="s">
+      <c r="B16" s="22" t="s">
+        <v>376</v>
+      </c>
+      <c r="C16" s="5" t="s">
         <v>70</v>
-      </c>
-      <c r="B16" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>74</v>
+        <v>71</v>
+      </c>
+      <c r="B17">
+        <v>5000</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>64</v>
+        <v>73</v>
+      </c>
+      <c r="B18">
+        <v>5</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="B20" t="b">
+        <v>1</v>
+      </c>
+      <c r="C20" s="5" t="s">
         <v>78</v>
-      </c>
-      <c r="B19" t="s">
-        <v>79</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="5" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="B21">
-        <v>5000</v>
+        <v>20</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="B22">
-        <v>5</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>87</v>
+        <v>84</v>
+      </c>
+      <c r="B22" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B23" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="B23">
-        <v>2</v>
-      </c>
-      <c r="C23" s="5" t="s">
+      <c r="B24" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
-      <c r="A24" s="18" t="s">
+    <row r="25" spans="1:3">
+      <c r="A25" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="B24" t="b">
+      <c r="B25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="B26" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="B27">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="B28">
         <v>1</v>
       </c>
-      <c r="C24" s="5" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="B25">
-        <v>20</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="B26" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="A27" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="B27" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
-      <c r="A28" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="B28" t="s">
-        <v>102</v>
-      </c>
     </row>
     <row r="29" spans="1:3">
-      <c r="A29" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="B29">
-        <v>5</v>
+      <c r="A29" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="B29" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="30" spans="1:3">
-      <c r="A30" s="6" t="s">
-        <v>104</v>
+      <c r="A30" s="7" t="s">
+        <v>127</v>
       </c>
       <c r="B30" t="s">
-        <v>105</v>
+        <v>128</v>
       </c>
     </row>
     <row r="31" spans="1:3">
-      <c r="A31" s="18" t="s">
-        <v>123</v>
-      </c>
-      <c r="B31">
-        <v>5</v>
+      <c r="A31" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="B31" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="B32">
+        <v>147</v>
+      </c>
+      <c r="B32" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="B33" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="B34" s="11" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="B35" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" s="10" t="s">
+        <v>216</v>
+      </c>
+      <c r="B36">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" s="19" t="s">
+        <v>226</v>
+      </c>
+      <c r="B37" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" s="18" t="s">
+        <v>232</v>
+      </c>
+      <c r="B38" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
-      <c r="A33" s="7" t="s">
-        <v>138</v>
-      </c>
-      <c r="B33" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2">
-      <c r="A34" s="7" t="s">
-        <v>140</v>
-      </c>
-      <c r="B34" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2">
-      <c r="A35" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="B35" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2">
-      <c r="A36" s="7" t="s">
-        <v>160</v>
-      </c>
-      <c r="B36" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2">
-      <c r="A37" s="8" t="s">
-        <v>161</v>
-      </c>
-      <c r="B37" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2">
-      <c r="A38" s="11" t="s">
-        <v>162</v>
-      </c>
-      <c r="B38" s="12" t="s">
-        <v>337</v>
-      </c>
-    </row>
     <row r="39" spans="1:2">
-      <c r="A39" s="8" t="s">
-        <v>180</v>
+      <c r="A39" s="13" t="s">
+        <v>236</v>
       </c>
       <c r="B39" t="s">
-        <v>179</v>
+        <v>368</v>
       </c>
     </row>
     <row r="40" spans="1:2">
-      <c r="A40" s="11" t="s">
-        <v>229</v>
-      </c>
-      <c r="B40">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2">
-      <c r="A41" s="20" t="s">
+      <c r="A40" s="12" t="s">
+        <v>235</v>
+      </c>
+      <c r="B40" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="58">
+      <c r="A41" s="12" t="s">
+        <v>241</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" s="13" t="s">
+        <v>269</v>
+      </c>
+      <c r="B42" s="3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" s="16" t="s">
+        <v>244</v>
+      </c>
+      <c r="B43" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="43.5">
+      <c r="A44" s="12" t="s">
+        <v>245</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" s="19" t="s">
+        <v>253</v>
+      </c>
+      <c r="B45" t="s">
         <v>239</v>
       </c>
-      <c r="B41" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2">
-      <c r="A42" s="19" t="s">
-        <v>245</v>
-      </c>
-      <c r="B42" t="b">
+    </row>
+    <row r="46" spans="1:2" ht="29">
+      <c r="A46" s="19" t="s">
+        <v>254</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" s="19" t="s">
+        <v>316</v>
+      </c>
+      <c r="B47" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="58">
+      <c r="A48" s="19" t="s">
+        <v>317</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="B49" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="29">
+      <c r="A50" s="12" t="s">
+        <v>258</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" s="19" t="s">
+        <v>343</v>
+      </c>
+      <c r="B51" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="43.5">
+      <c r="A52" s="19" t="s">
+        <v>344</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53" s="15" t="s">
+        <v>276</v>
+      </c>
+      <c r="B53" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54" s="14" t="s">
+        <v>277</v>
+      </c>
+      <c r="B54" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55" s="14" t="s">
+        <v>278</v>
+      </c>
+      <c r="B55" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56" t="s">
+        <v>275</v>
+      </c>
+      <c r="B56" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57" t="s">
+        <v>271</v>
+      </c>
+      <c r="B57" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58" t="s">
+        <v>273</v>
+      </c>
+      <c r="B58" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="A59" t="s">
+        <v>306</v>
+      </c>
+      <c r="B59" t="s">
+        <v>372</v>
+      </c>
+      <c r="C59" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="A60" t="s">
+        <v>307</v>
+      </c>
+      <c r="B60" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:2">
-      <c r="A43" s="14" t="s">
-        <v>250</v>
-      </c>
-      <c r="B43" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2">
-      <c r="A44" s="13" t="s">
-        <v>249</v>
-      </c>
-      <c r="B44" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" ht="58">
-      <c r="A45" s="13" t="s">
-        <v>255</v>
-      </c>
-      <c r="B45" s="3" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2">
-      <c r="A46" s="14" t="s">
-        <v>283</v>
-      </c>
-      <c r="B46" s="3">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2">
-      <c r="A47" s="17" t="s">
-        <v>258</v>
-      </c>
-      <c r="B47" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" ht="43.5">
-      <c r="A48" s="13" t="s">
-        <v>259</v>
-      </c>
-      <c r="B48" s="3" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2">
-      <c r="A49" s="20" t="s">
-        <v>267</v>
-      </c>
-      <c r="B49" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" ht="29">
-      <c r="A50" s="20" t="s">
-        <v>268</v>
-      </c>
-      <c r="B50" s="3" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2">
-      <c r="A51" s="20" t="s">
-        <v>331</v>
-      </c>
-      <c r="B51" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" ht="58">
-      <c r="A52" s="20" t="s">
-        <v>332</v>
-      </c>
-      <c r="B52" s="3" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2">
-      <c r="A53" s="13" t="s">
-        <v>271</v>
-      </c>
-      <c r="B53" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" ht="29">
-      <c r="A54" s="13" t="s">
-        <v>272</v>
-      </c>
-      <c r="B54" s="3" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2">
-      <c r="A55" s="20" t="s">
-        <v>359</v>
-      </c>
-      <c r="B55" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" ht="43.5">
-      <c r="A56" s="20" t="s">
-        <v>360</v>
-      </c>
-      <c r="B56" s="3" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2">
-      <c r="A57" s="16" t="s">
-        <v>290</v>
-      </c>
-      <c r="B57" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2">
-      <c r="A58" s="15" t="s">
-        <v>291</v>
-      </c>
-      <c r="B58" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2">
-      <c r="A59" s="15" t="s">
-        <v>292</v>
-      </c>
-      <c r="B59" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2">
-      <c r="A60" t="s">
-        <v>289</v>
-      </c>
-      <c r="B60" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2">
+    <row r="61" spans="1:3">
       <c r="A61" t="s">
-        <v>285</v>
-      </c>
-      <c r="B61" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
       <c r="A62" t="s">
-        <v>287</v>
-      </c>
-      <c r="B62" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2">
+        <v>309</v>
+      </c>
+      <c r="B62">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
       <c r="A63" t="s">
-        <v>320</v>
-      </c>
-      <c r="B63" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2">
-      <c r="A64" s="21" t="s">
-        <v>322</v>
-      </c>
-      <c r="B64" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2">
-      <c r="A65" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2">
-      <c r="A66" t="s">
-        <v>324</v>
-      </c>
-      <c r="B66">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2">
-      <c r="A67" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2">
-      <c r="A68" t="s">
-        <v>385</v>
-      </c>
-      <c r="B68" t="s">
-        <v>386</v>
+        <v>312</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
+      <c r="A64" t="s">
+        <v>369</v>
+      </c>
+      <c r="B64" t="s">
+        <v>370</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="17"/>
+  <phoneticPr fontId="19"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -3614,7 +3558,7 @@
     <row r="987" ht="14.25" customHeight="1"/>
     <row r="988" ht="14.25" customHeight="1"/>
   </sheetData>
-  <phoneticPr fontId="17"/>
+  <phoneticPr fontId="19"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3623,8 +3567,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="14.5"/>
@@ -3640,7 +3584,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>243</v>
+        <v>230</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>27</v>
@@ -3673,13 +3617,16 @@
     </row>
     <row r="2" spans="1:26">
       <c r="A2" t="s">
-        <v>241</v>
+        <v>228</v>
       </c>
       <c r="B2" t="s">
-        <v>240</v>
+        <v>227</v>
       </c>
       <c r="C2" t="s">
-        <v>340</v>
+        <v>373</v>
+      </c>
+      <c r="D2" t="s">
+        <v>371</v>
       </c>
     </row>
     <row r="3" spans="1:26">
@@ -3687,21 +3634,21 @@
         <v>41</v>
       </c>
       <c r="B3" t="s">
-        <v>341</v>
+        <v>325</v>
       </c>
       <c r="C3" t="s">
-        <v>340</v>
+        <v>373</v>
       </c>
     </row>
     <row r="4" spans="1:26">
       <c r="A4" t="s">
-        <v>339</v>
+        <v>324</v>
       </c>
       <c r="B4" t="s">
-        <v>342</v>
+        <v>326</v>
       </c>
       <c r="C4" t="s">
-        <v>340</v>
+        <v>373</v>
       </c>
     </row>
     <row r="5" spans="1:26">
@@ -3709,10 +3656,10 @@
         <v>44</v>
       </c>
       <c r="B5" t="s">
-        <v>343</v>
+        <v>327</v>
       </c>
       <c r="C5" t="s">
-        <v>340</v>
+        <v>373</v>
       </c>
     </row>
     <row r="6" spans="1:26">
@@ -3720,10 +3667,10 @@
         <v>45</v>
       </c>
       <c r="B6" t="s">
-        <v>344</v>
+        <v>328</v>
       </c>
       <c r="C6" t="s">
-        <v>340</v>
+        <v>373</v>
       </c>
     </row>
     <row r="7" spans="1:26">
@@ -3731,10 +3678,10 @@
         <v>46</v>
       </c>
       <c r="B7" t="s">
-        <v>345</v>
+        <v>329</v>
       </c>
       <c r="C7" t="s">
-        <v>340</v>
+        <v>373</v>
       </c>
     </row>
     <row r="8" spans="1:26">
@@ -3742,179 +3689,179 @@
         <v>47</v>
       </c>
       <c r="B8" t="s">
-        <v>346</v>
+        <v>330</v>
       </c>
       <c r="C8" t="s">
-        <v>340</v>
+        <v>373</v>
       </c>
     </row>
     <row r="9" spans="1:26">
       <c r="A9" t="s">
-        <v>137</v>
+        <v>124</v>
       </c>
       <c r="B9" t="s">
-        <v>347</v>
+        <v>331</v>
       </c>
       <c r="C9" t="s">
-        <v>340</v>
+        <v>373</v>
       </c>
     </row>
     <row r="10" spans="1:26">
       <c r="A10" t="s">
-        <v>311</v>
+        <v>297</v>
       </c>
       <c r="B10" t="s">
+        <v>332</v>
+      </c>
+      <c r="C10" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26">
+      <c r="A11" s="19" t="s">
+        <v>242</v>
+      </c>
+      <c r="B11" t="s">
+        <v>333</v>
+      </c>
+      <c r="C11" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26">
+      <c r="A12" s="19" t="s">
+        <v>243</v>
+      </c>
+      <c r="B12" t="s">
+        <v>334</v>
+      </c>
+      <c r="C12" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26">
+      <c r="A13" s="19" t="s">
+        <v>246</v>
+      </c>
+      <c r="B13" t="s">
+        <v>335</v>
+      </c>
+      <c r="C13" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26">
+      <c r="A14" s="19" t="s">
+        <v>247</v>
+      </c>
+      <c r="B14" t="s">
+        <v>336</v>
+      </c>
+      <c r="C14" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26">
+      <c r="A15" s="19" t="s">
+        <v>259</v>
+      </c>
+      <c r="B15" t="s">
+        <v>337</v>
+      </c>
+      <c r="C15" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26">
+      <c r="A16" s="19" t="s">
+        <v>260</v>
+      </c>
+      <c r="B16" t="s">
+        <v>338</v>
+      </c>
+      <c r="C16" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="19" t="s">
+        <v>255</v>
+      </c>
+      <c r="B17" t="s">
+        <v>339</v>
+      </c>
+      <c r="C17" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="19" t="s">
+        <v>256</v>
+      </c>
+      <c r="B18" t="s">
+        <v>340</v>
+      </c>
+      <c r="C18" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="19" t="s">
+        <v>318</v>
+      </c>
+      <c r="B19" t="s">
+        <v>341</v>
+      </c>
+      <c r="C19" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="19" t="s">
+        <v>319</v>
+      </c>
+      <c r="B20" t="s">
+        <v>342</v>
+      </c>
+      <c r="C20" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="19" t="s">
+        <v>345</v>
+      </c>
+      <c r="B21" t="s">
+        <v>347</v>
+      </c>
+      <c r="C21" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="19" t="s">
+        <v>346</v>
+      </c>
+      <c r="B22" t="s">
         <v>348</v>
       </c>
-      <c r="C10" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="11" spans="1:26">
-      <c r="A11" s="20" t="s">
-        <v>256</v>
-      </c>
-      <c r="B11" t="s">
-        <v>349</v>
-      </c>
-      <c r="C11" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="12" spans="1:26">
-      <c r="A12" s="20" t="s">
-        <v>257</v>
-      </c>
-      <c r="B12" t="s">
-        <v>350</v>
-      </c>
-      <c r="C12" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26">
-      <c r="A13" s="20" t="s">
-        <v>260</v>
-      </c>
-      <c r="B13" t="s">
-        <v>351</v>
-      </c>
-      <c r="C13" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="14" spans="1:26">
-      <c r="A14" s="20" t="s">
-        <v>261</v>
-      </c>
-      <c r="B14" t="s">
-        <v>352</v>
-      </c>
-      <c r="C14" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="15" spans="1:26">
-      <c r="A15" s="20" t="s">
-        <v>273</v>
-      </c>
-      <c r="B15" t="s">
-        <v>353</v>
-      </c>
-      <c r="C15" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="16" spans="1:26">
-      <c r="A16" s="20" t="s">
-        <v>274</v>
-      </c>
-      <c r="B16" t="s">
-        <v>354</v>
-      </c>
-      <c r="C16" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="20" t="s">
-        <v>269</v>
-      </c>
-      <c r="B17" t="s">
+      <c r="C22" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="19" t="s">
         <v>355</v>
       </c>
-      <c r="C17" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="20" t="s">
-        <v>270</v>
-      </c>
-      <c r="B18" t="s">
+      <c r="B23" t="s">
         <v>356</v>
       </c>
-      <c r="C18" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="20" t="s">
-        <v>333</v>
-      </c>
-      <c r="B19" t="s">
-        <v>357</v>
-      </c>
-      <c r="C19" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="20" t="s">
-        <v>334</v>
-      </c>
-      <c r="B20" t="s">
-        <v>358</v>
-      </c>
-      <c r="C20" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="20" t="s">
-        <v>361</v>
-      </c>
-      <c r="B21" t="s">
-        <v>363</v>
-      </c>
-      <c r="C21" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" s="20" t="s">
-        <v>362</v>
-      </c>
-      <c r="B22" t="s">
-        <v>364</v>
-      </c>
-      <c r="C22" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" s="20" t="s">
-        <v>371</v>
-      </c>
-      <c r="B23" t="s">
-        <v>372</v>
-      </c>
       <c r="C23" t="s">
-        <v>340</v>
+        <v>373</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="17"/>
+  <phoneticPr fontId="19"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3923,7 +3870,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1D9DC59-3960-42CB-B3EC-EFF452A90D4F}">
   <dimension ref="A1:Z86"/>
   <sheetViews>
-    <sheetView topLeftCell="A76" workbookViewId="0">
+    <sheetView topLeftCell="A73" workbookViewId="0">
       <selection activeCell="B85" sqref="B85"/>
     </sheetView>
   </sheetViews>
@@ -3970,682 +3917,682 @@
     </row>
     <row r="2" spans="1:26">
       <c r="A2" t="s">
-        <v>106</v>
+        <v>93</v>
       </c>
       <c r="B2" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:26">
       <c r="A3" t="s">
-        <v>297</v>
+        <v>283</v>
       </c>
       <c r="B3" t="s">
-        <v>298</v>
+        <v>284</v>
       </c>
     </row>
     <row r="4" spans="1:26">
       <c r="A4" t="s">
-        <v>296</v>
+        <v>282</v>
       </c>
       <c r="B4" t="s">
-        <v>248</v>
+        <v>234</v>
       </c>
     </row>
     <row r="5" spans="1:26">
       <c r="A5" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
       <c r="B5" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
     </row>
     <row r="6" spans="1:26">
       <c r="A6" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="B6" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
     </row>
     <row r="7" spans="1:26">
       <c r="A7" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
       <c r="B7" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:26">
       <c r="A8" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
       <c r="B8" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
     </row>
     <row r="9" spans="1:26">
       <c r="A9" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="B9" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
     </row>
     <row r="10" spans="1:26">
       <c r="A10" t="s">
-        <v>366</v>
+        <v>350</v>
       </c>
       <c r="B10" t="s">
-        <v>365</v>
+        <v>349</v>
       </c>
     </row>
     <row r="11" spans="1:26">
       <c r="A11" t="s">
-        <v>368</v>
+        <v>352</v>
       </c>
       <c r="B11" t="s">
-        <v>367</v>
+        <v>351</v>
       </c>
     </row>
     <row r="12" spans="1:26">
       <c r="A12" t="s">
-        <v>312</v>
+        <v>298</v>
       </c>
       <c r="B12" t="s">
-        <v>315</v>
+        <v>301</v>
       </c>
     </row>
     <row r="13" spans="1:26">
       <c r="A13" t="s">
-        <v>313</v>
+        <v>299</v>
       </c>
       <c r="B13" t="s">
-        <v>314</v>
+        <v>300</v>
       </c>
     </row>
     <row r="14" spans="1:26">
       <c r="A14" t="s">
-        <v>326</v>
+        <v>311</v>
       </c>
       <c r="B14" t="s">
-        <v>325</v>
+        <v>310</v>
       </c>
     </row>
     <row r="15" spans="1:26">
       <c r="A15" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
       <c r="B15" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
     </row>
     <row r="16" spans="1:26">
       <c r="A16" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
       <c r="B16" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
       <c r="B17" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>317</v>
+        <v>303</v>
       </c>
       <c r="B18" t="s">
-        <v>316</v>
+        <v>302</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
       <c r="B19" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="B20" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="B21" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>318</v>
+        <v>304</v>
       </c>
       <c r="B22" t="s">
-        <v>319</v>
+        <v>305</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="B23" t="s">
-        <v>134</v>
+        <v>121</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>132</v>
+        <v>119</v>
       </c>
       <c r="B24" t="s">
-        <v>135</v>
+        <v>122</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>144</v>
+        <v>131</v>
       </c>
       <c r="B25" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>262</v>
+        <v>248</v>
       </c>
       <c r="B26" t="s">
-        <v>264</v>
+        <v>250</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>263</v>
+        <v>249</v>
       </c>
       <c r="B27" t="s">
-        <v>264</v>
+        <v>250</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" t="s">
-        <v>149</v>
+        <v>136</v>
       </c>
       <c r="B28" t="s">
-        <v>148</v>
+        <v>135</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" t="s">
-        <v>308</v>
+        <v>294</v>
       </c>
       <c r="B29" t="s">
-        <v>309</v>
+        <v>295</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" t="s">
-        <v>282</v>
+        <v>268</v>
       </c>
       <c r="B30" t="s">
-        <v>310</v>
+        <v>296</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" t="s">
-        <v>145</v>
+        <v>132</v>
       </c>
       <c r="B31" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" t="s">
-        <v>146</v>
+        <v>133</v>
       </c>
       <c r="B32" t="s">
-        <v>152</v>
+        <v>139</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" t="s">
-        <v>147</v>
+        <v>134</v>
       </c>
       <c r="B33" t="s">
-        <v>153</v>
+        <v>140</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="B34" t="s">
-        <v>154</v>
+        <v>141</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" t="s">
-        <v>168</v>
+        <v>155</v>
       </c>
       <c r="B35" t="s">
-        <v>166</v>
+        <v>153</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" t="s">
-        <v>167</v>
+        <v>154</v>
       </c>
       <c r="B36" t="s">
-        <v>165</v>
+        <v>152</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" t="s">
-        <v>163</v>
+        <v>150</v>
       </c>
       <c r="B37" t="s">
-        <v>164</v>
+        <v>151</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
       <c r="B38" t="s">
-        <v>169</v>
+        <v>156</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" t="s">
-        <v>172</v>
+        <v>159</v>
       </c>
       <c r="B39" t="s">
-        <v>171</v>
+        <v>158</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" t="s">
-        <v>174</v>
+        <v>161</v>
       </c>
       <c r="B40" t="s">
-        <v>173</v>
+        <v>160</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41" t="s">
-        <v>305</v>
+        <v>291</v>
       </c>
       <c r="B41" t="s">
-        <v>306</v>
+        <v>292</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" t="s">
-        <v>175</v>
+        <v>162</v>
       </c>
       <c r="B42" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43" t="s">
-        <v>176</v>
+        <v>163</v>
       </c>
       <c r="B43" t="s">
-        <v>178</v>
+        <v>165</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44" t="s">
-        <v>182</v>
+        <v>169</v>
       </c>
       <c r="B44" t="s">
-        <v>181</v>
+        <v>168</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" t="s">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="B45" t="s">
-        <v>330</v>
+        <v>315</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46" t="s">
-        <v>369</v>
+        <v>353</v>
       </c>
       <c r="B46" t="s">
-        <v>370</v>
+        <v>354</v>
       </c>
     </row>
     <row r="47" spans="1:2">
       <c r="A47" t="s">
-        <v>266</v>
+        <v>252</v>
       </c>
       <c r="B47" t="s">
-        <v>265</v>
+        <v>251</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
       <c r="B48" t="s">
-        <v>183</v>
+        <v>170</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49" t="s">
-        <v>157</v>
+        <v>144</v>
       </c>
       <c r="B49" t="s">
-        <v>185</v>
+        <v>172</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
       <c r="B50" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="51" spans="1:2">
       <c r="A51" t="s">
-        <v>187</v>
+        <v>174</v>
       </c>
       <c r="B51" t="s">
-        <v>191</v>
+        <v>178</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52" t="s">
-        <v>193</v>
+        <v>180</v>
       </c>
       <c r="B52" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
     </row>
     <row r="53" spans="1:2">
       <c r="A53" t="s">
-        <v>194</v>
+        <v>181</v>
       </c>
       <c r="B53" t="s">
-        <v>195</v>
+        <v>182</v>
       </c>
     </row>
     <row r="54" spans="1:2">
       <c r="A54" t="s">
-        <v>197</v>
+        <v>184</v>
       </c>
       <c r="B54" t="s">
-        <v>196</v>
+        <v>183</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" t="s">
-        <v>188</v>
+        <v>175</v>
       </c>
       <c r="B55" t="s">
-        <v>199</v>
+        <v>186</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56" t="s">
-        <v>189</v>
+        <v>176</v>
       </c>
       <c r="B56" t="s">
-        <v>200</v>
+        <v>187</v>
       </c>
     </row>
     <row r="57" spans="1:2">
       <c r="A57" t="s">
-        <v>190</v>
+        <v>177</v>
       </c>
       <c r="B57" t="s">
-        <v>201</v>
+        <v>188</v>
       </c>
     </row>
     <row r="58" spans="1:2">
       <c r="A58" t="s">
-        <v>203</v>
+        <v>190</v>
       </c>
       <c r="B58" t="s">
-        <v>202</v>
+        <v>189</v>
       </c>
     </row>
     <row r="59" spans="1:2">
       <c r="A59" t="s">
-        <v>207</v>
+        <v>194</v>
       </c>
       <c r="B59" t="s">
-        <v>208</v>
+        <v>195</v>
       </c>
     </row>
     <row r="60" spans="1:2">
       <c r="A60" t="s">
-        <v>210</v>
+        <v>197</v>
       </c>
       <c r="B60" t="s">
-        <v>209</v>
+        <v>196</v>
       </c>
     </row>
     <row r="61" spans="1:2">
       <c r="A61" t="s">
-        <v>204</v>
+        <v>191</v>
       </c>
       <c r="B61" t="s">
-        <v>206</v>
+        <v>193</v>
       </c>
     </row>
     <row r="62" spans="1:2">
       <c r="A62" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="B62" t="s">
-        <v>211</v>
+        <v>198</v>
       </c>
     </row>
     <row r="63" spans="1:2">
       <c r="A63" t="s">
-        <v>212</v>
+        <v>199</v>
       </c>
       <c r="B63" t="s">
-        <v>213</v>
+        <v>200</v>
       </c>
     </row>
     <row r="64" spans="1:2">
       <c r="A64" t="s">
-        <v>214</v>
+        <v>201</v>
       </c>
       <c r="B64" t="s">
-        <v>216</v>
+        <v>203</v>
       </c>
     </row>
     <row r="65" spans="1:2">
       <c r="A65" t="s">
-        <v>215</v>
+        <v>202</v>
       </c>
       <c r="B65" t="s">
-        <v>217</v>
+        <v>204</v>
       </c>
     </row>
     <row r="66" spans="1:2">
       <c r="A66" t="s">
-        <v>219</v>
+        <v>206</v>
       </c>
       <c r="B66" t="s">
-        <v>218</v>
+        <v>205</v>
       </c>
     </row>
     <row r="67" spans="1:2">
       <c r="A67" t="s">
-        <v>299</v>
+        <v>285</v>
       </c>
       <c r="B67" t="s">
-        <v>300</v>
+        <v>286</v>
       </c>
     </row>
     <row r="68" spans="1:2">
       <c r="A68" t="s">
-        <v>223</v>
+        <v>210</v>
       </c>
       <c r="B68" t="s">
-        <v>224</v>
+        <v>211</v>
       </c>
     </row>
     <row r="69" spans="1:2">
       <c r="A69" t="s">
-        <v>225</v>
+        <v>212</v>
       </c>
       <c r="B69" t="s">
-        <v>224</v>
+        <v>211</v>
       </c>
     </row>
     <row r="70" spans="1:2">
       <c r="A70" t="s">
-        <v>226</v>
+        <v>213</v>
       </c>
       <c r="B70" t="s">
-        <v>227</v>
+        <v>214</v>
       </c>
     </row>
     <row r="71" spans="1:2">
       <c r="A71" t="s">
-        <v>228</v>
+        <v>215</v>
       </c>
       <c r="B71" t="s">
-        <v>230</v>
+        <v>217</v>
       </c>
     </row>
     <row r="72" spans="1:2">
       <c r="A72" t="s">
-        <v>231</v>
+        <v>218</v>
       </c>
       <c r="B72" t="s">
-        <v>232</v>
+        <v>219</v>
       </c>
     </row>
     <row r="73" spans="1:2">
       <c r="A73" t="s">
-        <v>235</v>
+        <v>222</v>
       </c>
       <c r="B73" t="s">
-        <v>234</v>
+        <v>221</v>
       </c>
     </row>
     <row r="74" spans="1:2">
       <c r="A74" t="s">
-        <v>236</v>
+        <v>223</v>
       </c>
       <c r="B74" t="s">
-        <v>234</v>
+        <v>221</v>
       </c>
     </row>
     <row r="75" spans="1:2">
       <c r="A75" t="s">
+        <v>207</v>
+      </c>
+      <c r="B75" t="s">
         <v>220</v>
-      </c>
-      <c r="B75" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="76" spans="1:2">
       <c r="A76" t="s">
-        <v>221</v>
+        <v>208</v>
       </c>
       <c r="B76" t="s">
-        <v>238</v>
+        <v>225</v>
       </c>
     </row>
     <row r="77" spans="1:2">
       <c r="A77" t="s">
-        <v>222</v>
+        <v>209</v>
       </c>
       <c r="B77" t="s">
-        <v>237</v>
+        <v>224</v>
       </c>
     </row>
     <row r="78" spans="1:2">
       <c r="A78" t="s">
-        <v>276</v>
+        <v>262</v>
       </c>
       <c r="B78" t="s">
-        <v>279</v>
+        <v>265</v>
       </c>
     </row>
     <row r="79" spans="1:2">
       <c r="A79" t="s">
-        <v>277</v>
+        <v>263</v>
       </c>
       <c r="B79" t="s">
-        <v>280</v>
+        <v>266</v>
       </c>
     </row>
     <row r="80" spans="1:2">
       <c r="A80" t="s">
-        <v>278</v>
+        <v>264</v>
       </c>
       <c r="B80" t="s">
-        <v>281</v>
+        <v>267</v>
       </c>
     </row>
     <row r="81" spans="1:2">
       <c r="A81" t="s">
-        <v>373</v>
+        <v>357</v>
       </c>
       <c r="B81" t="s">
-        <v>374</v>
+        <v>358</v>
       </c>
     </row>
     <row r="82" spans="1:2">
       <c r="A82" t="s">
-        <v>379</v>
+        <v>363</v>
       </c>
       <c r="B82" t="s">
-        <v>380</v>
+        <v>364</v>
       </c>
     </row>
     <row r="83" spans="1:2">
       <c r="A83" t="s">
-        <v>381</v>
+        <v>365</v>
       </c>
       <c r="B83" t="s">
-        <v>382</v>
+        <v>366</v>
       </c>
     </row>
     <row r="84" spans="1:2">
       <c r="A84" t="s">
-        <v>383</v>
+        <v>367</v>
       </c>
       <c r="B84" t="s">
-        <v>382</v>
+        <v>366</v>
       </c>
     </row>
     <row r="85" spans="1:2">
       <c r="A85" t="s">
-        <v>375</v>
+        <v>359</v>
       </c>
       <c r="B85" t="s">
-        <v>377</v>
+        <v>361</v>
       </c>
     </row>
     <row r="86" spans="1:2">
       <c r="A86" t="s">
-        <v>376</v>
+        <v>360</v>
       </c>
       <c r="B86" t="s">
-        <v>378</v>
+        <v>362</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Pointing config assets to PROD folder
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\55651C\Documents\GitHub\P002_090_PayCyleAfternoon_Dispatcher\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D31D28D7-D62D-4D87-A1CD-2D3144259812}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62580FCE-B728-4B57-B0BB-963B2340A31F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1160,9 +1160,6 @@
     <t>DEV</t>
   </si>
   <si>
-    <t>DEV/P002_PayCycleAfternoon</t>
-  </si>
-  <si>
     <t>excel</t>
   </si>
   <si>
@@ -1170,6 +1167,9 @@
   </si>
   <si>
     <t>outlook</t>
+  </si>
+  <si>
+    <t>PROD</t>
   </si>
 </sst>
 </file>
@@ -1789,8 +1789,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="B59" sqref="B59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="14.5"/>
@@ -1851,7 +1851,7 @@
         <v>28</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>29</v>
@@ -1884,7 +1884,7 @@
         <v>323</v>
       </c>
       <c r="B6" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="58">
@@ -1969,7 +1969,7 @@
         <v>65</v>
       </c>
       <c r="B14" s="21" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>66</v>
@@ -1980,7 +1980,7 @@
         <v>67</v>
       </c>
       <c r="B15" s="21" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>68</v>
@@ -1991,7 +1991,7 @@
         <v>69</v>
       </c>
       <c r="B16" s="22" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>70</v>
@@ -2352,8 +2352,8 @@
       <c r="A59" t="s">
         <v>306</v>
       </c>
-      <c r="B59" t="s">
-        <v>372</v>
+      <c r="B59" s="2" t="s">
+        <v>376</v>
       </c>
       <c r="C59" t="s">
         <v>372</v>
@@ -3567,8 +3567,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z23"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView topLeftCell="C12" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="14.5"/>
@@ -3623,7 +3623,7 @@
         <v>227</v>
       </c>
       <c r="C2" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="D2" t="s">
         <v>371</v>
@@ -3637,7 +3637,7 @@
         <v>325</v>
       </c>
       <c r="C3" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
     </row>
     <row r="4" spans="1:26">
@@ -3648,7 +3648,7 @@
         <v>326</v>
       </c>
       <c r="C4" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
     </row>
     <row r="5" spans="1:26">
@@ -3659,7 +3659,7 @@
         <v>327</v>
       </c>
       <c r="C5" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
     </row>
     <row r="6" spans="1:26">
@@ -3670,7 +3670,7 @@
         <v>328</v>
       </c>
       <c r="C6" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
     </row>
     <row r="7" spans="1:26">
@@ -3681,7 +3681,7 @@
         <v>329</v>
       </c>
       <c r="C7" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
     </row>
     <row r="8" spans="1:26">
@@ -3692,7 +3692,7 @@
         <v>330</v>
       </c>
       <c r="C8" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
     </row>
     <row r="9" spans="1:26">
@@ -3703,7 +3703,7 @@
         <v>331</v>
       </c>
       <c r="C9" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
     </row>
     <row r="10" spans="1:26">
@@ -3714,7 +3714,7 @@
         <v>332</v>
       </c>
       <c r="C10" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
     </row>
     <row r="11" spans="1:26">
@@ -3725,7 +3725,7 @@
         <v>333</v>
       </c>
       <c r="C11" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
     </row>
     <row r="12" spans="1:26">
@@ -3736,7 +3736,7 @@
         <v>334</v>
       </c>
       <c r="C12" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
     </row>
     <row r="13" spans="1:26">
@@ -3747,7 +3747,7 @@
         <v>335</v>
       </c>
       <c r="C13" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
     </row>
     <row r="14" spans="1:26">
@@ -3758,7 +3758,7 @@
         <v>336</v>
       </c>
       <c r="C14" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
     </row>
     <row r="15" spans="1:26">
@@ -3769,7 +3769,7 @@
         <v>337</v>
       </c>
       <c r="C15" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
     </row>
     <row r="16" spans="1:26">
@@ -3780,7 +3780,7 @@
         <v>338</v>
       </c>
       <c r="C16" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -3791,7 +3791,7 @@
         <v>339</v>
       </c>
       <c r="C17" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -3802,7 +3802,7 @@
         <v>340</v>
       </c>
       <c r="C18" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -3813,7 +3813,7 @@
         <v>341</v>
       </c>
       <c r="C19" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -3824,7 +3824,7 @@
         <v>342</v>
       </c>
       <c r="C20" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -3835,7 +3835,7 @@
         <v>347</v>
       </c>
       <c r="C21" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -3846,7 +3846,7 @@
         <v>348</v>
       </c>
       <c r="C22" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -3857,7 +3857,7 @@
         <v>356</v>
       </c>
       <c r="C23" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
made changes to table data extraction
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\55651C\Documents\GitHub\P002_090_PayCyleAfternoon_Dispatcher\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62580FCE-B728-4B57-B0BB-963B2340A31F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13589407-6BFF-40C3-8428-40E8963820D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="377">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="382">
   <si>
     <t>Name</t>
   </si>
@@ -99,11 +99,11 @@
   </si>
   <si>
     <t>Orchestrator queue Name. The value must match with the queue name defined on Orchestrator.</t>
-    <phoneticPr fontId="19"/>
+    <phoneticPr fontId="20"/>
   </si>
   <si>
     <t>Logging field which allows grouping of log data of two or more subprocesses under the same business process name</t>
-    <phoneticPr fontId="19"/>
+    <phoneticPr fontId="20"/>
   </si>
   <si>
     <t>Must be 0 if working with Orchestrator queues. If &gt; 0, the robot will retry the same transaction which failed with a system exception. Must be an integer value.</t>
@@ -1167,6 +1167,21 @@
   </si>
   <si>
     <t>outlook</t>
+  </si>
+  <si>
+    <t>TableRecordsNotExtracted</t>
+  </si>
+  <si>
+    <t>TableRecordsNotExtractedSE</t>
+  </si>
+  <si>
+    <t>TableIRecordsExtracted</t>
+  </si>
+  <si>
+    <t>Records from the table were extracted for OKBATCNN.</t>
+  </si>
+  <si>
+    <t>Records from the table could not be extracted for OKBATCNN.</t>
   </si>
   <si>
     <t>PROD</t>
@@ -1179,11 +1194,18 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="26">
+  <fonts count="27">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1391,54 +1413,65 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="24">
+  <cellStyleXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="4" fontId="24" fillId="2" borderId="1" applyNumberFormat="0" applyProtection="0">
+    <xf numFmtId="4" fontId="25" fillId="2" borderId="1" applyNumberFormat="0" applyProtection="0">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="20"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="20"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="20" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="20" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="20" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="20" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="20" applyFont="1"/>
+    <xf numFmtId="49" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="20" applyFont="1"/>
-    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="20" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="20" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="20" applyFont="1"/>
@@ -1451,11 +1484,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="20" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="20" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="24">
+  <cellStyles count="34">
     <cellStyle name="Comma 2" xfId="2" xr:uid="{DA952E48-534A-4104-8A72-2BE892964A18}"/>
     <cellStyle name="Comma 3" xfId="11" xr:uid="{856AAB38-97AE-41B8-BFBC-5E8E757493AE}"/>
+    <cellStyle name="Comma 3 2" xfId="25" xr:uid="{59AD52EF-9265-4C99-B7C0-96AA5BE68D7A}"/>
     <cellStyle name="Comma 4" xfId="15" xr:uid="{15E63A3B-FADD-4F72-8A15-82B5F65A0D08}"/>
+    <cellStyle name="Comma 4 2" xfId="28" xr:uid="{CACC3E0D-1D35-4171-B90F-4619D6C6B8C3}"/>
     <cellStyle name="Comma 5" xfId="18" xr:uid="{927AECA0-D30A-42CF-8940-CE1B2E2FC2DF}"/>
+    <cellStyle name="Comma 5 2" xfId="31" xr:uid="{972055C7-AC82-400E-9C46-7F9F28DBE6B2}"/>
     <cellStyle name="Hyperlink 2" xfId="5" xr:uid="{3D82F709-362D-4D82-AFB0-BF8FA139F966}"/>
     <cellStyle name="Hyperlink 3" xfId="21" xr:uid="{021947CE-673E-4762-9284-139DFB8EC828}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1467,14 +1503,21 @@
     <cellStyle name="Normal 3 2" xfId="9" xr:uid="{42A2E569-406F-4F88-9D89-0967D461C4A6}"/>
     <cellStyle name="Normal 3 3" xfId="12" xr:uid="{DF97DA59-1504-4713-9E90-2506C826A8F0}"/>
     <cellStyle name="Normal 3 3 2" xfId="16" xr:uid="{5E963977-ADDB-4375-8D08-CB31A899C327}"/>
+    <cellStyle name="Normal 3 3 2 2" xfId="29" xr:uid="{E4FCCAFF-2ABE-4A68-9245-4EF7BE607772}"/>
     <cellStyle name="Normal 3 3 3" xfId="19" xr:uid="{BE6F8EAD-9690-4445-B85E-271A9106613E}"/>
+    <cellStyle name="Normal 3 3 3 2" xfId="32" xr:uid="{20438A2C-738D-4F7B-9F61-8A821F016EEC}"/>
+    <cellStyle name="Normal 3 3 4" xfId="26" xr:uid="{BB3D5AA7-1E59-4F9E-86AD-1D0332E7DC0A}"/>
     <cellStyle name="Normal 4" xfId="8" xr:uid="{001D71C5-E68F-46CC-B40D-E3877B1676E5}"/>
     <cellStyle name="Normal 5" xfId="10" xr:uid="{38E4D36A-9FBD-45B5-9807-A8E6ED80E2EF}"/>
     <cellStyle name="Normal 5 2" xfId="13" xr:uid="{8D28BC5A-F907-41A1-A063-1AAC30CF5B75}"/>
     <cellStyle name="Normal 6" xfId="1" xr:uid="{C6427557-9C6F-4EC1-9295-1AF4A89B723F}"/>
+    <cellStyle name="Normal 6 2" xfId="24" xr:uid="{5B84B998-B639-4BFA-8D21-4F21BD5FCD1B}"/>
     <cellStyle name="Normal 7" xfId="14" xr:uid="{056F67E3-BB13-454C-BF5A-57B42DEA4E92}"/>
+    <cellStyle name="Normal 7 2" xfId="27" xr:uid="{15D93997-1060-4ED5-AF43-33921A873836}"/>
     <cellStyle name="Normal 8" xfId="17" xr:uid="{277C702A-9C7F-4606-AD28-BDC694550D52}"/>
+    <cellStyle name="Normal 8 2" xfId="30" xr:uid="{69067180-D109-4D08-B6A9-9C3724870505}"/>
     <cellStyle name="Normal 9" xfId="20" xr:uid="{783F6A26-8E57-4958-BF9F-3668E09F38F3}"/>
+    <cellStyle name="Normal 9 2" xfId="33" xr:uid="{D4F11773-BC2F-45EF-AFE3-C77A81CD6F4E}"/>
     <cellStyle name="SAPBEXstdItem" xfId="6" xr:uid="{1DFDC2AD-EB11-42DC-9F9E-B0A36E09E15D}"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1789,8 +1832,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="B59" sqref="B59"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="14.5"/>
@@ -2031,7 +2074,7 @@
       </c>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" s="17" t="s">
+      <c r="A20" s="23" t="s">
         <v>77</v>
       </c>
       <c r="B20" t="b">
@@ -2097,7 +2140,7 @@
         <v>110</v>
       </c>
       <c r="B27">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -2353,7 +2396,7 @@
         <v>306</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>376</v>
+        <v>381</v>
       </c>
       <c r="C59" t="s">
         <v>372</v>
@@ -2394,7 +2437,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="19"/>
+  <phoneticPr fontId="20"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -2404,7 +2447,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -3558,7 +3601,7 @@
     <row r="987" ht="14.25" customHeight="1"/>
     <row r="988" ht="14.25" customHeight="1"/>
   </sheetData>
-  <phoneticPr fontId="19"/>
+  <phoneticPr fontId="20"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3567,8 +3610,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z23"/>
   <sheetViews>
-    <sheetView topLeftCell="C12" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="14.5"/>
@@ -3861,17 +3904,17 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="19"/>
+  <phoneticPr fontId="20"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1D9DC59-3960-42CB-B3EC-EFF452A90D4F}">
-  <dimension ref="A1:Z86"/>
+  <dimension ref="A1:Z89"/>
   <sheetViews>
-    <sheetView topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="B85" sqref="B85"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -4149,449 +4192,473 @@
     </row>
     <row r="31" spans="1:2">
       <c r="A31" t="s">
-        <v>132</v>
+        <v>376</v>
       </c>
       <c r="B31" t="s">
-        <v>138</v>
+        <v>380</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" t="s">
-        <v>133</v>
+        <v>377</v>
       </c>
       <c r="B32" t="s">
-        <v>139</v>
+        <v>380</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" t="s">
-        <v>134</v>
+        <v>378</v>
       </c>
       <c r="B33" t="s">
-        <v>140</v>
+        <v>379</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="B34" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" t="s">
-        <v>155</v>
+        <v>133</v>
       </c>
       <c r="B35" t="s">
-        <v>153</v>
+        <v>139</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" t="s">
-        <v>154</v>
+        <v>134</v>
       </c>
       <c r="B36" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="B37" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B38" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="B39" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
       <c r="B40" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41" t="s">
-        <v>291</v>
+        <v>157</v>
       </c>
       <c r="B41" t="s">
-        <v>292</v>
+        <v>156</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B42" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B43" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44" t="s">
-        <v>169</v>
+        <v>291</v>
       </c>
       <c r="B44" t="s">
-        <v>168</v>
+        <v>292</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="B45" t="s">
-        <v>315</v>
+        <v>164</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46" t="s">
-        <v>353</v>
+        <v>163</v>
       </c>
       <c r="B46" t="s">
-        <v>354</v>
+        <v>165</v>
       </c>
     </row>
     <row r="47" spans="1:2">
       <c r="A47" t="s">
-        <v>252</v>
+        <v>169</v>
       </c>
       <c r="B47" t="s">
-        <v>251</v>
+        <v>168</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48" t="s">
-        <v>143</v>
+        <v>171</v>
       </c>
       <c r="B48" t="s">
-        <v>170</v>
+        <v>315</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49" t="s">
-        <v>144</v>
+        <v>353</v>
       </c>
       <c r="B49" t="s">
-        <v>172</v>
+        <v>354</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50" t="s">
-        <v>145</v>
+        <v>252</v>
       </c>
       <c r="B50" t="s">
-        <v>173</v>
+        <v>251</v>
       </c>
     </row>
     <row r="51" spans="1:2">
       <c r="A51" t="s">
-        <v>174</v>
+        <v>143</v>
       </c>
       <c r="B51" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52" t="s">
-        <v>180</v>
+        <v>144</v>
       </c>
       <c r="B52" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
     </row>
     <row r="53" spans="1:2">
       <c r="A53" t="s">
-        <v>181</v>
+        <v>145</v>
       </c>
       <c r="B53" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
     </row>
     <row r="54" spans="1:2">
       <c r="A54" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="B54" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
       <c r="B55" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
       <c r="B56" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
     </row>
     <row r="57" spans="1:2">
       <c r="A57" t="s">
-        <v>177</v>
+        <v>184</v>
       </c>
       <c r="B57" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
     </row>
     <row r="58" spans="1:2">
       <c r="A58" t="s">
-        <v>190</v>
+        <v>175</v>
       </c>
       <c r="B58" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="59" spans="1:2">
       <c r="A59" t="s">
-        <v>194</v>
+        <v>176</v>
       </c>
       <c r="B59" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
     </row>
     <row r="60" spans="1:2">
       <c r="A60" t="s">
-        <v>197</v>
+        <v>177</v>
       </c>
       <c r="B60" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
     </row>
     <row r="61" spans="1:2">
       <c r="A61" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B61" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
     </row>
     <row r="62" spans="1:2">
       <c r="A62" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="B62" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="63" spans="1:2">
       <c r="A63" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B63" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
     </row>
     <row r="64" spans="1:2">
       <c r="A64" t="s">
-        <v>201</v>
+        <v>191</v>
       </c>
       <c r="B64" t="s">
-        <v>203</v>
+        <v>193</v>
       </c>
     </row>
     <row r="65" spans="1:2">
       <c r="A65" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="B65" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
     </row>
     <row r="66" spans="1:2">
       <c r="A66" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="B66" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
     </row>
     <row r="67" spans="1:2">
       <c r="A67" t="s">
-        <v>285</v>
+        <v>201</v>
       </c>
       <c r="B67" t="s">
-        <v>286</v>
+        <v>203</v>
       </c>
     </row>
     <row r="68" spans="1:2">
       <c r="A68" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="B68" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
     </row>
     <row r="69" spans="1:2">
       <c r="A69" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="B69" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
     </row>
     <row r="70" spans="1:2">
       <c r="A70" t="s">
-        <v>213</v>
+        <v>285</v>
       </c>
       <c r="B70" t="s">
-        <v>214</v>
+        <v>286</v>
       </c>
     </row>
     <row r="71" spans="1:2">
       <c r="A71" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="B71" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
     </row>
     <row r="72" spans="1:2">
       <c r="A72" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="B72" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
     </row>
     <row r="73" spans="1:2">
       <c r="A73" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="B73" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
     </row>
     <row r="74" spans="1:2">
       <c r="A74" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
       <c r="B74" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
     </row>
     <row r="75" spans="1:2">
       <c r="A75" t="s">
-        <v>207</v>
+        <v>218</v>
       </c>
       <c r="B75" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="76" spans="1:2">
       <c r="A76" t="s">
-        <v>208</v>
+        <v>222</v>
       </c>
       <c r="B76" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
     </row>
     <row r="77" spans="1:2">
       <c r="A77" t="s">
-        <v>209</v>
+        <v>223</v>
       </c>
       <c r="B77" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
     </row>
     <row r="78" spans="1:2">
       <c r="A78" t="s">
-        <v>262</v>
+        <v>207</v>
       </c>
       <c r="B78" t="s">
-        <v>265</v>
+        <v>220</v>
       </c>
     </row>
     <row r="79" spans="1:2">
       <c r="A79" t="s">
-        <v>263</v>
+        <v>208</v>
       </c>
       <c r="B79" t="s">
-        <v>266</v>
+        <v>225</v>
       </c>
     </row>
     <row r="80" spans="1:2">
       <c r="A80" t="s">
-        <v>264</v>
+        <v>209</v>
       </c>
       <c r="B80" t="s">
-        <v>267</v>
+        <v>224</v>
       </c>
     </row>
     <row r="81" spans="1:2">
       <c r="A81" t="s">
-        <v>357</v>
+        <v>262</v>
       </c>
       <c r="B81" t="s">
-        <v>358</v>
+        <v>265</v>
       </c>
     </row>
     <row r="82" spans="1:2">
       <c r="A82" t="s">
-        <v>363</v>
+        <v>263</v>
       </c>
       <c r="B82" t="s">
-        <v>364</v>
+        <v>266</v>
       </c>
     </row>
     <row r="83" spans="1:2">
       <c r="A83" t="s">
-        <v>365</v>
+        <v>264</v>
       </c>
       <c r="B83" t="s">
-        <v>366</v>
+        <v>267</v>
       </c>
     </row>
     <row r="84" spans="1:2">
       <c r="A84" t="s">
-        <v>367</v>
+        <v>357</v>
       </c>
       <c r="B84" t="s">
-        <v>366</v>
+        <v>358</v>
       </c>
     </row>
     <row r="85" spans="1:2">
       <c r="A85" t="s">
-        <v>359</v>
+        <v>363</v>
       </c>
       <c r="B85" t="s">
-        <v>361</v>
+        <v>364</v>
       </c>
     </row>
     <row r="86" spans="1:2">
       <c r="A86" t="s">
+        <v>365</v>
+      </c>
+      <c r="B86" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2">
+      <c r="A87" t="s">
+        <v>367</v>
+      </c>
+      <c r="B87" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2">
+      <c r="A88" t="s">
+        <v>359</v>
+      </c>
+      <c r="B88" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2">
+      <c r="A89" t="s">
         <v>360</v>
       </c>
-      <c r="B86" t="s">
+      <c r="B89" t="s">
         <v>362</v>
       </c>
     </row>

</xml_diff>

<commit_message>
made changes to the Peoplesoft login as password expiry exception added.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\55651C\Documents\GitHub\P002_090_PayCyleAfternoon_Dispatcher\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13589407-6BFF-40C3-8428-40E8963820D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{977E1869-97A5-40F6-954D-7428BAC06BA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="382">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="394">
   <si>
     <t>Name</t>
   </si>
@@ -99,11 +99,11 @@
   </si>
   <si>
     <t>Orchestrator queue Name. The value must match with the queue name defined on Orchestrator.</t>
-    <phoneticPr fontId="20"/>
+    <phoneticPr fontId="21"/>
   </si>
   <si>
     <t>Logging field which allows grouping of log data of two or more subprocesses under the same business process name</t>
-    <phoneticPr fontId="20"/>
+    <phoneticPr fontId="21"/>
   </si>
   <si>
     <t>Must be 0 if working with Orchestrator queues. If &gt; 0, the robot will retry the same transaction which failed with a system exception. Must be an integer value.</t>
@@ -698,9 +698,6 @@
   </si>
   <si>
     <t>Attachment File is present.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Workflow to send an email has completed successfully.</t>
   </si>
   <si>
     <t>Attachment file not found on mentioned path.</t>
@@ -1145,9 +1142,6 @@
     <t>LocalFolderNotPresentSE</t>
   </si>
   <si>
-    <t>BE_1,BE_2,SE_4,SE_2,BE_3,SE_3</t>
-  </si>
-  <si>
     <t>ProcessFolderName</t>
   </si>
   <si>
@@ -1157,9 +1151,6 @@
     <t>PROD/P002_090_PayCycleAfternoon</t>
   </si>
   <si>
-    <t>DEV</t>
-  </si>
-  <si>
     <t>excel</t>
   </si>
   <si>
@@ -1182,6 +1173,51 @@
   </si>
   <si>
     <t>Records from the table could not be extracted for OKBATCNN.</t>
+  </si>
+  <si>
+    <t>PeoplesoftCredentialsExpiredSE</t>
+  </si>
+  <si>
+    <t>People Soft Credenatials expired.</t>
+  </si>
+  <si>
+    <t>SE_5: People Soft Credenatials have expired.</t>
+  </si>
+  <si>
+    <t>PeoplesoftCredentialsExpiredSE_5</t>
+  </si>
+  <si>
+    <t>BE_1,BE_2,SE_4,SE_2,BE_3,SE_3,SE_5</t>
+  </si>
+  <si>
+    <t>Workflow to send an email has completed successfully.</t>
+  </si>
+  <si>
+    <t>SE_5Subject</t>
+  </si>
+  <si>
+    <t>SE_5Body</t>
+  </si>
+  <si>
+    <t>Peoplesoft Credentials Expired for Pay Cycle Afternoon Process</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hi Statewide Accounting Team,&lt;br&gt;&lt;br&gt;PeopleSoft credentials expired for user ID &lt;Bot_user_ID&gt;. &lt;br&gt;&lt;br&gt;Automation support team: Please confirm that the login credentials are valid / updated prior to the next Bot run&lt;br&gt; &lt;br&gt; Thanks,&lt;br&gt;Automation Team               </t>
+  </si>
+  <si>
+    <t>P002_090_PayCycleAfternoon_SE_5RecipientEmailAddress</t>
+  </si>
+  <si>
+    <t>P002_090_PayCycleAfternoon_SE_5CCEmailAddress</t>
+  </si>
+  <si>
+    <t>SE_5RecipientEmailAddress</t>
+  </si>
+  <si>
+    <t>SE_5CCEmailAddress</t>
+  </si>
+  <si>
+    <t>ProcessRunFolderName</t>
   </si>
   <si>
     <t>PROD</t>
@@ -1194,11 +1230,18 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="27">
+  <fonts count="28">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1415,62 +1458,63 @@
   </borders>
   <cellStyleXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="23" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="4" fontId="25" fillId="2" borderId="1" applyNumberFormat="0" applyProtection="0">
+    <xf numFmtId="4" fontId="26" fillId="2" borderId="1" applyNumberFormat="0" applyProtection="0">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="20"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="20"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="20" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="20" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="20" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="20" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="20" applyFont="1"/>
+    <xf numFmtId="49" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="20" applyFont="1"/>
-    <xf numFmtId="49" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="20" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="20" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="20" applyFont="1"/>
@@ -1830,10 +1874,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z64"/>
+  <dimension ref="A1:Z66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
+      <selection activeCell="B60" sqref="B60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="14.5"/>
@@ -1883,7 +1927,7 @@
         <v>185</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>20</v>
@@ -1893,8 +1937,9 @@
       <c r="A3" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>371</v>
+      <c r="B3" s="2" t="str">
+        <f>_xlfn.CONCAT(Constants!$B$18,"/P002_090_PayCycleAfternoon")</f>
+        <v>PROD/P002_090_PayCycleAfternoon</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>29</v>
@@ -1905,7 +1950,7 @@
         <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>21</v>
@@ -1924,10 +1969,11 @@
     </row>
     <row r="6" spans="1:26">
       <c r="A6" t="s">
-        <v>323</v>
-      </c>
-      <c r="B6" t="s">
-        <v>371</v>
+        <v>322</v>
+      </c>
+      <c r="B6" t="str">
+        <f>_xlfn.CONCAT(Constants!$B$18,"/P002_090_PayCycleAfternoon")</f>
+        <v>PROD/P002_090_PayCycleAfternoon</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="58">
@@ -1935,7 +1981,7 @@
         <v>48</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C7" t="s">
         <v>49</v>
@@ -2012,7 +2058,7 @@
         <v>65</v>
       </c>
       <c r="B14" s="21" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>66</v>
@@ -2023,7 +2069,7 @@
         <v>67</v>
       </c>
       <c r="B15" s="21" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>68</v>
@@ -2034,7 +2080,7 @@
         <v>69</v>
       </c>
       <c r="B16" s="22" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>70</v>
@@ -2188,7 +2234,7 @@
         <v>148</v>
       </c>
       <c r="B33" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -2196,7 +2242,7 @@
         <v>149</v>
       </c>
       <c r="B34" s="11" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -2217,15 +2263,15 @@
     </row>
     <row r="37" spans="1:2">
       <c r="A37" s="19" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B37" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" s="18" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B38" t="b">
         <v>1</v>
@@ -2233,31 +2279,31 @@
     </row>
     <row r="39" spans="1:2">
       <c r="A39" s="13" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B39" t="s">
-        <v>368</v>
+        <v>382</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" s="12" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B40" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="58">
       <c r="A41" s="12" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" s="13" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B42" s="3">
         <v>15</v>
@@ -2265,179 +2311,193 @@
     </row>
     <row r="43" spans="1:2">
       <c r="A43" s="16" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B43" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="43.5">
       <c r="A44" s="12" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" s="19" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B45" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="29">
       <c r="A46" s="19" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="47" spans="1:2">
       <c r="A47" s="19" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B47" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="58">
       <c r="A48" s="19" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B48" s="3" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" s="12" t="s">
+        <v>256</v>
+      </c>
+      <c r="B49" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="29">
+      <c r="A50" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="B50" s="3" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="49" spans="1:3">
-      <c r="A49" s="12" t="s">
-        <v>257</v>
-      </c>
-      <c r="B49" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" ht="29">
-      <c r="A50" s="12" t="s">
-        <v>258</v>
-      </c>
-      <c r="B50" s="3" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3">
+    <row r="51" spans="1:2">
       <c r="A51" s="19" t="s">
+        <v>342</v>
+      </c>
+      <c r="B51" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="43.5">
+      <c r="A52" s="19" t="s">
         <v>343</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B52" s="3" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="43.5">
-      <c r="A52" s="19" t="s">
-        <v>344</v>
-      </c>
-      <c r="B52" s="3" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3">
-      <c r="A53" s="15" t="s">
+    <row r="53" spans="1:2">
+      <c r="A53" s="24" t="s">
+        <v>384</v>
+      </c>
+      <c r="B53" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" ht="43.5">
+      <c r="A54" s="24" t="s">
+        <v>385</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" s="15" t="s">
+        <v>275</v>
+      </c>
+      <c r="B55" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" s="14" t="s">
         <v>276</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B56" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="54" spans="1:3">
-      <c r="A54" s="14" t="s">
+    <row r="57" spans="1:2">
+      <c r="A57" s="14" t="s">
         <v>277</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B57" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="55" spans="1:3">
-      <c r="A55" s="14" t="s">
-        <v>278</v>
-      </c>
-      <c r="B55" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3">
-      <c r="A56" t="s">
-        <v>275</v>
-      </c>
-      <c r="B56" t="s">
+    <row r="58" spans="1:2">
+      <c r="A58" t="s">
         <v>274</v>
       </c>
-    </row>
-    <row r="57" spans="1:3">
-      <c r="A57" t="s">
+      <c r="B58" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59" t="s">
+        <v>270</v>
+      </c>
+      <c r="B59" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60" t="s">
+        <v>272</v>
+      </c>
+      <c r="B60" t="s">
         <v>271</v>
       </c>
-      <c r="B57" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3">
-      <c r="A58" t="s">
-        <v>273</v>
-      </c>
-      <c r="B58" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3">
-      <c r="A59" t="s">
+    </row>
+    <row r="61" spans="1:2">
+      <c r="A61" t="s">
+        <v>305</v>
+      </c>
+      <c r="B61" s="2" t="str">
+        <f>Constants!$B$18</f>
+        <v>PROD</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
+      <c r="A62" t="s">
         <v>306</v>
       </c>
-      <c r="B59" s="2" t="s">
-        <v>381</v>
-      </c>
-      <c r="C59" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3">
-      <c r="A60" t="s">
+      <c r="B62" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
+      <c r="A63" t="s">
         <v>307</v>
       </c>
-      <c r="B60" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3">
-      <c r="A61" t="s">
+    </row>
+    <row r="64" spans="1:2">
+      <c r="A64" t="s">
         <v>308</v>
       </c>
-    </row>
-    <row r="62" spans="1:3">
-      <c r="A62" t="s">
-        <v>309</v>
-      </c>
-      <c r="B62">
+      <c r="B64">
         <v>2</v>
       </c>
     </row>
-    <row r="63" spans="1:3">
-      <c r="A63" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3">
-      <c r="A64" t="s">
-        <v>369</v>
-      </c>
-      <c r="B64" t="s">
-        <v>370</v>
+    <row r="65" spans="1:2">
+      <c r="A65" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
+      <c r="A66" t="s">
+        <v>367</v>
+      </c>
+      <c r="B66" t="s">
+        <v>368</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="20"/>
+  <phoneticPr fontId="21"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -2445,13 +2505,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z988"/>
+  <dimension ref="A1:Z18"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
@@ -2459,7 +2519,7 @@
     <col min="4" max="26" width="8.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="14.25" customHeight="1">
+    <row r="1" spans="1:26" ht="18.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2515,8 +2575,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1">
+    <row r="5" spans="1:26">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -2527,8 +2586,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1">
+    <row r="7" spans="1:26">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -2539,7 +2597,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1">
+    <row r="8" spans="1:26">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -2550,7 +2608,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1">
+    <row r="9" spans="1:26">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -2561,7 +2619,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1">
+    <row r="10" spans="1:26">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -2572,7 +2630,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1">
+    <row r="11" spans="1:26">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -2583,7 +2641,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1">
+    <row r="12" spans="1:26">
       <c r="A12" t="s">
         <v>31</v>
       </c>
@@ -2594,8 +2652,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1">
+    <row r="14" spans="1:26">
       <c r="A14" t="s">
         <v>32</v>
       </c>
@@ -2606,7 +2663,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1">
+    <row r="15" spans="1:26">
       <c r="A15" t="s">
         <v>33</v>
       </c>
@@ -2617,7 +2674,6 @@
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" spans="1:3" ht="29">
       <c r="A17" t="s">
         <v>37</v>
@@ -2629,989 +2685,26 @@
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="19" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="20" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="21" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="22" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="23" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="24" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="25" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="26" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="27" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="28" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="29" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="30" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="31" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="32" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="33" ht="14.25" customHeight="1"/>
-    <row r="34" ht="14.25" customHeight="1"/>
-    <row r="35" ht="14.25" customHeight="1"/>
-    <row r="36" ht="14.25" customHeight="1"/>
-    <row r="37" ht="14.25" customHeight="1"/>
-    <row r="38" ht="14.25" customHeight="1"/>
-    <row r="39" ht="14.25" customHeight="1"/>
-    <row r="40" ht="14.25" customHeight="1"/>
-    <row r="41" ht="14.25" customHeight="1"/>
-    <row r="42" ht="14.25" customHeight="1"/>
-    <row r="43" ht="14.25" customHeight="1"/>
-    <row r="44" ht="14.25" customHeight="1"/>
-    <row r="45" ht="14.25" customHeight="1"/>
-    <row r="46" ht="14.25" customHeight="1"/>
-    <row r="47" ht="14.25" customHeight="1"/>
-    <row r="48" ht="14.25" customHeight="1"/>
-    <row r="49" ht="14.25" customHeight="1"/>
-    <row r="50" ht="14.25" customHeight="1"/>
-    <row r="51" ht="14.25" customHeight="1"/>
-    <row r="52" ht="14.25" customHeight="1"/>
-    <row r="53" ht="14.25" customHeight="1"/>
-    <row r="54" ht="14.25" customHeight="1"/>
-    <row r="55" ht="14.25" customHeight="1"/>
-    <row r="56" ht="14.25" customHeight="1"/>
-    <row r="57" ht="14.25" customHeight="1"/>
-    <row r="58" ht="14.25" customHeight="1"/>
-    <row r="59" ht="14.25" customHeight="1"/>
-    <row r="60" ht="14.25" customHeight="1"/>
-    <row r="61" ht="14.25" customHeight="1"/>
-    <row r="62" ht="14.25" customHeight="1"/>
-    <row r="63" ht="14.25" customHeight="1"/>
-    <row r="64" ht="14.25" customHeight="1"/>
-    <row r="65" ht="14.25" customHeight="1"/>
-    <row r="66" ht="14.25" customHeight="1"/>
-    <row r="67" ht="14.25" customHeight="1"/>
-    <row r="68" ht="14.25" customHeight="1"/>
-    <row r="69" ht="14.25" customHeight="1"/>
-    <row r="70" ht="14.25" customHeight="1"/>
-    <row r="71" ht="14.25" customHeight="1"/>
-    <row r="72" ht="14.25" customHeight="1"/>
-    <row r="73" ht="14.25" customHeight="1"/>
-    <row r="74" ht="14.25" customHeight="1"/>
-    <row r="75" ht="14.25" customHeight="1"/>
-    <row r="76" ht="14.25" customHeight="1"/>
-    <row r="77" ht="14.25" customHeight="1"/>
-    <row r="78" ht="14.25" customHeight="1"/>
-    <row r="79" ht="14.25" customHeight="1"/>
-    <row r="80" ht="14.25" customHeight="1"/>
-    <row r="81" ht="14.25" customHeight="1"/>
-    <row r="82" ht="14.25" customHeight="1"/>
-    <row r="83" ht="14.25" customHeight="1"/>
-    <row r="84" ht="14.25" customHeight="1"/>
-    <row r="85" ht="14.25" customHeight="1"/>
-    <row r="86" ht="14.25" customHeight="1"/>
-    <row r="87" ht="14.25" customHeight="1"/>
-    <row r="88" ht="14.25" customHeight="1"/>
-    <row r="89" ht="14.25" customHeight="1"/>
-    <row r="90" ht="14.25" customHeight="1"/>
-    <row r="91" ht="14.25" customHeight="1"/>
-    <row r="92" ht="14.25" customHeight="1"/>
-    <row r="93" ht="14.25" customHeight="1"/>
-    <row r="94" ht="14.25" customHeight="1"/>
-    <row r="95" ht="14.25" customHeight="1"/>
-    <row r="96" ht="14.25" customHeight="1"/>
-    <row r="97" ht="14.25" customHeight="1"/>
-    <row r="98" ht="14.25" customHeight="1"/>
-    <row r="99" ht="14.25" customHeight="1"/>
-    <row r="100" ht="14.25" customHeight="1"/>
-    <row r="101" ht="14.25" customHeight="1"/>
-    <row r="102" ht="14.25" customHeight="1"/>
-    <row r="103" ht="14.25" customHeight="1"/>
-    <row r="104" ht="14.25" customHeight="1"/>
-    <row r="105" ht="14.25" customHeight="1"/>
-    <row r="106" ht="14.25" customHeight="1"/>
-    <row r="107" ht="14.25" customHeight="1"/>
-    <row r="108" ht="14.25" customHeight="1"/>
-    <row r="109" ht="14.25" customHeight="1"/>
-    <row r="110" ht="14.25" customHeight="1"/>
-    <row r="111" ht="14.25" customHeight="1"/>
-    <row r="112" ht="14.25" customHeight="1"/>
-    <row r="113" ht="14.25" customHeight="1"/>
-    <row r="114" ht="14.25" customHeight="1"/>
-    <row r="115" ht="14.25" customHeight="1"/>
-    <row r="116" ht="14.25" customHeight="1"/>
-    <row r="117" ht="14.25" customHeight="1"/>
-    <row r="118" ht="14.25" customHeight="1"/>
-    <row r="119" ht="14.25" customHeight="1"/>
-    <row r="120" ht="14.25" customHeight="1"/>
-    <row r="121" ht="14.25" customHeight="1"/>
-    <row r="122" ht="14.25" customHeight="1"/>
-    <row r="123" ht="14.25" customHeight="1"/>
-    <row r="124" ht="14.25" customHeight="1"/>
-    <row r="125" ht="14.25" customHeight="1"/>
-    <row r="126" ht="14.25" customHeight="1"/>
-    <row r="127" ht="14.25" customHeight="1"/>
-    <row r="128" ht="14.25" customHeight="1"/>
-    <row r="129" ht="14.25" customHeight="1"/>
-    <row r="130" ht="14.25" customHeight="1"/>
-    <row r="131" ht="14.25" customHeight="1"/>
-    <row r="132" ht="14.25" customHeight="1"/>
-    <row r="133" ht="14.25" customHeight="1"/>
-    <row r="134" ht="14.25" customHeight="1"/>
-    <row r="135" ht="14.25" customHeight="1"/>
-    <row r="136" ht="14.25" customHeight="1"/>
-    <row r="137" ht="14.25" customHeight="1"/>
-    <row r="138" ht="14.25" customHeight="1"/>
-    <row r="139" ht="14.25" customHeight="1"/>
-    <row r="140" ht="14.25" customHeight="1"/>
-    <row r="141" ht="14.25" customHeight="1"/>
-    <row r="142" ht="14.25" customHeight="1"/>
-    <row r="143" ht="14.25" customHeight="1"/>
-    <row r="144" ht="14.25" customHeight="1"/>
-    <row r="145" ht="14.25" customHeight="1"/>
-    <row r="146" ht="14.25" customHeight="1"/>
-    <row r="147" ht="14.25" customHeight="1"/>
-    <row r="148" ht="14.25" customHeight="1"/>
-    <row r="149" ht="14.25" customHeight="1"/>
-    <row r="150" ht="14.25" customHeight="1"/>
-    <row r="151" ht="14.25" customHeight="1"/>
-    <row r="152" ht="14.25" customHeight="1"/>
-    <row r="153" ht="14.25" customHeight="1"/>
-    <row r="154" ht="14.25" customHeight="1"/>
-    <row r="155" ht="14.25" customHeight="1"/>
-    <row r="156" ht="14.25" customHeight="1"/>
-    <row r="157" ht="14.25" customHeight="1"/>
-    <row r="158" ht="14.25" customHeight="1"/>
-    <row r="159" ht="14.25" customHeight="1"/>
-    <row r="160" ht="14.25" customHeight="1"/>
-    <row r="161" ht="14.25" customHeight="1"/>
-    <row r="162" ht="14.25" customHeight="1"/>
-    <row r="163" ht="14.25" customHeight="1"/>
-    <row r="164" ht="14.25" customHeight="1"/>
-    <row r="165" ht="14.25" customHeight="1"/>
-    <row r="166" ht="14.25" customHeight="1"/>
-    <row r="167" ht="14.25" customHeight="1"/>
-    <row r="168" ht="14.25" customHeight="1"/>
-    <row r="169" ht="14.25" customHeight="1"/>
-    <row r="170" ht="14.25" customHeight="1"/>
-    <row r="171" ht="14.25" customHeight="1"/>
-    <row r="172" ht="14.25" customHeight="1"/>
-    <row r="173" ht="14.25" customHeight="1"/>
-    <row r="174" ht="14.25" customHeight="1"/>
-    <row r="175" ht="14.25" customHeight="1"/>
-    <row r="176" ht="14.25" customHeight="1"/>
-    <row r="177" ht="14.25" customHeight="1"/>
-    <row r="178" ht="14.25" customHeight="1"/>
-    <row r="179" ht="14.25" customHeight="1"/>
-    <row r="180" ht="14.25" customHeight="1"/>
-    <row r="181" ht="14.25" customHeight="1"/>
-    <row r="182" ht="14.25" customHeight="1"/>
-    <row r="183" ht="14.25" customHeight="1"/>
-    <row r="184" ht="14.25" customHeight="1"/>
-    <row r="185" ht="14.25" customHeight="1"/>
-    <row r="186" ht="14.25" customHeight="1"/>
-    <row r="187" ht="14.25" customHeight="1"/>
-    <row r="188" ht="14.25" customHeight="1"/>
-    <row r="189" ht="14.25" customHeight="1"/>
-    <row r="190" ht="14.25" customHeight="1"/>
-    <row r="191" ht="14.25" customHeight="1"/>
-    <row r="192" ht="14.25" customHeight="1"/>
-    <row r="193" ht="14.25" customHeight="1"/>
-    <row r="194" ht="14.25" customHeight="1"/>
-    <row r="195" ht="14.25" customHeight="1"/>
-    <row r="196" ht="14.25" customHeight="1"/>
-    <row r="197" ht="14.25" customHeight="1"/>
-    <row r="198" ht="14.25" customHeight="1"/>
-    <row r="199" ht="14.25" customHeight="1"/>
-    <row r="200" ht="14.25" customHeight="1"/>
-    <row r="201" ht="14.25" customHeight="1"/>
-    <row r="202" ht="14.25" customHeight="1"/>
-    <row r="203" ht="14.25" customHeight="1"/>
-    <row r="204" ht="14.25" customHeight="1"/>
-    <row r="205" ht="14.25" customHeight="1"/>
-    <row r="206" ht="14.25" customHeight="1"/>
-    <row r="207" ht="14.25" customHeight="1"/>
-    <row r="208" ht="14.25" customHeight="1"/>
-    <row r="209" ht="14.25" customHeight="1"/>
-    <row r="210" ht="14.25" customHeight="1"/>
-    <row r="211" ht="14.25" customHeight="1"/>
-    <row r="212" ht="14.25" customHeight="1"/>
-    <row r="213" ht="14.25" customHeight="1"/>
-    <row r="214" ht="14.25" customHeight="1"/>
-    <row r="215" ht="14.25" customHeight="1"/>
-    <row r="216" ht="14.25" customHeight="1"/>
-    <row r="217" ht="14.25" customHeight="1"/>
-    <row r="218" ht="14.25" customHeight="1"/>
-    <row r="219" ht="14.25" customHeight="1"/>
-    <row r="220" ht="14.25" customHeight="1"/>
-    <row r="221" ht="14.25" customHeight="1"/>
-    <row r="222" ht="14.25" customHeight="1"/>
-    <row r="223" ht="14.25" customHeight="1"/>
-    <row r="224" ht="14.25" customHeight="1"/>
-    <row r="225" ht="14.25" customHeight="1"/>
-    <row r="226" ht="14.25" customHeight="1"/>
-    <row r="227" ht="14.25" customHeight="1"/>
-    <row r="228" ht="14.25" customHeight="1"/>
-    <row r="229" ht="14.25" customHeight="1"/>
-    <row r="230" ht="14.25" customHeight="1"/>
-    <row r="231" ht="14.25" customHeight="1"/>
-    <row r="232" ht="14.25" customHeight="1"/>
-    <row r="233" ht="14.25" customHeight="1"/>
-    <row r="234" ht="14.25" customHeight="1"/>
-    <row r="235" ht="14.25" customHeight="1"/>
-    <row r="236" ht="14.25" customHeight="1"/>
-    <row r="237" ht="14.25" customHeight="1"/>
-    <row r="238" ht="14.25" customHeight="1"/>
-    <row r="239" ht="14.25" customHeight="1"/>
-    <row r="240" ht="14.25" customHeight="1"/>
-    <row r="241" ht="14.25" customHeight="1"/>
-    <row r="242" ht="14.25" customHeight="1"/>
-    <row r="243" ht="14.25" customHeight="1"/>
-    <row r="244" ht="14.25" customHeight="1"/>
-    <row r="245" ht="14.25" customHeight="1"/>
-    <row r="246" ht="14.25" customHeight="1"/>
-    <row r="247" ht="14.25" customHeight="1"/>
-    <row r="248" ht="14.25" customHeight="1"/>
-    <row r="249" ht="14.25" customHeight="1"/>
-    <row r="250" ht="14.25" customHeight="1"/>
-    <row r="251" ht="14.25" customHeight="1"/>
-    <row r="252" ht="14.25" customHeight="1"/>
-    <row r="253" ht="14.25" customHeight="1"/>
-    <row r="254" ht="14.25" customHeight="1"/>
-    <row r="255" ht="14.25" customHeight="1"/>
-    <row r="256" ht="14.25" customHeight="1"/>
-    <row r="257" ht="14.25" customHeight="1"/>
-    <row r="258" ht="14.25" customHeight="1"/>
-    <row r="259" ht="14.25" customHeight="1"/>
-    <row r="260" ht="14.25" customHeight="1"/>
-    <row r="261" ht="14.25" customHeight="1"/>
-    <row r="262" ht="14.25" customHeight="1"/>
-    <row r="263" ht="14.25" customHeight="1"/>
-    <row r="264" ht="14.25" customHeight="1"/>
-    <row r="265" ht="14.25" customHeight="1"/>
-    <row r="266" ht="14.25" customHeight="1"/>
-    <row r="267" ht="14.25" customHeight="1"/>
-    <row r="268" ht="14.25" customHeight="1"/>
-    <row r="269" ht="14.25" customHeight="1"/>
-    <row r="270" ht="14.25" customHeight="1"/>
-    <row r="271" ht="14.25" customHeight="1"/>
-    <row r="272" ht="14.25" customHeight="1"/>
-    <row r="273" ht="14.25" customHeight="1"/>
-    <row r="274" ht="14.25" customHeight="1"/>
-    <row r="275" ht="14.25" customHeight="1"/>
-    <row r="276" ht="14.25" customHeight="1"/>
-    <row r="277" ht="14.25" customHeight="1"/>
-    <row r="278" ht="14.25" customHeight="1"/>
-    <row r="279" ht="14.25" customHeight="1"/>
-    <row r="280" ht="14.25" customHeight="1"/>
-    <row r="281" ht="14.25" customHeight="1"/>
-    <row r="282" ht="14.25" customHeight="1"/>
-    <row r="283" ht="14.25" customHeight="1"/>
-    <row r="284" ht="14.25" customHeight="1"/>
-    <row r="285" ht="14.25" customHeight="1"/>
-    <row r="286" ht="14.25" customHeight="1"/>
-    <row r="287" ht="14.25" customHeight="1"/>
-    <row r="288" ht="14.25" customHeight="1"/>
-    <row r="289" ht="14.25" customHeight="1"/>
-    <row r="290" ht="14.25" customHeight="1"/>
-    <row r="291" ht="14.25" customHeight="1"/>
-    <row r="292" ht="14.25" customHeight="1"/>
-    <row r="293" ht="14.25" customHeight="1"/>
-    <row r="294" ht="14.25" customHeight="1"/>
-    <row r="295" ht="14.25" customHeight="1"/>
-    <row r="296" ht="14.25" customHeight="1"/>
-    <row r="297" ht="14.25" customHeight="1"/>
-    <row r="298" ht="14.25" customHeight="1"/>
-    <row r="299" ht="14.25" customHeight="1"/>
-    <row r="300" ht="14.25" customHeight="1"/>
-    <row r="301" ht="14.25" customHeight="1"/>
-    <row r="302" ht="14.25" customHeight="1"/>
-    <row r="303" ht="14.25" customHeight="1"/>
-    <row r="304" ht="14.25" customHeight="1"/>
-    <row r="305" ht="14.25" customHeight="1"/>
-    <row r="306" ht="14.25" customHeight="1"/>
-    <row r="307" ht="14.25" customHeight="1"/>
-    <row r="308" ht="14.25" customHeight="1"/>
-    <row r="309" ht="14.25" customHeight="1"/>
-    <row r="310" ht="14.25" customHeight="1"/>
-    <row r="311" ht="14.25" customHeight="1"/>
-    <row r="312" ht="14.25" customHeight="1"/>
-    <row r="313" ht="14.25" customHeight="1"/>
-    <row r="314" ht="14.25" customHeight="1"/>
-    <row r="315" ht="14.25" customHeight="1"/>
-    <row r="316" ht="14.25" customHeight="1"/>
-    <row r="317" ht="14.25" customHeight="1"/>
-    <row r="318" ht="14.25" customHeight="1"/>
-    <row r="319" ht="14.25" customHeight="1"/>
-    <row r="320" ht="14.25" customHeight="1"/>
-    <row r="321" ht="14.25" customHeight="1"/>
-    <row r="322" ht="14.25" customHeight="1"/>
-    <row r="323" ht="14.25" customHeight="1"/>
-    <row r="324" ht="14.25" customHeight="1"/>
-    <row r="325" ht="14.25" customHeight="1"/>
-    <row r="326" ht="14.25" customHeight="1"/>
-    <row r="327" ht="14.25" customHeight="1"/>
-    <row r="328" ht="14.25" customHeight="1"/>
-    <row r="329" ht="14.25" customHeight="1"/>
-    <row r="330" ht="14.25" customHeight="1"/>
-    <row r="331" ht="14.25" customHeight="1"/>
-    <row r="332" ht="14.25" customHeight="1"/>
-    <row r="333" ht="14.25" customHeight="1"/>
-    <row r="334" ht="14.25" customHeight="1"/>
-    <row r="335" ht="14.25" customHeight="1"/>
-    <row r="336" ht="14.25" customHeight="1"/>
-    <row r="337" ht="14.25" customHeight="1"/>
-    <row r="338" ht="14.25" customHeight="1"/>
-    <row r="339" ht="14.25" customHeight="1"/>
-    <row r="340" ht="14.25" customHeight="1"/>
-    <row r="341" ht="14.25" customHeight="1"/>
-    <row r="342" ht="14.25" customHeight="1"/>
-    <row r="343" ht="14.25" customHeight="1"/>
-    <row r="344" ht="14.25" customHeight="1"/>
-    <row r="345" ht="14.25" customHeight="1"/>
-    <row r="346" ht="14.25" customHeight="1"/>
-    <row r="347" ht="14.25" customHeight="1"/>
-    <row r="348" ht="14.25" customHeight="1"/>
-    <row r="349" ht="14.25" customHeight="1"/>
-    <row r="350" ht="14.25" customHeight="1"/>
-    <row r="351" ht="14.25" customHeight="1"/>
-    <row r="352" ht="14.25" customHeight="1"/>
-    <row r="353" ht="14.25" customHeight="1"/>
-    <row r="354" ht="14.25" customHeight="1"/>
-    <row r="355" ht="14.25" customHeight="1"/>
-    <row r="356" ht="14.25" customHeight="1"/>
-    <row r="357" ht="14.25" customHeight="1"/>
-    <row r="358" ht="14.25" customHeight="1"/>
-    <row r="359" ht="14.25" customHeight="1"/>
-    <row r="360" ht="14.25" customHeight="1"/>
-    <row r="361" ht="14.25" customHeight="1"/>
-    <row r="362" ht="14.25" customHeight="1"/>
-    <row r="363" ht="14.25" customHeight="1"/>
-    <row r="364" ht="14.25" customHeight="1"/>
-    <row r="365" ht="14.25" customHeight="1"/>
-    <row r="366" ht="14.25" customHeight="1"/>
-    <row r="367" ht="14.25" customHeight="1"/>
-    <row r="368" ht="14.25" customHeight="1"/>
-    <row r="369" ht="14.25" customHeight="1"/>
-    <row r="370" ht="14.25" customHeight="1"/>
-    <row r="371" ht="14.25" customHeight="1"/>
-    <row r="372" ht="14.25" customHeight="1"/>
-    <row r="373" ht="14.25" customHeight="1"/>
-    <row r="374" ht="14.25" customHeight="1"/>
-    <row r="375" ht="14.25" customHeight="1"/>
-    <row r="376" ht="14.25" customHeight="1"/>
-    <row r="377" ht="14.25" customHeight="1"/>
-    <row r="378" ht="14.25" customHeight="1"/>
-    <row r="379" ht="14.25" customHeight="1"/>
-    <row r="380" ht="14.25" customHeight="1"/>
-    <row r="381" ht="14.25" customHeight="1"/>
-    <row r="382" ht="14.25" customHeight="1"/>
-    <row r="383" ht="14.25" customHeight="1"/>
-    <row r="384" ht="14.25" customHeight="1"/>
-    <row r="385" ht="14.25" customHeight="1"/>
-    <row r="386" ht="14.25" customHeight="1"/>
-    <row r="387" ht="14.25" customHeight="1"/>
-    <row r="388" ht="14.25" customHeight="1"/>
-    <row r="389" ht="14.25" customHeight="1"/>
-    <row r="390" ht="14.25" customHeight="1"/>
-    <row r="391" ht="14.25" customHeight="1"/>
-    <row r="392" ht="14.25" customHeight="1"/>
-    <row r="393" ht="14.25" customHeight="1"/>
-    <row r="394" ht="14.25" customHeight="1"/>
-    <row r="395" ht="14.25" customHeight="1"/>
-    <row r="396" ht="14.25" customHeight="1"/>
-    <row r="397" ht="14.25" customHeight="1"/>
-    <row r="398" ht="14.25" customHeight="1"/>
-    <row r="399" ht="14.25" customHeight="1"/>
-    <row r="400" ht="14.25" customHeight="1"/>
-    <row r="401" ht="14.25" customHeight="1"/>
-    <row r="402" ht="14.25" customHeight="1"/>
-    <row r="403" ht="14.25" customHeight="1"/>
-    <row r="404" ht="14.25" customHeight="1"/>
-    <row r="405" ht="14.25" customHeight="1"/>
-    <row r="406" ht="14.25" customHeight="1"/>
-    <row r="407" ht="14.25" customHeight="1"/>
-    <row r="408" ht="14.25" customHeight="1"/>
-    <row r="409" ht="14.25" customHeight="1"/>
-    <row r="410" ht="14.25" customHeight="1"/>
-    <row r="411" ht="14.25" customHeight="1"/>
-    <row r="412" ht="14.25" customHeight="1"/>
-    <row r="413" ht="14.25" customHeight="1"/>
-    <row r="414" ht="14.25" customHeight="1"/>
-    <row r="415" ht="14.25" customHeight="1"/>
-    <row r="416" ht="14.25" customHeight="1"/>
-    <row r="417" ht="14.25" customHeight="1"/>
-    <row r="418" ht="14.25" customHeight="1"/>
-    <row r="419" ht="14.25" customHeight="1"/>
-    <row r="420" ht="14.25" customHeight="1"/>
-    <row r="421" ht="14.25" customHeight="1"/>
-    <row r="422" ht="14.25" customHeight="1"/>
-    <row r="423" ht="14.25" customHeight="1"/>
-    <row r="424" ht="14.25" customHeight="1"/>
-    <row r="425" ht="14.25" customHeight="1"/>
-    <row r="426" ht="14.25" customHeight="1"/>
-    <row r="427" ht="14.25" customHeight="1"/>
-    <row r="428" ht="14.25" customHeight="1"/>
-    <row r="429" ht="14.25" customHeight="1"/>
-    <row r="430" ht="14.25" customHeight="1"/>
-    <row r="431" ht="14.25" customHeight="1"/>
-    <row r="432" ht="14.25" customHeight="1"/>
-    <row r="433" ht="14.25" customHeight="1"/>
-    <row r="434" ht="14.25" customHeight="1"/>
-    <row r="435" ht="14.25" customHeight="1"/>
-    <row r="436" ht="14.25" customHeight="1"/>
-    <row r="437" ht="14.25" customHeight="1"/>
-    <row r="438" ht="14.25" customHeight="1"/>
-    <row r="439" ht="14.25" customHeight="1"/>
-    <row r="440" ht="14.25" customHeight="1"/>
-    <row r="441" ht="14.25" customHeight="1"/>
-    <row r="442" ht="14.25" customHeight="1"/>
-    <row r="443" ht="14.25" customHeight="1"/>
-    <row r="444" ht="14.25" customHeight="1"/>
-    <row r="445" ht="14.25" customHeight="1"/>
-    <row r="446" ht="14.25" customHeight="1"/>
-    <row r="447" ht="14.25" customHeight="1"/>
-    <row r="448" ht="14.25" customHeight="1"/>
-    <row r="449" ht="14.25" customHeight="1"/>
-    <row r="450" ht="14.25" customHeight="1"/>
-    <row r="451" ht="14.25" customHeight="1"/>
-    <row r="452" ht="14.25" customHeight="1"/>
-    <row r="453" ht="14.25" customHeight="1"/>
-    <row r="454" ht="14.25" customHeight="1"/>
-    <row r="455" ht="14.25" customHeight="1"/>
-    <row r="456" ht="14.25" customHeight="1"/>
-    <row r="457" ht="14.25" customHeight="1"/>
-    <row r="458" ht="14.25" customHeight="1"/>
-    <row r="459" ht="14.25" customHeight="1"/>
-    <row r="460" ht="14.25" customHeight="1"/>
-    <row r="461" ht="14.25" customHeight="1"/>
-    <row r="462" ht="14.25" customHeight="1"/>
-    <row r="463" ht="14.25" customHeight="1"/>
-    <row r="464" ht="14.25" customHeight="1"/>
-    <row r="465" ht="14.25" customHeight="1"/>
-    <row r="466" ht="14.25" customHeight="1"/>
-    <row r="467" ht="14.25" customHeight="1"/>
-    <row r="468" ht="14.25" customHeight="1"/>
-    <row r="469" ht="14.25" customHeight="1"/>
-    <row r="470" ht="14.25" customHeight="1"/>
-    <row r="471" ht="14.25" customHeight="1"/>
-    <row r="472" ht="14.25" customHeight="1"/>
-    <row r="473" ht="14.25" customHeight="1"/>
-    <row r="474" ht="14.25" customHeight="1"/>
-    <row r="475" ht="14.25" customHeight="1"/>
-    <row r="476" ht="14.25" customHeight="1"/>
-    <row r="477" ht="14.25" customHeight="1"/>
-    <row r="478" ht="14.25" customHeight="1"/>
-    <row r="479" ht="14.25" customHeight="1"/>
-    <row r="480" ht="14.25" customHeight="1"/>
-    <row r="481" ht="14.25" customHeight="1"/>
-    <row r="482" ht="14.25" customHeight="1"/>
-    <row r="483" ht="14.25" customHeight="1"/>
-    <row r="484" ht="14.25" customHeight="1"/>
-    <row r="485" ht="14.25" customHeight="1"/>
-    <row r="486" ht="14.25" customHeight="1"/>
-    <row r="487" ht="14.25" customHeight="1"/>
-    <row r="488" ht="14.25" customHeight="1"/>
-    <row r="489" ht="14.25" customHeight="1"/>
-    <row r="490" ht="14.25" customHeight="1"/>
-    <row r="491" ht="14.25" customHeight="1"/>
-    <row r="492" ht="14.25" customHeight="1"/>
-    <row r="493" ht="14.25" customHeight="1"/>
-    <row r="494" ht="14.25" customHeight="1"/>
-    <row r="495" ht="14.25" customHeight="1"/>
-    <row r="496" ht="14.25" customHeight="1"/>
-    <row r="497" ht="14.25" customHeight="1"/>
-    <row r="498" ht="14.25" customHeight="1"/>
-    <row r="499" ht="14.25" customHeight="1"/>
-    <row r="500" ht="14.25" customHeight="1"/>
-    <row r="501" ht="14.25" customHeight="1"/>
-    <row r="502" ht="14.25" customHeight="1"/>
-    <row r="503" ht="14.25" customHeight="1"/>
-    <row r="504" ht="14.25" customHeight="1"/>
-    <row r="505" ht="14.25" customHeight="1"/>
-    <row r="506" ht="14.25" customHeight="1"/>
-    <row r="507" ht="14.25" customHeight="1"/>
-    <row r="508" ht="14.25" customHeight="1"/>
-    <row r="509" ht="14.25" customHeight="1"/>
-    <row r="510" ht="14.25" customHeight="1"/>
-    <row r="511" ht="14.25" customHeight="1"/>
-    <row r="512" ht="14.25" customHeight="1"/>
-    <row r="513" ht="14.25" customHeight="1"/>
-    <row r="514" ht="14.25" customHeight="1"/>
-    <row r="515" ht="14.25" customHeight="1"/>
-    <row r="516" ht="14.25" customHeight="1"/>
-    <row r="517" ht="14.25" customHeight="1"/>
-    <row r="518" ht="14.25" customHeight="1"/>
-    <row r="519" ht="14.25" customHeight="1"/>
-    <row r="520" ht="14.25" customHeight="1"/>
-    <row r="521" ht="14.25" customHeight="1"/>
-    <row r="522" ht="14.25" customHeight="1"/>
-    <row r="523" ht="14.25" customHeight="1"/>
-    <row r="524" ht="14.25" customHeight="1"/>
-    <row r="525" ht="14.25" customHeight="1"/>
-    <row r="526" ht="14.25" customHeight="1"/>
-    <row r="527" ht="14.25" customHeight="1"/>
-    <row r="528" ht="14.25" customHeight="1"/>
-    <row r="529" ht="14.25" customHeight="1"/>
-    <row r="530" ht="14.25" customHeight="1"/>
-    <row r="531" ht="14.25" customHeight="1"/>
-    <row r="532" ht="14.25" customHeight="1"/>
-    <row r="533" ht="14.25" customHeight="1"/>
-    <row r="534" ht="14.25" customHeight="1"/>
-    <row r="535" ht="14.25" customHeight="1"/>
-    <row r="536" ht="14.25" customHeight="1"/>
-    <row r="537" ht="14.25" customHeight="1"/>
-    <row r="538" ht="14.25" customHeight="1"/>
-    <row r="539" ht="14.25" customHeight="1"/>
-    <row r="540" ht="14.25" customHeight="1"/>
-    <row r="541" ht="14.25" customHeight="1"/>
-    <row r="542" ht="14.25" customHeight="1"/>
-    <row r="543" ht="14.25" customHeight="1"/>
-    <row r="544" ht="14.25" customHeight="1"/>
-    <row r="545" ht="14.25" customHeight="1"/>
-    <row r="546" ht="14.25" customHeight="1"/>
-    <row r="547" ht="14.25" customHeight="1"/>
-    <row r="548" ht="14.25" customHeight="1"/>
-    <row r="549" ht="14.25" customHeight="1"/>
-    <row r="550" ht="14.25" customHeight="1"/>
-    <row r="551" ht="14.25" customHeight="1"/>
-    <row r="552" ht="14.25" customHeight="1"/>
-    <row r="553" ht="14.25" customHeight="1"/>
-    <row r="554" ht="14.25" customHeight="1"/>
-    <row r="555" ht="14.25" customHeight="1"/>
-    <row r="556" ht="14.25" customHeight="1"/>
-    <row r="557" ht="14.25" customHeight="1"/>
-    <row r="558" ht="14.25" customHeight="1"/>
-    <row r="559" ht="14.25" customHeight="1"/>
-    <row r="560" ht="14.25" customHeight="1"/>
-    <row r="561" ht="14.25" customHeight="1"/>
-    <row r="562" ht="14.25" customHeight="1"/>
-    <row r="563" ht="14.25" customHeight="1"/>
-    <row r="564" ht="14.25" customHeight="1"/>
-    <row r="565" ht="14.25" customHeight="1"/>
-    <row r="566" ht="14.25" customHeight="1"/>
-    <row r="567" ht="14.25" customHeight="1"/>
-    <row r="568" ht="14.25" customHeight="1"/>
-    <row r="569" ht="14.25" customHeight="1"/>
-    <row r="570" ht="14.25" customHeight="1"/>
-    <row r="571" ht="14.25" customHeight="1"/>
-    <row r="572" ht="14.25" customHeight="1"/>
-    <row r="573" ht="14.25" customHeight="1"/>
-    <row r="574" ht="14.25" customHeight="1"/>
-    <row r="575" ht="14.25" customHeight="1"/>
-    <row r="576" ht="14.25" customHeight="1"/>
-    <row r="577" ht="14.25" customHeight="1"/>
-    <row r="578" ht="14.25" customHeight="1"/>
-    <row r="579" ht="14.25" customHeight="1"/>
-    <row r="580" ht="14.25" customHeight="1"/>
-    <row r="581" ht="14.25" customHeight="1"/>
-    <row r="582" ht="14.25" customHeight="1"/>
-    <row r="583" ht="14.25" customHeight="1"/>
-    <row r="584" ht="14.25" customHeight="1"/>
-    <row r="585" ht="14.25" customHeight="1"/>
-    <row r="586" ht="14.25" customHeight="1"/>
-    <row r="587" ht="14.25" customHeight="1"/>
-    <row r="588" ht="14.25" customHeight="1"/>
-    <row r="589" ht="14.25" customHeight="1"/>
-    <row r="590" ht="14.25" customHeight="1"/>
-    <row r="591" ht="14.25" customHeight="1"/>
-    <row r="592" ht="14.25" customHeight="1"/>
-    <row r="593" ht="14.25" customHeight="1"/>
-    <row r="594" ht="14.25" customHeight="1"/>
-    <row r="595" ht="14.25" customHeight="1"/>
-    <row r="596" ht="14.25" customHeight="1"/>
-    <row r="597" ht="14.25" customHeight="1"/>
-    <row r="598" ht="14.25" customHeight="1"/>
-    <row r="599" ht="14.25" customHeight="1"/>
-    <row r="600" ht="14.25" customHeight="1"/>
-    <row r="601" ht="14.25" customHeight="1"/>
-    <row r="602" ht="14.25" customHeight="1"/>
-    <row r="603" ht="14.25" customHeight="1"/>
-    <row r="604" ht="14.25" customHeight="1"/>
-    <row r="605" ht="14.25" customHeight="1"/>
-    <row r="606" ht="14.25" customHeight="1"/>
-    <row r="607" ht="14.25" customHeight="1"/>
-    <row r="608" ht="14.25" customHeight="1"/>
-    <row r="609" ht="14.25" customHeight="1"/>
-    <row r="610" ht="14.25" customHeight="1"/>
-    <row r="611" ht="14.25" customHeight="1"/>
-    <row r="612" ht="14.25" customHeight="1"/>
-    <row r="613" ht="14.25" customHeight="1"/>
-    <row r="614" ht="14.25" customHeight="1"/>
-    <row r="615" ht="14.25" customHeight="1"/>
-    <row r="616" ht="14.25" customHeight="1"/>
-    <row r="617" ht="14.25" customHeight="1"/>
-    <row r="618" ht="14.25" customHeight="1"/>
-    <row r="619" ht="14.25" customHeight="1"/>
-    <row r="620" ht="14.25" customHeight="1"/>
-    <row r="621" ht="14.25" customHeight="1"/>
-    <row r="622" ht="14.25" customHeight="1"/>
-    <row r="623" ht="14.25" customHeight="1"/>
-    <row r="624" ht="14.25" customHeight="1"/>
-    <row r="625" ht="14.25" customHeight="1"/>
-    <row r="626" ht="14.25" customHeight="1"/>
-    <row r="627" ht="14.25" customHeight="1"/>
-    <row r="628" ht="14.25" customHeight="1"/>
-    <row r="629" ht="14.25" customHeight="1"/>
-    <row r="630" ht="14.25" customHeight="1"/>
-    <row r="631" ht="14.25" customHeight="1"/>
-    <row r="632" ht="14.25" customHeight="1"/>
-    <row r="633" ht="14.25" customHeight="1"/>
-    <row r="634" ht="14.25" customHeight="1"/>
-    <row r="635" ht="14.25" customHeight="1"/>
-    <row r="636" ht="14.25" customHeight="1"/>
-    <row r="637" ht="14.25" customHeight="1"/>
-    <row r="638" ht="14.25" customHeight="1"/>
-    <row r="639" ht="14.25" customHeight="1"/>
-    <row r="640" ht="14.25" customHeight="1"/>
-    <row r="641" ht="14.25" customHeight="1"/>
-    <row r="642" ht="14.25" customHeight="1"/>
-    <row r="643" ht="14.25" customHeight="1"/>
-    <row r="644" ht="14.25" customHeight="1"/>
-    <row r="645" ht="14.25" customHeight="1"/>
-    <row r="646" ht="14.25" customHeight="1"/>
-    <row r="647" ht="14.25" customHeight="1"/>
-    <row r="648" ht="14.25" customHeight="1"/>
-    <row r="649" ht="14.25" customHeight="1"/>
-    <row r="650" ht="14.25" customHeight="1"/>
-    <row r="651" ht="14.25" customHeight="1"/>
-    <row r="652" ht="14.25" customHeight="1"/>
-    <row r="653" ht="14.25" customHeight="1"/>
-    <row r="654" ht="14.25" customHeight="1"/>
-    <row r="655" ht="14.25" customHeight="1"/>
-    <row r="656" ht="14.25" customHeight="1"/>
-    <row r="657" ht="14.25" customHeight="1"/>
-    <row r="658" ht="14.25" customHeight="1"/>
-    <row r="659" ht="14.25" customHeight="1"/>
-    <row r="660" ht="14.25" customHeight="1"/>
-    <row r="661" ht="14.25" customHeight="1"/>
-    <row r="662" ht="14.25" customHeight="1"/>
-    <row r="663" ht="14.25" customHeight="1"/>
-    <row r="664" ht="14.25" customHeight="1"/>
-    <row r="665" ht="14.25" customHeight="1"/>
-    <row r="666" ht="14.25" customHeight="1"/>
-    <row r="667" ht="14.25" customHeight="1"/>
-    <row r="668" ht="14.25" customHeight="1"/>
-    <row r="669" ht="14.25" customHeight="1"/>
-    <row r="670" ht="14.25" customHeight="1"/>
-    <row r="671" ht="14.25" customHeight="1"/>
-    <row r="672" ht="14.25" customHeight="1"/>
-    <row r="673" ht="14.25" customHeight="1"/>
-    <row r="674" ht="14.25" customHeight="1"/>
-    <row r="675" ht="14.25" customHeight="1"/>
-    <row r="676" ht="14.25" customHeight="1"/>
-    <row r="677" ht="14.25" customHeight="1"/>
-    <row r="678" ht="14.25" customHeight="1"/>
-    <row r="679" ht="14.25" customHeight="1"/>
-    <row r="680" ht="14.25" customHeight="1"/>
-    <row r="681" ht="14.25" customHeight="1"/>
-    <row r="682" ht="14.25" customHeight="1"/>
-    <row r="683" ht="14.25" customHeight="1"/>
-    <row r="684" ht="14.25" customHeight="1"/>
-    <row r="685" ht="14.25" customHeight="1"/>
-    <row r="686" ht="14.25" customHeight="1"/>
-    <row r="687" ht="14.25" customHeight="1"/>
-    <row r="688" ht="14.25" customHeight="1"/>
-    <row r="689" ht="14.25" customHeight="1"/>
-    <row r="690" ht="14.25" customHeight="1"/>
-    <row r="691" ht="14.25" customHeight="1"/>
-    <row r="692" ht="14.25" customHeight="1"/>
-    <row r="693" ht="14.25" customHeight="1"/>
-    <row r="694" ht="14.25" customHeight="1"/>
-    <row r="695" ht="14.25" customHeight="1"/>
-    <row r="696" ht="14.25" customHeight="1"/>
-    <row r="697" ht="14.25" customHeight="1"/>
-    <row r="698" ht="14.25" customHeight="1"/>
-    <row r="699" ht="14.25" customHeight="1"/>
-    <row r="700" ht="14.25" customHeight="1"/>
-    <row r="701" ht="14.25" customHeight="1"/>
-    <row r="702" ht="14.25" customHeight="1"/>
-    <row r="703" ht="14.25" customHeight="1"/>
-    <row r="704" ht="14.25" customHeight="1"/>
-    <row r="705" ht="14.25" customHeight="1"/>
-    <row r="706" ht="14.25" customHeight="1"/>
-    <row r="707" ht="14.25" customHeight="1"/>
-    <row r="708" ht="14.25" customHeight="1"/>
-    <row r="709" ht="14.25" customHeight="1"/>
-    <row r="710" ht="14.25" customHeight="1"/>
-    <row r="711" ht="14.25" customHeight="1"/>
-    <row r="712" ht="14.25" customHeight="1"/>
-    <row r="713" ht="14.25" customHeight="1"/>
-    <row r="714" ht="14.25" customHeight="1"/>
-    <row r="715" ht="14.25" customHeight="1"/>
-    <row r="716" ht="14.25" customHeight="1"/>
-    <row r="717" ht="14.25" customHeight="1"/>
-    <row r="718" ht="14.25" customHeight="1"/>
-    <row r="719" ht="14.25" customHeight="1"/>
-    <row r="720" ht="14.25" customHeight="1"/>
-    <row r="721" ht="14.25" customHeight="1"/>
-    <row r="722" ht="14.25" customHeight="1"/>
-    <row r="723" ht="14.25" customHeight="1"/>
-    <row r="724" ht="14.25" customHeight="1"/>
-    <row r="725" ht="14.25" customHeight="1"/>
-    <row r="726" ht="14.25" customHeight="1"/>
-    <row r="727" ht="14.25" customHeight="1"/>
-    <row r="728" ht="14.25" customHeight="1"/>
-    <row r="729" ht="14.25" customHeight="1"/>
-    <row r="730" ht="14.25" customHeight="1"/>
-    <row r="731" ht="14.25" customHeight="1"/>
-    <row r="732" ht="14.25" customHeight="1"/>
-    <row r="733" ht="14.25" customHeight="1"/>
-    <row r="734" ht="14.25" customHeight="1"/>
-    <row r="735" ht="14.25" customHeight="1"/>
-    <row r="736" ht="14.25" customHeight="1"/>
-    <row r="737" ht="14.25" customHeight="1"/>
-    <row r="738" ht="14.25" customHeight="1"/>
-    <row r="739" ht="14.25" customHeight="1"/>
-    <row r="740" ht="14.25" customHeight="1"/>
-    <row r="741" ht="14.25" customHeight="1"/>
-    <row r="742" ht="14.25" customHeight="1"/>
-    <row r="743" ht="14.25" customHeight="1"/>
-    <row r="744" ht="14.25" customHeight="1"/>
-    <row r="745" ht="14.25" customHeight="1"/>
-    <row r="746" ht="14.25" customHeight="1"/>
-    <row r="747" ht="14.25" customHeight="1"/>
-    <row r="748" ht="14.25" customHeight="1"/>
-    <row r="749" ht="14.25" customHeight="1"/>
-    <row r="750" ht="14.25" customHeight="1"/>
-    <row r="751" ht="14.25" customHeight="1"/>
-    <row r="752" ht="14.25" customHeight="1"/>
-    <row r="753" ht="14.25" customHeight="1"/>
-    <row r="754" ht="14.25" customHeight="1"/>
-    <row r="755" ht="14.25" customHeight="1"/>
-    <row r="756" ht="14.25" customHeight="1"/>
-    <row r="757" ht="14.25" customHeight="1"/>
-    <row r="758" ht="14.25" customHeight="1"/>
-    <row r="759" ht="14.25" customHeight="1"/>
-    <row r="760" ht="14.25" customHeight="1"/>
-    <row r="761" ht="14.25" customHeight="1"/>
-    <row r="762" ht="14.25" customHeight="1"/>
-    <row r="763" ht="14.25" customHeight="1"/>
-    <row r="764" ht="14.25" customHeight="1"/>
-    <row r="765" ht="14.25" customHeight="1"/>
-    <row r="766" ht="14.25" customHeight="1"/>
-    <row r="767" ht="14.25" customHeight="1"/>
-    <row r="768" ht="14.25" customHeight="1"/>
-    <row r="769" ht="14.25" customHeight="1"/>
-    <row r="770" ht="14.25" customHeight="1"/>
-    <row r="771" ht="14.25" customHeight="1"/>
-    <row r="772" ht="14.25" customHeight="1"/>
-    <row r="773" ht="14.25" customHeight="1"/>
-    <row r="774" ht="14.25" customHeight="1"/>
-    <row r="775" ht="14.25" customHeight="1"/>
-    <row r="776" ht="14.25" customHeight="1"/>
-    <row r="777" ht="14.25" customHeight="1"/>
-    <row r="778" ht="14.25" customHeight="1"/>
-    <row r="779" ht="14.25" customHeight="1"/>
-    <row r="780" ht="14.25" customHeight="1"/>
-    <row r="781" ht="14.25" customHeight="1"/>
-    <row r="782" ht="14.25" customHeight="1"/>
-    <row r="783" ht="14.25" customHeight="1"/>
-    <row r="784" ht="14.25" customHeight="1"/>
-    <row r="785" ht="14.25" customHeight="1"/>
-    <row r="786" ht="14.25" customHeight="1"/>
-    <row r="787" ht="14.25" customHeight="1"/>
-    <row r="788" ht="14.25" customHeight="1"/>
-    <row r="789" ht="14.25" customHeight="1"/>
-    <row r="790" ht="14.25" customHeight="1"/>
-    <row r="791" ht="14.25" customHeight="1"/>
-    <row r="792" ht="14.25" customHeight="1"/>
-    <row r="793" ht="14.25" customHeight="1"/>
-    <row r="794" ht="14.25" customHeight="1"/>
-    <row r="795" ht="14.25" customHeight="1"/>
-    <row r="796" ht="14.25" customHeight="1"/>
-    <row r="797" ht="14.25" customHeight="1"/>
-    <row r="798" ht="14.25" customHeight="1"/>
-    <row r="799" ht="14.25" customHeight="1"/>
-    <row r="800" ht="14.25" customHeight="1"/>
-    <row r="801" ht="14.25" customHeight="1"/>
-    <row r="802" ht="14.25" customHeight="1"/>
-    <row r="803" ht="14.25" customHeight="1"/>
-    <row r="804" ht="14.25" customHeight="1"/>
-    <row r="805" ht="14.25" customHeight="1"/>
-    <row r="806" ht="14.25" customHeight="1"/>
-    <row r="807" ht="14.25" customHeight="1"/>
-    <row r="808" ht="14.25" customHeight="1"/>
-    <row r="809" ht="14.25" customHeight="1"/>
-    <row r="810" ht="14.25" customHeight="1"/>
-    <row r="811" ht="14.25" customHeight="1"/>
-    <row r="812" ht="14.25" customHeight="1"/>
-    <row r="813" ht="14.25" customHeight="1"/>
-    <row r="814" ht="14.25" customHeight="1"/>
-    <row r="815" ht="14.25" customHeight="1"/>
-    <row r="816" ht="14.25" customHeight="1"/>
-    <row r="817" ht="14.25" customHeight="1"/>
-    <row r="818" ht="14.25" customHeight="1"/>
-    <row r="819" ht="14.25" customHeight="1"/>
-    <row r="820" ht="14.25" customHeight="1"/>
-    <row r="821" ht="14.25" customHeight="1"/>
-    <row r="822" ht="14.25" customHeight="1"/>
-    <row r="823" ht="14.25" customHeight="1"/>
-    <row r="824" ht="14.25" customHeight="1"/>
-    <row r="825" ht="14.25" customHeight="1"/>
-    <row r="826" ht="14.25" customHeight="1"/>
-    <row r="827" ht="14.25" customHeight="1"/>
-    <row r="828" ht="14.25" customHeight="1"/>
-    <row r="829" ht="14.25" customHeight="1"/>
-    <row r="830" ht="14.25" customHeight="1"/>
-    <row r="831" ht="14.25" customHeight="1"/>
-    <row r="832" ht="14.25" customHeight="1"/>
-    <row r="833" ht="14.25" customHeight="1"/>
-    <row r="834" ht="14.25" customHeight="1"/>
-    <row r="835" ht="14.25" customHeight="1"/>
-    <row r="836" ht="14.25" customHeight="1"/>
-    <row r="837" ht="14.25" customHeight="1"/>
-    <row r="838" ht="14.25" customHeight="1"/>
-    <row r="839" ht="14.25" customHeight="1"/>
-    <row r="840" ht="14.25" customHeight="1"/>
-    <row r="841" ht="14.25" customHeight="1"/>
-    <row r="842" ht="14.25" customHeight="1"/>
-    <row r="843" ht="14.25" customHeight="1"/>
-    <row r="844" ht="14.25" customHeight="1"/>
-    <row r="845" ht="14.25" customHeight="1"/>
-    <row r="846" ht="14.25" customHeight="1"/>
-    <row r="847" ht="14.25" customHeight="1"/>
-    <row r="848" ht="14.25" customHeight="1"/>
-    <row r="849" ht="14.25" customHeight="1"/>
-    <row r="850" ht="14.25" customHeight="1"/>
-    <row r="851" ht="14.25" customHeight="1"/>
-    <row r="852" ht="14.25" customHeight="1"/>
-    <row r="853" ht="14.25" customHeight="1"/>
-    <row r="854" ht="14.25" customHeight="1"/>
-    <row r="855" ht="14.25" customHeight="1"/>
-    <row r="856" ht="14.25" customHeight="1"/>
-    <row r="857" ht="14.25" customHeight="1"/>
-    <row r="858" ht="14.25" customHeight="1"/>
-    <row r="859" ht="14.25" customHeight="1"/>
-    <row r="860" ht="14.25" customHeight="1"/>
-    <row r="861" ht="14.25" customHeight="1"/>
-    <row r="862" ht="14.25" customHeight="1"/>
-    <row r="863" ht="14.25" customHeight="1"/>
-    <row r="864" ht="14.25" customHeight="1"/>
-    <row r="865" ht="14.25" customHeight="1"/>
-    <row r="866" ht="14.25" customHeight="1"/>
-    <row r="867" ht="14.25" customHeight="1"/>
-    <row r="868" ht="14.25" customHeight="1"/>
-    <row r="869" ht="14.25" customHeight="1"/>
-    <row r="870" ht="14.25" customHeight="1"/>
-    <row r="871" ht="14.25" customHeight="1"/>
-    <row r="872" ht="14.25" customHeight="1"/>
-    <row r="873" ht="14.25" customHeight="1"/>
-    <row r="874" ht="14.25" customHeight="1"/>
-    <row r="875" ht="14.25" customHeight="1"/>
-    <row r="876" ht="14.25" customHeight="1"/>
-    <row r="877" ht="14.25" customHeight="1"/>
-    <row r="878" ht="14.25" customHeight="1"/>
-    <row r="879" ht="14.25" customHeight="1"/>
-    <row r="880" ht="14.25" customHeight="1"/>
-    <row r="881" ht="14.25" customHeight="1"/>
-    <row r="882" ht="14.25" customHeight="1"/>
-    <row r="883" ht="14.25" customHeight="1"/>
-    <row r="884" ht="14.25" customHeight="1"/>
-    <row r="885" ht="14.25" customHeight="1"/>
-    <row r="886" ht="14.25" customHeight="1"/>
-    <row r="887" ht="14.25" customHeight="1"/>
-    <row r="888" ht="14.25" customHeight="1"/>
-    <row r="889" ht="14.25" customHeight="1"/>
-    <row r="890" ht="14.25" customHeight="1"/>
-    <row r="891" ht="14.25" customHeight="1"/>
-    <row r="892" ht="14.25" customHeight="1"/>
-    <row r="893" ht="14.25" customHeight="1"/>
-    <row r="894" ht="14.25" customHeight="1"/>
-    <row r="895" ht="14.25" customHeight="1"/>
-    <row r="896" ht="14.25" customHeight="1"/>
-    <row r="897" ht="14.25" customHeight="1"/>
-    <row r="898" ht="14.25" customHeight="1"/>
-    <row r="899" ht="14.25" customHeight="1"/>
-    <row r="900" ht="14.25" customHeight="1"/>
-    <row r="901" ht="14.25" customHeight="1"/>
-    <row r="902" ht="14.25" customHeight="1"/>
-    <row r="903" ht="14.25" customHeight="1"/>
-    <row r="904" ht="14.25" customHeight="1"/>
-    <row r="905" ht="14.25" customHeight="1"/>
-    <row r="906" ht="14.25" customHeight="1"/>
-    <row r="907" ht="14.25" customHeight="1"/>
-    <row r="908" ht="14.25" customHeight="1"/>
-    <row r="909" ht="14.25" customHeight="1"/>
-    <row r="910" ht="14.25" customHeight="1"/>
-    <row r="911" ht="14.25" customHeight="1"/>
-    <row r="912" ht="14.25" customHeight="1"/>
-    <row r="913" ht="14.25" customHeight="1"/>
-    <row r="914" ht="14.25" customHeight="1"/>
-    <row r="915" ht="14.25" customHeight="1"/>
-    <row r="916" ht="14.25" customHeight="1"/>
-    <row r="917" ht="14.25" customHeight="1"/>
-    <row r="918" ht="14.25" customHeight="1"/>
-    <row r="919" ht="14.25" customHeight="1"/>
-    <row r="920" ht="14.25" customHeight="1"/>
-    <row r="921" ht="14.25" customHeight="1"/>
-    <row r="922" ht="14.25" customHeight="1"/>
-    <row r="923" ht="14.25" customHeight="1"/>
-    <row r="924" ht="14.25" customHeight="1"/>
-    <row r="925" ht="14.25" customHeight="1"/>
-    <row r="926" ht="14.25" customHeight="1"/>
-    <row r="927" ht="14.25" customHeight="1"/>
-    <row r="928" ht="14.25" customHeight="1"/>
-    <row r="929" ht="14.25" customHeight="1"/>
-    <row r="930" ht="14.25" customHeight="1"/>
-    <row r="931" ht="14.25" customHeight="1"/>
-    <row r="932" ht="14.25" customHeight="1"/>
-    <row r="933" ht="14.25" customHeight="1"/>
-    <row r="934" ht="14.25" customHeight="1"/>
-    <row r="935" ht="14.25" customHeight="1"/>
-    <row r="936" ht="14.25" customHeight="1"/>
-    <row r="937" ht="14.25" customHeight="1"/>
-    <row r="938" ht="14.25" customHeight="1"/>
-    <row r="939" ht="14.25" customHeight="1"/>
-    <row r="940" ht="14.25" customHeight="1"/>
-    <row r="941" ht="14.25" customHeight="1"/>
-    <row r="942" ht="14.25" customHeight="1"/>
-    <row r="943" ht="14.25" customHeight="1"/>
-    <row r="944" ht="14.25" customHeight="1"/>
-    <row r="945" ht="14.25" customHeight="1"/>
-    <row r="946" ht="14.25" customHeight="1"/>
-    <row r="947" ht="14.25" customHeight="1"/>
-    <row r="948" ht="14.25" customHeight="1"/>
-    <row r="949" ht="14.25" customHeight="1"/>
-    <row r="950" ht="14.25" customHeight="1"/>
-    <row r="951" ht="14.25" customHeight="1"/>
-    <row r="952" ht="14.25" customHeight="1"/>
-    <row r="953" ht="14.25" customHeight="1"/>
-    <row r="954" ht="14.25" customHeight="1"/>
-    <row r="955" ht="14.25" customHeight="1"/>
-    <row r="956" ht="14.25" customHeight="1"/>
-    <row r="957" ht="14.25" customHeight="1"/>
-    <row r="958" ht="14.25" customHeight="1"/>
-    <row r="959" ht="14.25" customHeight="1"/>
-    <row r="960" ht="14.25" customHeight="1"/>
-    <row r="961" ht="14.25" customHeight="1"/>
-    <row r="962" ht="14.25" customHeight="1"/>
-    <row r="963" ht="14.25" customHeight="1"/>
-    <row r="964" ht="14.25" customHeight="1"/>
-    <row r="965" ht="14.25" customHeight="1"/>
-    <row r="966" ht="14.25" customHeight="1"/>
-    <row r="967" ht="14.25" customHeight="1"/>
-    <row r="968" ht="14.25" customHeight="1"/>
-    <row r="969" ht="14.25" customHeight="1"/>
-    <row r="970" ht="14.25" customHeight="1"/>
-    <row r="971" ht="14.25" customHeight="1"/>
-    <row r="972" ht="14.25" customHeight="1"/>
-    <row r="973" ht="14.25" customHeight="1"/>
-    <row r="974" ht="14.25" customHeight="1"/>
-    <row r="975" ht="14.25" customHeight="1"/>
-    <row r="976" ht="14.25" customHeight="1"/>
-    <row r="977" ht="14.25" customHeight="1"/>
-    <row r="978" ht="14.25" customHeight="1"/>
-    <row r="979" ht="14.25" customHeight="1"/>
-    <row r="980" ht="14.25" customHeight="1"/>
-    <row r="981" ht="14.25" customHeight="1"/>
-    <row r="982" ht="14.25" customHeight="1"/>
-    <row r="983" ht="14.25" customHeight="1"/>
-    <row r="984" ht="14.25" customHeight="1"/>
-    <row r="985" ht="14.25" customHeight="1"/>
-    <row r="986" ht="14.25" customHeight="1"/>
-    <row r="987" ht="14.25" customHeight="1"/>
-    <row r="988" ht="14.25" customHeight="1"/>
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>392</v>
+      </c>
+      <c r="B18" t="s">
+        <v>393</v>
+      </c>
+    </row>
   </sheetData>
-  <phoneticPr fontId="20"/>
+  <phoneticPr fontId="21"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:Z23"/>
+  <dimension ref="A1:Z25"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="14.5"/>
@@ -3627,7 +2720,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>27</v>
@@ -3660,16 +2753,17 @@
     </row>
     <row r="2" spans="1:26">
       <c r="A2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B2" t="s">
-        <v>227</v>
-      </c>
-      <c r="C2" t="s">
-        <v>371</v>
+        <v>226</v>
+      </c>
+      <c r="C2" t="str">
+        <f>_xlfn.CONCAT(Constants!$B$18,"/P002_090_PayCycleAfternoon")</f>
+        <v>PROD/P002_090_PayCycleAfternoon</v>
       </c>
       <c r="D2" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
     <row r="3" spans="1:26">
@@ -3677,21 +2771,23 @@
         <v>41</v>
       </c>
       <c r="B3" t="s">
-        <v>325</v>
-      </c>
-      <c r="C3" t="s">
-        <v>371</v>
+        <v>324</v>
+      </c>
+      <c r="C3" t="str">
+        <f>_xlfn.CONCAT(Constants!$B$18,"/P002_090_PayCycleAfternoon")</f>
+        <v>PROD/P002_090_PayCycleAfternoon</v>
       </c>
     </row>
     <row r="4" spans="1:26">
       <c r="A4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B4" t="s">
-        <v>326</v>
-      </c>
-      <c r="C4" t="s">
-        <v>371</v>
+        <v>325</v>
+      </c>
+      <c r="C4" t="str">
+        <f>_xlfn.CONCAT(Constants!$B$18,"/P002_090_PayCycleAfternoon")</f>
+        <v>PROD/P002_090_PayCycleAfternoon</v>
       </c>
     </row>
     <row r="5" spans="1:26">
@@ -3699,10 +2795,11 @@
         <v>44</v>
       </c>
       <c r="B5" t="s">
-        <v>327</v>
-      </c>
-      <c r="C5" t="s">
-        <v>371</v>
+        <v>326</v>
+      </c>
+      <c r="C5" t="str">
+        <f>_xlfn.CONCAT(Constants!$B$18,"/P002_090_PayCycleAfternoon")</f>
+        <v>PROD/P002_090_PayCycleAfternoon</v>
       </c>
     </row>
     <row r="6" spans="1:26">
@@ -3710,10 +2807,11 @@
         <v>45</v>
       </c>
       <c r="B6" t="s">
-        <v>328</v>
-      </c>
-      <c r="C6" t="s">
-        <v>371</v>
+        <v>327</v>
+      </c>
+      <c r="C6" t="str">
+        <f>_xlfn.CONCAT(Constants!$B$18,"/P002_090_PayCycleAfternoon")</f>
+        <v>PROD/P002_090_PayCycleAfternoon</v>
       </c>
     </row>
     <row r="7" spans="1:26">
@@ -3721,10 +2819,11 @@
         <v>46</v>
       </c>
       <c r="B7" t="s">
-        <v>329</v>
-      </c>
-      <c r="C7" t="s">
-        <v>371</v>
+        <v>328</v>
+      </c>
+      <c r="C7" t="str">
+        <f>_xlfn.CONCAT(Constants!$B$18,"/P002_090_PayCycleAfternoon")</f>
+        <v>PROD/P002_090_PayCycleAfternoon</v>
       </c>
     </row>
     <row r="8" spans="1:26">
@@ -3732,10 +2831,11 @@
         <v>47</v>
       </c>
       <c r="B8" t="s">
-        <v>330</v>
-      </c>
-      <c r="C8" t="s">
-        <v>371</v>
+        <v>329</v>
+      </c>
+      <c r="C8" t="str">
+        <f>_xlfn.CONCAT(Constants!$B$18,"/P002_090_PayCycleAfternoon")</f>
+        <v>PROD/P002_090_PayCycleAfternoon</v>
       </c>
     </row>
     <row r="9" spans="1:26">
@@ -3743,178 +2843,217 @@
         <v>124</v>
       </c>
       <c r="B9" t="s">
-        <v>331</v>
-      </c>
-      <c r="C9" t="s">
-        <v>371</v>
+        <v>330</v>
+      </c>
+      <c r="C9" t="str">
+        <f>_xlfn.CONCAT(Constants!$B$18,"/P002_090_PayCycleAfternoon")</f>
+        <v>PROD/P002_090_PayCycleAfternoon</v>
       </c>
     </row>
     <row r="10" spans="1:26">
       <c r="A10" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B10" t="s">
-        <v>332</v>
-      </c>
-      <c r="C10" t="s">
-        <v>371</v>
+        <v>331</v>
+      </c>
+      <c r="C10" t="str">
+        <f>_xlfn.CONCAT(Constants!$B$18,"/P002_090_PayCycleAfternoon")</f>
+        <v>PROD/P002_090_PayCycleAfternoon</v>
       </c>
     </row>
     <row r="11" spans="1:26">
       <c r="A11" s="19" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B11" t="s">
-        <v>333</v>
-      </c>
-      <c r="C11" t="s">
-        <v>371</v>
+        <v>332</v>
+      </c>
+      <c r="C11" t="str">
+        <f>_xlfn.CONCAT(Constants!$B$18,"/P002_090_PayCycleAfternoon")</f>
+        <v>PROD/P002_090_PayCycleAfternoon</v>
       </c>
     </row>
     <row r="12" spans="1:26">
       <c r="A12" s="19" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B12" t="s">
-        <v>334</v>
-      </c>
-      <c r="C12" t="s">
-        <v>371</v>
+        <v>333</v>
+      </c>
+      <c r="C12" t="str">
+        <f>_xlfn.CONCAT(Constants!$B$18,"/P002_090_PayCycleAfternoon")</f>
+        <v>PROD/P002_090_PayCycleAfternoon</v>
       </c>
     </row>
     <row r="13" spans="1:26">
       <c r="A13" s="19" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B13" t="s">
-        <v>335</v>
-      </c>
-      <c r="C13" t="s">
-        <v>371</v>
+        <v>334</v>
+      </c>
+      <c r="C13" t="str">
+        <f>_xlfn.CONCAT(Constants!$B$18,"/P002_090_PayCycleAfternoon")</f>
+        <v>PROD/P002_090_PayCycleAfternoon</v>
       </c>
     </row>
     <row r="14" spans="1:26">
       <c r="A14" s="19" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B14" t="s">
-        <v>336</v>
-      </c>
-      <c r="C14" t="s">
-        <v>371</v>
+        <v>335</v>
+      </c>
+      <c r="C14" t="str">
+        <f>_xlfn.CONCAT(Constants!$B$18,"/P002_090_PayCycleAfternoon")</f>
+        <v>PROD/P002_090_PayCycleAfternoon</v>
       </c>
     </row>
     <row r="15" spans="1:26">
       <c r="A15" s="19" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B15" t="s">
-        <v>337</v>
-      </c>
-      <c r="C15" t="s">
-        <v>371</v>
+        <v>336</v>
+      </c>
+      <c r="C15" t="str">
+        <f>_xlfn.CONCAT(Constants!$B$18,"/P002_090_PayCycleAfternoon")</f>
+        <v>PROD/P002_090_PayCycleAfternoon</v>
       </c>
     </row>
     <row r="16" spans="1:26">
       <c r="A16" s="19" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B16" t="s">
-        <v>338</v>
-      </c>
-      <c r="C16" t="s">
-        <v>371</v>
+        <v>337</v>
+      </c>
+      <c r="C16" t="str">
+        <f>_xlfn.CONCAT(Constants!$B$18,"/P002_090_PayCycleAfternoon")</f>
+        <v>PROD/P002_090_PayCycleAfternoon</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="19" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B17" t="s">
-        <v>339</v>
-      </c>
-      <c r="C17" t="s">
-        <v>371</v>
+        <v>338</v>
+      </c>
+      <c r="C17" t="str">
+        <f>_xlfn.CONCAT(Constants!$B$18,"/P002_090_PayCycleAfternoon")</f>
+        <v>PROD/P002_090_PayCycleAfternoon</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="19" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B18" t="s">
-        <v>340</v>
-      </c>
-      <c r="C18" t="s">
-        <v>371</v>
+        <v>339</v>
+      </c>
+      <c r="C18" t="str">
+        <f>_xlfn.CONCAT(Constants!$B$18,"/P002_090_PayCycleAfternoon")</f>
+        <v>PROD/P002_090_PayCycleAfternoon</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="19" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B19" t="s">
-        <v>341</v>
-      </c>
-      <c r="C19" t="s">
-        <v>371</v>
+        <v>340</v>
+      </c>
+      <c r="C19" t="str">
+        <f>_xlfn.CONCAT(Constants!$B$18,"/P002_090_PayCycleAfternoon")</f>
+        <v>PROD/P002_090_PayCycleAfternoon</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="19" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B20" t="s">
-        <v>342</v>
-      </c>
-      <c r="C20" t="s">
-        <v>371</v>
+        <v>341</v>
+      </c>
+      <c r="C20" t="str">
+        <f>_xlfn.CONCAT(Constants!$B$18,"/P002_090_PayCycleAfternoon")</f>
+        <v>PROD/P002_090_PayCycleAfternoon</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="19" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B21" t="s">
-        <v>347</v>
-      </c>
-      <c r="C21" t="s">
-        <v>371</v>
+        <v>346</v>
+      </c>
+      <c r="C21" t="str">
+        <f>_xlfn.CONCAT(Constants!$B$18,"/P002_090_PayCycleAfternoon")</f>
+        <v>PROD/P002_090_PayCycleAfternoon</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="19" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B22" t="s">
-        <v>348</v>
-      </c>
-      <c r="C22" t="s">
-        <v>371</v>
+        <v>347</v>
+      </c>
+      <c r="C22" t="str">
+        <f>_xlfn.CONCAT(Constants!$B$18,"/P002_090_PayCycleAfternoon")</f>
+        <v>PROD/P002_090_PayCycleAfternoon</v>
       </c>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" s="19" t="s">
+      <c r="A23" s="24" t="s">
+        <v>390</v>
+      </c>
+      <c r="B23" t="s">
+        <v>388</v>
+      </c>
+      <c r="C23" t="str">
+        <f>_xlfn.CONCAT(Constants!$B$18,"/P002_090_PayCycleAfternoon")</f>
+        <v>PROD/P002_090_PayCycleAfternoon</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="24" t="s">
+        <v>391</v>
+      </c>
+      <c r="B24" t="s">
+        <v>389</v>
+      </c>
+      <c r="C24" t="str">
+        <f>_xlfn.CONCAT(Constants!$B$18,"/P002_090_PayCycleAfternoon")</f>
+        <v>PROD/P002_090_PayCycleAfternoon</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="19" t="s">
+        <v>354</v>
+      </c>
+      <c r="B25" t="s">
         <v>355</v>
       </c>
-      <c r="B23" t="s">
-        <v>356</v>
-      </c>
-      <c r="C23" t="s">
-        <v>371</v>
+      <c r="C25" t="str">
+        <f>_xlfn.CONCAT(Constants!$B$18,"/P002_090_PayCycleAfternoon")</f>
+        <v>PROD/P002_090_PayCycleAfternoon</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="20"/>
+  <phoneticPr fontId="21"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1D9DC59-3960-42CB-B3EC-EFF452A90D4F}">
-  <dimension ref="A1:Z89"/>
+  <dimension ref="A1:Z91"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -3968,18 +3107,18 @@
     </row>
     <row r="3" spans="1:26">
       <c r="A3" t="s">
+        <v>282</v>
+      </c>
+      <c r="B3" t="s">
         <v>283</v>
-      </c>
-      <c r="B3" t="s">
-        <v>284</v>
       </c>
     </row>
     <row r="4" spans="1:26">
       <c r="A4" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="5" spans="1:26">
@@ -4024,551 +3163,551 @@
     </row>
     <row r="10" spans="1:26">
       <c r="A10" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B10" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="11" spans="1:26">
       <c r="A11" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B11" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="12" spans="1:26">
       <c r="A12" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B12" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="13" spans="1:26">
       <c r="A13" t="s">
+        <v>298</v>
+      </c>
+      <c r="B13" t="s">
         <v>299</v>
-      </c>
-      <c r="B13" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="14" spans="1:26">
       <c r="A14" t="s">
-        <v>311</v>
+        <v>378</v>
       </c>
       <c r="B14" t="s">
-        <v>310</v>
+        <v>379</v>
       </c>
     </row>
     <row r="15" spans="1:26">
       <c r="A15" t="s">
-        <v>104</v>
+        <v>381</v>
       </c>
       <c r="B15" t="s">
-        <v>108</v>
+        <v>380</v>
       </c>
     </row>
     <row r="16" spans="1:26">
       <c r="A16" t="s">
-        <v>105</v>
+        <v>310</v>
       </c>
       <c r="B16" t="s">
-        <v>109</v>
+        <v>309</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="B17" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>303</v>
+        <v>105</v>
       </c>
       <c r="B18" t="s">
-        <v>302</v>
+        <v>109</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B19" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>113</v>
+        <v>302</v>
       </c>
       <c r="B20" t="s">
-        <v>116</v>
+        <v>301</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B21" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>304</v>
+        <v>113</v>
       </c>
       <c r="B22" t="s">
-        <v>305</v>
+        <v>116</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B23" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>119</v>
+        <v>303</v>
       </c>
       <c r="B24" t="s">
-        <v>122</v>
+        <v>304</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="B25" t="s">
-        <v>137</v>
+        <v>121</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>248</v>
+        <v>119</v>
       </c>
       <c r="B26" t="s">
-        <v>250</v>
+        <v>122</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>249</v>
+        <v>131</v>
       </c>
       <c r="B27" t="s">
-        <v>250</v>
+        <v>137</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" t="s">
-        <v>136</v>
+        <v>247</v>
       </c>
       <c r="B28" t="s">
-        <v>135</v>
+        <v>249</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" t="s">
-        <v>294</v>
+        <v>248</v>
       </c>
       <c r="B29" t="s">
-        <v>295</v>
+        <v>249</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" t="s">
-        <v>268</v>
+        <v>136</v>
       </c>
       <c r="B30" t="s">
-        <v>296</v>
+        <v>135</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" t="s">
-        <v>376</v>
+        <v>293</v>
       </c>
       <c r="B31" t="s">
-        <v>380</v>
+        <v>294</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" t="s">
-        <v>377</v>
+        <v>267</v>
       </c>
       <c r="B32" t="s">
-        <v>380</v>
+        <v>295</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
       <c r="B33" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" t="s">
-        <v>132</v>
+        <v>374</v>
       </c>
       <c r="B34" t="s">
-        <v>138</v>
+        <v>377</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" t="s">
-        <v>133</v>
+        <v>375</v>
       </c>
       <c r="B35" t="s">
-        <v>139</v>
+        <v>376</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B36" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="B37" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" t="s">
-        <v>155</v>
+        <v>134</v>
       </c>
       <c r="B38" t="s">
-        <v>153</v>
+        <v>140</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
       <c r="B39" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="B40" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B41" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="B42" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="B43" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44" t="s">
-        <v>291</v>
+        <v>159</v>
       </c>
       <c r="B44" t="s">
-        <v>292</v>
+        <v>158</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B45" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46" t="s">
-        <v>163</v>
+        <v>290</v>
       </c>
       <c r="B46" t="s">
-        <v>165</v>
+        <v>291</v>
       </c>
     </row>
     <row r="47" spans="1:2">
       <c r="A47" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="B47" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="B48" t="s">
-        <v>315</v>
+        <v>165</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49" t="s">
-        <v>353</v>
+        <v>169</v>
       </c>
       <c r="B49" t="s">
-        <v>354</v>
+        <v>168</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50" t="s">
-        <v>252</v>
+        <v>171</v>
       </c>
       <c r="B50" t="s">
-        <v>251</v>
+        <v>314</v>
       </c>
     </row>
     <row r="51" spans="1:2">
       <c r="A51" t="s">
-        <v>143</v>
+        <v>352</v>
       </c>
       <c r="B51" t="s">
-        <v>170</v>
+        <v>353</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52" t="s">
-        <v>144</v>
+        <v>251</v>
       </c>
       <c r="B52" t="s">
-        <v>172</v>
+        <v>250</v>
       </c>
     </row>
     <row r="53" spans="1:2">
       <c r="A53" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B53" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="54" spans="1:2">
       <c r="A54" t="s">
-        <v>174</v>
+        <v>144</v>
       </c>
       <c r="B54" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" t="s">
-        <v>180</v>
+        <v>145</v>
       </c>
       <c r="B55" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="B56" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
     </row>
     <row r="57" spans="1:2">
       <c r="A57" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="B57" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
     </row>
     <row r="58" spans="1:2">
       <c r="A58" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
       <c r="B58" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
     </row>
     <row r="59" spans="1:2">
       <c r="A59" t="s">
-        <v>176</v>
+        <v>184</v>
       </c>
       <c r="B59" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
     </row>
     <row r="60" spans="1:2">
       <c r="A60" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B60" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="61" spans="1:2">
       <c r="A61" t="s">
-        <v>190</v>
+        <v>176</v>
       </c>
       <c r="B61" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="62" spans="1:2">
       <c r="A62" t="s">
-        <v>194</v>
+        <v>177</v>
       </c>
       <c r="B62" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
     </row>
     <row r="63" spans="1:2">
       <c r="A63" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="B63" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
     </row>
     <row r="64" spans="1:2">
       <c r="A64" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="B64" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
     </row>
     <row r="65" spans="1:2">
       <c r="A65" t="s">
-        <v>192</v>
+        <v>197</v>
       </c>
       <c r="B65" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="66" spans="1:2">
       <c r="A66" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="B66" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
     </row>
     <row r="67" spans="1:2">
       <c r="A67" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="B67" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
     </row>
     <row r="68" spans="1:2">
       <c r="A68" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B68" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
     </row>
     <row r="69" spans="1:2">
       <c r="A69" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="B69" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="70" spans="1:2">
       <c r="A70" t="s">
-        <v>285</v>
+        <v>202</v>
       </c>
       <c r="B70" t="s">
-        <v>286</v>
+        <v>204</v>
       </c>
     </row>
     <row r="71" spans="1:2">
       <c r="A71" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="B71" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
     </row>
     <row r="72" spans="1:2">
       <c r="A72" t="s">
-        <v>212</v>
+        <v>284</v>
       </c>
       <c r="B72" t="s">
-        <v>211</v>
+        <v>285</v>
       </c>
     </row>
     <row r="73" spans="1:2">
       <c r="A73" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="B73" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
     </row>
     <row r="74" spans="1:2">
       <c r="A74" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="B74" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
     </row>
     <row r="75" spans="1:2">
       <c r="A75" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="B75" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
     </row>
     <row r="76" spans="1:2">
       <c r="A76" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="B76" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
     </row>
     <row r="77" spans="1:2">
       <c r="A77" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="B77" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="78" spans="1:2">
       <c r="A78" t="s">
-        <v>207</v>
+        <v>221</v>
       </c>
       <c r="B78" t="s">
         <v>220</v>
@@ -4576,90 +3715,106 @@
     </row>
     <row r="79" spans="1:2">
       <c r="A79" t="s">
-        <v>208</v>
+        <v>222</v>
       </c>
       <c r="B79" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
     </row>
     <row r="80" spans="1:2">
       <c r="A80" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B80" t="s">
-        <v>224</v>
+        <v>383</v>
       </c>
     </row>
     <row r="81" spans="1:2">
       <c r="A81" t="s">
-        <v>262</v>
+        <v>208</v>
       </c>
       <c r="B81" t="s">
-        <v>265</v>
+        <v>224</v>
       </c>
     </row>
     <row r="82" spans="1:2">
       <c r="A82" t="s">
-        <v>263</v>
+        <v>209</v>
       </c>
       <c r="B82" t="s">
-        <v>266</v>
+        <v>223</v>
       </c>
     </row>
     <row r="83" spans="1:2">
       <c r="A83" t="s">
+        <v>261</v>
+      </c>
+      <c r="B83" t="s">
         <v>264</v>
-      </c>
-      <c r="B83" t="s">
-        <v>267</v>
       </c>
     </row>
     <row r="84" spans="1:2">
       <c r="A84" t="s">
-        <v>357</v>
+        <v>262</v>
       </c>
       <c r="B84" t="s">
-        <v>358</v>
+        <v>265</v>
       </c>
     </row>
     <row r="85" spans="1:2">
       <c r="A85" t="s">
-        <v>363</v>
+        <v>263</v>
       </c>
       <c r="B85" t="s">
-        <v>364</v>
+        <v>266</v>
       </c>
     </row>
     <row r="86" spans="1:2">
       <c r="A86" t="s">
-        <v>365</v>
+        <v>356</v>
       </c>
       <c r="B86" t="s">
-        <v>366</v>
+        <v>357</v>
       </c>
     </row>
     <row r="87" spans="1:2">
       <c r="A87" t="s">
-        <v>367</v>
+        <v>362</v>
       </c>
       <c r="B87" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
     </row>
     <row r="88" spans="1:2">
       <c r="A88" t="s">
-        <v>359</v>
+        <v>364</v>
       </c>
       <c r="B88" t="s">
-        <v>361</v>
+        <v>365</v>
       </c>
     </row>
     <row r="89" spans="1:2">
       <c r="A89" t="s">
+        <v>366</v>
+      </c>
+      <c r="B89" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2">
+      <c r="A90" t="s">
+        <v>358</v>
+      </c>
+      <c r="B90" t="s">
         <v>360</v>
       </c>
-      <c r="B89" t="s">
-        <v>362</v>
+    </row>
+    <row r="91" spans="1:2">
+      <c r="A91" t="s">
+        <v>359</v>
+      </c>
+      <c r="B91" t="s">
+        <v>361</v>
       </c>
     </row>
   </sheetData>

</xml_diff>